<commit_message>
[VM:Susmitha.palacherla@6/23/2014 9:02:34 AM] Updated per SCR 12897 to modigy and add DIM_Source values.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13617
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="DIM_Source" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="176">
   <si>
     <t>SourceID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Quality Call Listening</t>
   </si>
   <si>
-    <t>CMS Customer Call Listening</t>
-  </si>
-  <si>
     <t>Leadership Listening</t>
   </si>
   <si>
@@ -544,6 +541,12 @@
   </si>
   <si>
     <t>Verint Monitoring</t>
+  </si>
+  <si>
+    <t>CMS Reported Item</t>
+  </si>
+  <si>
+    <t>Internal CCO Reporting</t>
   </si>
 </sst>
 </file>
@@ -882,9 +885,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -989,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +1016,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1049,7 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,7 +1060,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,7 +1093,7 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1104,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,194 +1115,216 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>216</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>217</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>22</v>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>218</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1319,10 +1346,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1338,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1381,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1370,7 +1397,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,7 +1405,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1402,16 +1429,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1433,13 +1460,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,13 +1474,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1461,13 +1488,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1475,13 +1502,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,13 +1516,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1503,13 +1530,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1517,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,13 +1572,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
         <v>58</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,13 +1586,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,13 +1600,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,13 +1614,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
         <v>66</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,13 +1628,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
         <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,13 +1642,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,13 +1656,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
         <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,13 +1670,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
         <v>76</v>
-      </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,13 +1684,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
         <v>78</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,13 +1698,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,13 +1712,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1713,10 +1740,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
         <v>84</v>
-      </c>
-      <c r="B1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1732,7 +1759,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +1767,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1748,7 +1775,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1756,7 +1783,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1764,7 +1791,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1772,7 +1799,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1780,7 +1807,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1788,7 +1815,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1796,7 +1823,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1804,7 +1831,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1812,7 +1839,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1820,7 +1847,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1828,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1836,7 +1863,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1858,10 +1885,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
         <v>99</v>
-      </c>
-      <c r="B1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1877,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1885,7 +1912,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1893,7 +1920,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1901,7 +1928,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1917,7 +1944,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1925,7 +1952,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1933,7 +1960,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1941,7 +1968,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1949,7 +1976,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1957,7 +1984,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1965,7 +1992,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1973,7 +2000,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +2008,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1989,7 +2016,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1997,7 +2024,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2005,7 +2032,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2013,7 +2040,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2021,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2029,7 +2056,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,7 +2064,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2045,7 +2072,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2053,7 +2080,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2061,7 +2088,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2069,7 +2096,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2077,7 +2104,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2085,7 +2112,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2093,7 +2120,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2101,7 +2128,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2109,7 +2136,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2117,7 +2144,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2125,7 +2152,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2133,7 +2160,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2141,7 +2168,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2149,7 +2176,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2157,7 +2184,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2165,7 +2192,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2173,7 +2200,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2181,7 +2208,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2189,7 +2216,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2224,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2205,7 +2232,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2213,7 +2240,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2221,7 +2248,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2229,7 +2256,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,7 +2264,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2245,7 +2272,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2257,7 +2284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -2270,10 +2297,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
         <v>147</v>
-      </c>
-      <c r="B1" t="s">
-        <v>148</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2317,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5">
         <v>104</v>
@@ -2328,7 +2355,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6">
         <v>104</v>
@@ -2339,7 +2366,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7">
         <v>104</v>
@@ -2350,7 +2377,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8">
         <v>214</v>
@@ -2361,7 +2388,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9">
         <v>214</v>
@@ -2372,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10">
         <v>214</v>
@@ -2383,7 +2410,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11">
         <v>214</v>
@@ -2394,7 +2421,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12">
         <v>214</v>
@@ -2405,7 +2432,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13">
         <v>214</v>
@@ -2416,7 +2443,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14">
         <v>214</v>
@@ -2427,7 +2454,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>217</v>
@@ -2438,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16">
         <v>205</v>
@@ -2449,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>215</v>
@@ -2460,7 +2487,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18">
         <v>209</v>
@@ -2471,7 +2498,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19">
         <v>216</v>
@@ -2482,7 +2509,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C20">
         <v>212</v>
@@ -2493,7 +2520,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21">
         <v>212</v>
@@ -2504,7 +2531,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C22">
         <v>212</v>
@@ -2515,7 +2542,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C23">
         <v>212</v>
@@ -2526,7 +2553,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24">
         <v>212</v>
@@ -2537,7 +2564,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C25">
         <v>212</v>
@@ -2548,7 +2575,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26">
         <v>212</v>
@@ -2559,7 +2586,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C27">
         <v>212</v>
@@ -2570,7 +2597,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C28">
         <v>212</v>
@@ -2581,7 +2608,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29">
         <v>212</v>
@@ -2592,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30">
         <v>212</v>
@@ -2603,7 +2630,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C31">
         <v>212</v>
@@ -2614,7 +2641,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32">
         <v>212</v>
@@ -2625,7 +2652,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33">
         <v>211</v>
@@ -2636,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C34">
         <v>207</v>
@@ -2647,7 +2674,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C35">
         <v>213</v>
@@ -2658,7 +2685,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C36">
         <v>212</v>
@@ -2669,7 +2696,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C37">
         <v>212</v>
@@ -2680,7 +2707,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38">
         <v>212</v>
@@ -2691,7 +2718,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C39">
         <v>212</v>
@@ -2702,7 +2729,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40">
         <v>212</v>
@@ -2713,7 +2740,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41">
         <v>212</v>
@@ -2724,7 +2751,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C42">
         <v>213</v>
@@ -2746,7 +2773,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44">
         <v>204</v>
@@ -2757,7 +2784,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45">
         <v>204</v>
@@ -2768,7 +2795,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C46">
         <v>204</v>
@@ -2779,7 +2806,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C47">
         <v>204</v>
@@ -2790,7 +2817,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48">
         <v>208</v>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@7/11/2014 9:55:26 AM] Updated per scr 13129 to add new SubCoachingReason value.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13639
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DIM_Source" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="177">
   <si>
     <t>SourceID</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>Internal CCO Reporting</t>
+  </si>
+  <si>
+    <t>ETS</t>
   </si>
 </sst>
 </file>
@@ -887,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -1873,9 +1876,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2275,6 +2280,14 @@
         <v>145</v>
       </c>
     </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2284,7 +2297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@10/24/2014 10:52:50 AM] Additional updates for SCR 13479. Internal version 7.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13759
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="452">
   <si>
     <t>SourceID</t>
   </si>
@@ -1382,6 +1382,9 @@
   </si>
   <si>
     <t>splReasonPrty</t>
+  </si>
+  <si>
+    <t>Additional update for warning. Added ETS as Sub Coaching Reason.</t>
   </si>
 </sst>
 </file>
@@ -1739,14 +1742,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.5703125" customWidth="1"/>
@@ -1866,6 +1871,23 @@
       </c>
       <c r="E7" t="s">
         <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41934</v>
+      </c>
+      <c r="C8" t="s">
+        <v>434</v>
+      </c>
+      <c r="D8">
+        <v>13479</v>
+      </c>
+      <c r="E8" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -2705,9 +2727,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N150"/>
+  <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A113" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2757,22 +2779,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="s">
-        <v>444</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>96</v>
+        <v>-1</v>
       </c>
       <c r="D2" t="s">
-        <v>448</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2781,10 +2803,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2793,24 +2815,24 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>444</v>
+        <v>84</v>
       </c>
       <c r="C3">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2819,13 +2841,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -2834,27 +2856,27 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>442</v>
+        <v>85</v>
       </c>
       <c r="C4">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>449</v>
+        <v>107</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2863,13 +2885,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>1</v>
@@ -2881,24 +2903,24 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>443</v>
+        <v>85</v>
       </c>
       <c r="C5">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>449</v>
+        <v>108</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2907,13 +2929,13 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -2925,24 +2947,24 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>444</v>
+        <v>85</v>
       </c>
       <c r="C6">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>449</v>
+        <v>109</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2951,13 +2973,13 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -2969,33 +2991,33 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -3004,7 +3026,7 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3021,16 +3043,16 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3054,7 +3076,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -3071,10 +3093,10 @@
         <v>85</v>
       </c>
       <c r="C9">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3115,10 +3137,10 @@
         <v>85</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3159,10 +3181,10 @@
         <v>85</v>
       </c>
       <c r="C11">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>206</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3197,16 +3219,16 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C12">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>172</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3215,7 +3237,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -3241,16 +3263,16 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>206</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -3271,10 +3293,10 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3285,16 +3307,16 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="C14">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -3318,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3329,16 +3351,16 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="C15">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3362,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3373,16 +3395,16 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="C16">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3400,13 +3422,13 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3417,16 +3439,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="C17">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>234</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3435,7 +3457,7 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -3444,13 +3466,13 @@
         <v>1</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -3461,16 +3483,16 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>181</v>
       </c>
       <c r="C18">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="D18" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3488,10 +3510,10 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -3505,16 +3527,16 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>181</v>
+        <v>87</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3538,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -3549,16 +3571,16 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="C20">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>206</v>
+        <v>100</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -3573,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -3585,24 +3607,24 @@
         <v>1</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C21">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>344</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -3617,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -3626,13 +3648,13 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3643,10 +3665,10 @@
         <v>88</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>345</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -3670,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -3687,10 +3709,10 @@
         <v>88</v>
       </c>
       <c r="C23">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -3731,10 +3753,10 @@
         <v>88</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>345</v>
+        <v>103</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -3758,7 +3780,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -3775,10 +3797,10 @@
         <v>88</v>
       </c>
       <c r="C25">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -3819,10 +3841,10 @@
         <v>88</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -3863,10 +3885,10 @@
         <v>88</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>347</v>
+        <v>236</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -3907,10 +3929,10 @@
         <v>88</v>
       </c>
       <c r="C28">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>105</v>
+        <v>237</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -3951,10 +3973,10 @@
         <v>88</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>236</v>
+        <v>101</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -3995,10 +4017,10 @@
         <v>88</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -4033,16 +4055,16 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -4057,7 +4079,7 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -4066,21 +4088,21 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C32">
         <v>42</v>
@@ -4101,7 +4123,7 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32">
         <v>1</v>
@@ -4110,27 +4132,27 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -4165,16 +4187,16 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C34">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>134</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -4209,16 +4231,16 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C35">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -4259,10 +4281,10 @@
         <v>91</v>
       </c>
       <c r="C36">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -4303,10 +4325,10 @@
         <v>91</v>
       </c>
       <c r="C37">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -4347,10 +4369,10 @@
         <v>91</v>
       </c>
       <c r="C38">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>119</v>
+        <v>348</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -4391,10 +4413,10 @@
         <v>91</v>
       </c>
       <c r="C39">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>349</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -4435,10 +4457,10 @@
         <v>91</v>
       </c>
       <c r="C40">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>348</v>
+        <v>115</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -4479,10 +4501,10 @@
         <v>91</v>
       </c>
       <c r="C41">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>349</v>
+        <v>122</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -4523,10 +4545,10 @@
         <v>91</v>
       </c>
       <c r="C42">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -4567,10 +4589,10 @@
         <v>91</v>
       </c>
       <c r="C43">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -4611,10 +4633,10 @@
         <v>91</v>
       </c>
       <c r="C44">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>123</v>
+        <v>350</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -4655,10 +4677,10 @@
         <v>91</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>351</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -4699,10 +4721,10 @@
         <v>91</v>
       </c>
       <c r="C46">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>350</v>
+        <v>206</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -4737,16 +4759,16 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C47">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>351</v>
+        <v>140</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -4781,16 +4803,16 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C48">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>206</v>
+        <v>352</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -4831,10 +4853,10 @@
         <v>92</v>
       </c>
       <c r="C49">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -4875,10 +4897,10 @@
         <v>92</v>
       </c>
       <c r="C50">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D50" t="s">
-        <v>352</v>
+        <v>139</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -4919,10 +4941,10 @@
         <v>92</v>
       </c>
       <c r="C51">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="D51" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -4963,10 +4985,10 @@
         <v>92</v>
       </c>
       <c r="C52">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D52" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -5001,16 +5023,16 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C53">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D53" t="s">
-        <v>138</v>
+        <v>206</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -5022,7 +5044,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -5031,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53">
         <v>0</v>
@@ -5045,16 +5067,16 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C54">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -5066,16 +5088,16 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54">
         <v>1</v>
       </c>
       <c r="J54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54">
         <v>0</v>
@@ -5095,10 +5117,10 @@
         <v>93</v>
       </c>
       <c r="C55">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -5116,7 +5138,7 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -5133,16 +5155,16 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C56">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D56" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -5154,19 +5176,19 @@
         <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>1</v>
       </c>
       <c r="J56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56">
         <v>0</v>
@@ -5177,16 +5199,16 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C57">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D57" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -5198,13 +5220,13 @@
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>1</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -5221,16 +5243,16 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C58">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D58" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -5248,13 +5270,13 @@
         <v>1</v>
       </c>
       <c r="J58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M58">
         <v>0</v>
@@ -5265,16 +5287,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="C59">
         <v>42</v>
       </c>
       <c r="D59" t="s">
-        <v>206</v>
+        <v>17</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -5292,10 +5314,10 @@
         <v>1</v>
       </c>
       <c r="J59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -5309,16 +5331,16 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="C60">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>195</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -5339,7 +5361,7 @@
         <v>0</v>
       </c>
       <c r="K60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60">
         <v>0</v>
@@ -5359,10 +5381,10 @@
         <v>182</v>
       </c>
       <c r="C61">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D61" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5403,10 +5425,10 @@
         <v>182</v>
       </c>
       <c r="C62">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D62" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -5447,10 +5469,10 @@
         <v>182</v>
       </c>
       <c r="C63">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -5491,10 +5513,10 @@
         <v>182</v>
       </c>
       <c r="C64">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D64" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -5535,10 +5557,10 @@
         <v>182</v>
       </c>
       <c r="C65">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -5579,10 +5601,10 @@
         <v>182</v>
       </c>
       <c r="C66">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D66" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -5623,10 +5645,10 @@
         <v>182</v>
       </c>
       <c r="C67">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -5667,10 +5689,10 @@
         <v>182</v>
       </c>
       <c r="C68">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D68" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -5711,10 +5733,10 @@
         <v>182</v>
       </c>
       <c r="C69">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D69" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -5749,16 +5771,16 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C70">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D70" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -5799,10 +5821,10 @@
         <v>183</v>
       </c>
       <c r="C71">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D71" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -5843,10 +5865,10 @@
         <v>183</v>
       </c>
       <c r="C72">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -5881,16 +5903,16 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C73">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D73" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -5931,10 +5953,10 @@
         <v>184</v>
       </c>
       <c r="C74">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D74" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -5975,10 +5997,10 @@
         <v>184</v>
       </c>
       <c r="C75">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D75" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -5999,7 +6021,7 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -6019,10 +6041,10 @@
         <v>184</v>
       </c>
       <c r="C76">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D76" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -6043,7 +6065,7 @@
         <v>0</v>
       </c>
       <c r="K76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76">
         <v>0</v>
@@ -6063,10 +6085,10 @@
         <v>184</v>
       </c>
       <c r="C77">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -6101,10 +6123,10 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C78">
         <v>42</v>
@@ -6125,7 +6147,7 @@
         <v>1</v>
       </c>
       <c r="I78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -6145,16 +6167,16 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C79">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D79" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -6169,7 +6191,7 @@
         <v>1</v>
       </c>
       <c r="I79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -6195,10 +6217,10 @@
         <v>186</v>
       </c>
       <c r="C80">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D80" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -6233,16 +6255,16 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B81" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C81">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D81" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -6283,10 +6305,10 @@
         <v>187</v>
       </c>
       <c r="C82">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D82" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -6327,10 +6349,10 @@
         <v>187</v>
       </c>
       <c r="C83">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D83" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -6371,10 +6393,10 @@
         <v>187</v>
       </c>
       <c r="C84">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D84" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -6415,10 +6437,10 @@
         <v>187</v>
       </c>
       <c r="C85">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D85" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -6459,10 +6481,10 @@
         <v>187</v>
       </c>
       <c r="C86">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D86" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -6497,16 +6519,16 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C87">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="D87" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -6527,10 +6549,10 @@
         <v>0</v>
       </c>
       <c r="K87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M87">
         <v>0</v>
@@ -6547,10 +6569,10 @@
         <v>188</v>
       </c>
       <c r="C88">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D88" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -6591,10 +6613,10 @@
         <v>188</v>
       </c>
       <c r="C89">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="D89" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -6629,10 +6651,10 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C90">
         <v>42</v>
@@ -6673,16 +6695,16 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B91" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="C91">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D91" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -6723,10 +6745,10 @@
         <v>189</v>
       </c>
       <c r="C92">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D92" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -6767,10 +6789,10 @@
         <v>189</v>
       </c>
       <c r="C93">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D93" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -6811,10 +6833,10 @@
         <v>189</v>
       </c>
       <c r="C94">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D94" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -6855,10 +6877,10 @@
         <v>189</v>
       </c>
       <c r="C95">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D95" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -6899,10 +6921,10 @@
         <v>189</v>
       </c>
       <c r="C96">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D96" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -6943,10 +6965,10 @@
         <v>189</v>
       </c>
       <c r="C97">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D97" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -6987,10 +7009,10 @@
         <v>189</v>
       </c>
       <c r="C98">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="D98" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -7025,10 +7047,10 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C99">
         <v>42</v>
@@ -7046,7 +7068,7 @@
         <v>1</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99">
         <v>1</v>
@@ -7069,16 +7091,16 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B100" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C100">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="D100" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -7090,7 +7112,7 @@
         <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100">
         <v>1</v>
@@ -7119,10 +7141,10 @@
         <v>191</v>
       </c>
       <c r="C101">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D101" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -7163,10 +7185,10 @@
         <v>191</v>
       </c>
       <c r="C102">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D102" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -7207,10 +7229,10 @@
         <v>191</v>
       </c>
       <c r="C103">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D103" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -7251,10 +7273,10 @@
         <v>191</v>
       </c>
       <c r="C104">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="D104" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -7289,16 +7311,16 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C105">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="D105" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -7339,10 +7361,10 @@
         <v>192</v>
       </c>
       <c r="C106">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D106" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -7383,10 +7405,10 @@
         <v>192</v>
       </c>
       <c r="C107">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D107" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -7427,10 +7449,10 @@
         <v>192</v>
       </c>
       <c r="C108">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="D108" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -7465,16 +7487,16 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B109" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C109">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D109" t="s">
-        <v>206</v>
+        <v>353</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -7515,10 +7537,10 @@
         <v>193</v>
       </c>
       <c r="C110">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D110" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -7559,10 +7581,10 @@
         <v>193</v>
       </c>
       <c r="C111">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D111" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -7603,10 +7625,10 @@
         <v>193</v>
       </c>
       <c r="C112">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D112" t="s">
-        <v>355</v>
+        <v>114</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -7647,10 +7669,10 @@
         <v>193</v>
       </c>
       <c r="C113">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D113" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -7691,10 +7713,10 @@
         <v>193</v>
       </c>
       <c r="C114">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D114" t="s">
-        <v>116</v>
+        <v>356</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -7735,10 +7757,10 @@
         <v>193</v>
       </c>
       <c r="C115">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D115" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -7779,10 +7801,10 @@
         <v>193</v>
       </c>
       <c r="C116">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D116" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -7823,10 +7845,10 @@
         <v>193</v>
       </c>
       <c r="C117">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D117" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -7867,10 +7889,10 @@
         <v>193</v>
       </c>
       <c r="C118">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D118" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -7911,10 +7933,10 @@
         <v>193</v>
       </c>
       <c r="C119">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D119" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -7955,10 +7977,10 @@
         <v>193</v>
       </c>
       <c r="C120">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D120" t="s">
-        <v>361</v>
+        <v>206</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -7993,16 +8015,16 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>193</v>
+        <v>442</v>
       </c>
       <c r="C121">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="D121" t="s">
-        <v>206</v>
+        <v>449</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -8011,42 +8033,42 @@
         <v>1</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121">
         <v>1</v>
       </c>
       <c r="I121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K121">
         <v>0</v>
       </c>
       <c r="L121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>181</v>
+        <v>442</v>
       </c>
       <c r="C122">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="D122" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -8055,42 +8077,42 @@
         <v>1</v>
       </c>
       <c r="G122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H122">
         <v>1</v>
       </c>
       <c r="I122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K122">
         <v>0</v>
       </c>
       <c r="L122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>181</v>
+        <v>442</v>
       </c>
       <c r="C123">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>234</v>
+        <v>98</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -8099,42 +8121,42 @@
         <v>1</v>
       </c>
       <c r="G123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H123">
         <v>1</v>
       </c>
       <c r="I123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K123">
         <v>0</v>
       </c>
       <c r="L123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>181</v>
+        <v>442</v>
       </c>
       <c r="C124">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="D124" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -8143,42 +8165,42 @@
         <v>1</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
         <v>1</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K124">
         <v>0</v>
       </c>
       <c r="L124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>95</v>
+        <v>442</v>
       </c>
       <c r="C125">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D125" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -8187,28 +8209,28 @@
         <v>1</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
         <v>1</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L125">
         <v>0</v>
       </c>
       <c r="M125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -8219,10 +8241,10 @@
         <v>442</v>
       </c>
       <c r="C126">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D126" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -8263,10 +8285,10 @@
         <v>442</v>
       </c>
       <c r="C127">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D127" t="s">
-        <v>206</v>
+        <v>445</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -8307,10 +8329,10 @@
         <v>442</v>
       </c>
       <c r="C128">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D128" t="s">
-        <v>221</v>
+        <v>446</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -8351,10 +8373,10 @@
         <v>442</v>
       </c>
       <c r="C129">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D129" t="s">
-        <v>86</v>
+        <v>447</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -8395,10 +8417,10 @@
         <v>442</v>
       </c>
       <c r="C130">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D130" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -8439,10 +8461,10 @@
         <v>442</v>
       </c>
       <c r="C131">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D131" t="s">
-        <v>446</v>
+        <v>92</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -8477,16 +8499,16 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B132" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C132">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>447</v>
+        <v>98</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -8521,16 +8543,16 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B133" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C133">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D133" t="s">
-        <v>448</v>
+        <v>206</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -8565,16 +8587,16 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B134" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C134">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D134" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -8615,10 +8637,10 @@
         <v>443</v>
       </c>
       <c r="C135">
-        <v>1</v>
+        <v>92</v>
       </c>
       <c r="D135" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -8659,10 +8681,10 @@
         <v>443</v>
       </c>
       <c r="C136">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D136" t="s">
-        <v>206</v>
+        <v>445</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -8703,10 +8725,10 @@
         <v>443</v>
       </c>
       <c r="C137">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="D137" t="s">
-        <v>221</v>
+        <v>446</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -8747,10 +8769,10 @@
         <v>443</v>
       </c>
       <c r="C138">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D138" t="s">
-        <v>86</v>
+        <v>447</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -8791,10 +8813,10 @@
         <v>443</v>
       </c>
       <c r="C139">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D139" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -8835,10 +8857,10 @@
         <v>443</v>
       </c>
       <c r="C140">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D140" t="s">
-        <v>446</v>
+        <v>92</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -8879,10 +8901,10 @@
         <v>443</v>
       </c>
       <c r="C141">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="D141" t="s">
-        <v>447</v>
+        <v>172</v>
       </c>
       <c r="E141">
         <v>1</v>
@@ -8923,10 +8945,10 @@
         <v>443</v>
       </c>
       <c r="C142">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D142" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E142">
         <v>1</v>
@@ -8961,16 +8983,16 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B143" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C143">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D143" t="s">
-        <v>92</v>
+        <v>449</v>
       </c>
       <c r="E143">
         <v>1</v>
@@ -9011,10 +9033,10 @@
         <v>444</v>
       </c>
       <c r="C144">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D144" t="s">
-        <v>98</v>
+        <v>172</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -9055,10 +9077,10 @@
         <v>444</v>
       </c>
       <c r="C145">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -9099,10 +9121,10 @@
         <v>444</v>
       </c>
       <c r="C146">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D146" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -9143,10 +9165,10 @@
         <v>444</v>
       </c>
       <c r="C147">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D147" t="s">
-        <v>86</v>
+        <v>221</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -9187,10 +9209,10 @@
         <v>444</v>
       </c>
       <c r="C148">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D148" t="s">
-        <v>445</v>
+        <v>86</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -9231,10 +9253,10 @@
         <v>444</v>
       </c>
       <c r="C149">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D149" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -9275,39 +9297,171 @@
         <v>444</v>
       </c>
       <c r="C150">
+        <v>94</v>
+      </c>
+      <c r="D150" t="s">
+        <v>446</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>1</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="I150">
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>1</v>
+      </c>
+      <c r="K150">
+        <v>0</v>
+      </c>
+      <c r="L150">
+        <v>0</v>
+      </c>
+      <c r="M150">
+        <v>1</v>
+      </c>
+      <c r="N150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>30</v>
+      </c>
+      <c r="B151" t="s">
+        <v>444</v>
+      </c>
+      <c r="C151">
         <v>95</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D151" t="s">
         <v>447</v>
       </c>
-      <c r="E150">
-        <v>1</v>
-      </c>
-      <c r="F150">
-        <v>1</v>
-      </c>
-      <c r="G150">
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <v>1</v>
-      </c>
-      <c r="I150">
-        <v>0</v>
-      </c>
-      <c r="J150">
-        <v>1</v>
-      </c>
-      <c r="K150">
-        <v>0</v>
-      </c>
-      <c r="L150">
-        <v>0</v>
-      </c>
-      <c r="M150">
-        <v>1</v>
-      </c>
-      <c r="N150">
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>1</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>1</v>
+      </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
+      <c r="L151">
+        <v>0</v>
+      </c>
+      <c r="M151">
+        <v>1</v>
+      </c>
+      <c r="N151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>30</v>
+      </c>
+      <c r="B152" t="s">
+        <v>444</v>
+      </c>
+      <c r="C152">
+        <v>96</v>
+      </c>
+      <c r="D152" t="s">
+        <v>448</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152">
+        <v>1</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+      <c r="K152">
+        <v>0</v>
+      </c>
+      <c r="L152">
+        <v>0</v>
+      </c>
+      <c r="M152">
+        <v>1</v>
+      </c>
+      <c r="N152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>30</v>
+      </c>
+      <c r="B153" t="s">
+        <v>444</v>
+      </c>
+      <c r="C153">
+        <v>97</v>
+      </c>
+      <c r="D153" t="s">
+        <v>92</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>1</v>
+      </c>
+      <c r="K153">
+        <v>0</v>
+      </c>
+      <c r="L153">
+        <v>0</v>
+      </c>
+      <c r="M153">
+        <v>1</v>
+      </c>
+      <c r="N153">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@10/27/2014 9:27:04 AM] Update for SCR 13609. Internal version 8.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13767
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="453">
   <si>
     <t>SourceID</t>
   </si>
@@ -1385,6 +1385,9 @@
   </si>
   <si>
     <t>Additional update for warning. Added ETS as Sub Coaching Reason.</t>
+  </si>
+  <si>
+    <t>Added job_code WACQ03 with isQuality = 1 in Employee_Selection table</t>
   </si>
 </sst>
 </file>
@@ -1742,11 +1745,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1888,6 +1889,23 @@
       </c>
       <c r="E8" t="s">
         <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41936</v>
+      </c>
+      <c r="C9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D9">
+        <v>13609</v>
+      </c>
+      <c r="E9" t="s">
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -16024,10 +16042,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16168,6 +16186,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@11/7/2014 10:32:12 AM] Updates for SCR 13573. Internal version 9.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13793
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="456">
   <si>
     <t>SourceID</t>
   </si>
@@ -1366,21 +1366,6 @@
     <t>Final Written Warning</t>
   </si>
   <si>
-    <t>Call Avoidance</t>
-  </si>
-  <si>
-    <t>Conduct</t>
-  </si>
-  <si>
-    <t>Dress Code</t>
-  </si>
-  <si>
-    <t>GDIT Policy</t>
-  </si>
-  <si>
-    <t>Performance</t>
-  </si>
-  <si>
     <t>splReasonPrty</t>
   </si>
   <si>
@@ -1388,6 +1373,30 @@
   </si>
   <si>
     <t>Added job_code WACQ03 with isQuality = 1 in Employee_Selection table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements changes to Sub Coaching Reasons list for CSR warnings </t>
+  </si>
+  <si>
+    <t>Conduct (including Call Avoidance)</t>
+  </si>
+  <si>
+    <t>Quality/Performance</t>
+  </si>
+  <si>
+    <t>Security or Privacy Issue</t>
+  </si>
+  <si>
+    <t>Other Policy (non-Security/Privacy)</t>
+  </si>
+  <si>
+    <t>WPWL51</t>
+  </si>
+  <si>
+    <t>Manager, Regional</t>
+  </si>
+  <si>
+    <t>Added job_code WPWL51 (Manager, Regional)to Module_Submission table for submitting Supervisor ecls.</t>
   </si>
 </sst>
 </file>
@@ -1745,9 +1754,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1755,7 +1766,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.5703125" customWidth="1"/>
+    <col min="5" max="5" width="96.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,7 +1899,7 @@
         <v>13479</v>
       </c>
       <c r="E8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1905,7 +1916,41 @@
         <v>13609</v>
       </c>
       <c r="E9" t="s">
-        <v>452</v>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41946</v>
+      </c>
+      <c r="C10" t="s">
+        <v>434</v>
+      </c>
+      <c r="D10">
+        <v>13479</v>
+      </c>
+      <c r="E10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41948</v>
+      </c>
+      <c r="C11" t="s">
+        <v>434</v>
+      </c>
+      <c r="D11">
+        <v>13753</v>
+      </c>
+      <c r="E11" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +1961,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2667,6 +2712,23 @@
         <v>1</v>
       </c>
       <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>453</v>
+      </c>
+      <c r="B45" t="s">
+        <v>454</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
         <v>0</v>
       </c>
     </row>
@@ -2745,9 +2807,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N153"/>
+  <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2792,7 +2854,7 @@
         <v>343</v>
       </c>
       <c r="N1" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3413,16 +3475,16 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>87</v>
       </c>
       <c r="C16">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3440,13 +3502,13 @@
         <v>1</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3457,16 +3519,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="C17">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>100</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3481,10 +3543,10 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3493,24 +3555,24 @@
         <v>1</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>181</v>
+        <v>88</v>
       </c>
       <c r="C18">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>235</v>
+        <v>344</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3525,10 +3587,10 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3537,24 +3599,24 @@
         <v>1</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C19">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>345</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3569,7 +3631,7 @@
         <v>1</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -3581,10 +3643,10 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -3595,10 +3657,10 @@
         <v>88</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>346</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -3639,10 +3701,10 @@
         <v>88</v>
       </c>
       <c r="C21">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>344</v>
+        <v>103</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -3683,10 +3745,10 @@
         <v>88</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -3710,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -3727,10 +3789,10 @@
         <v>88</v>
       </c>
       <c r="C23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>346</v>
+        <v>105</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -3771,10 +3833,10 @@
         <v>88</v>
       </c>
       <c r="C24">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -3815,10 +3877,10 @@
         <v>88</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>347</v>
+        <v>237</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -3859,10 +3921,10 @@
         <v>88</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -3903,10 +3965,10 @@
         <v>88</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -3941,16 +4003,16 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>237</v>
+        <v>106</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -3965,7 +4027,7 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -3974,27 +4036,27 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>206</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -4009,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -4018,21 +4080,21 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C30">
         <v>42</v>
@@ -4053,7 +4115,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
         <v>1</v>
@@ -4062,27 +4124,27 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -4117,16 +4179,16 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C32">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -4161,16 +4223,16 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>206</v>
+        <v>119</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -4211,10 +4273,10 @@
         <v>91</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -4255,10 +4317,10 @@
         <v>91</v>
       </c>
       <c r="C35">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>348</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -4299,10 +4361,10 @@
         <v>91</v>
       </c>
       <c r="C36">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>349</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -4343,10 +4405,10 @@
         <v>91</v>
       </c>
       <c r="C37">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -4387,10 +4449,10 @@
         <v>91</v>
       </c>
       <c r="C38">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>348</v>
+        <v>122</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -4431,10 +4493,10 @@
         <v>91</v>
       </c>
       <c r="C39">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D39" t="s">
-        <v>349</v>
+        <v>123</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -4475,10 +4537,10 @@
         <v>91</v>
       </c>
       <c r="C40">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -4519,10 +4581,10 @@
         <v>91</v>
       </c>
       <c r="C41">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>122</v>
+        <v>350</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -4563,10 +4625,10 @@
         <v>91</v>
       </c>
       <c r="C42">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>351</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -4607,10 +4669,10 @@
         <v>91</v>
       </c>
       <c r="C43">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>206</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -4645,16 +4707,16 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C44">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>140</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -4689,16 +4751,16 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C45">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -4733,16 +4795,16 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -4783,10 +4845,10 @@
         <v>92</v>
       </c>
       <c r="C47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -4827,10 +4889,10 @@
         <v>92</v>
       </c>
       <c r="C48">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>352</v>
+        <v>138</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -4871,10 +4933,10 @@
         <v>92</v>
       </c>
       <c r="C49">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>19</v>
+        <v>206</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -4909,16 +4971,16 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C50">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -4930,7 +4992,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -4939,7 +5001,7 @@
         <v>1</v>
       </c>
       <c r="K50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -4953,16 +5015,16 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -4974,16 +5036,16 @@
         <v>1</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51">
         <v>1</v>
       </c>
       <c r="J51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -4997,16 +5059,16 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C52">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -5018,16 +5080,16 @@
         <v>1</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52">
         <v>1</v>
       </c>
       <c r="J52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52">
         <v>0</v>
@@ -5041,10 +5103,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C53">
         <v>42</v>
@@ -5062,7 +5124,7 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53">
         <v>1</v>
@@ -5071,10 +5133,10 @@
         <v>1</v>
       </c>
       <c r="K53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -5085,16 +5147,16 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C54">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -5106,13 +5168,13 @@
         <v>1</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54">
         <v>1</v>
       </c>
       <c r="J54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -5129,16 +5191,16 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D55" t="s">
-        <v>194</v>
+        <v>17</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -5150,7 +5212,7 @@
         <v>1</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55">
         <v>1</v>
@@ -5159,7 +5221,7 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -5173,16 +5235,16 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>182</v>
       </c>
       <c r="C56">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D56" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -5200,13 +5262,13 @@
         <v>1</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56">
         <v>0</v>
@@ -5217,16 +5279,16 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>182</v>
       </c>
       <c r="C57">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D57" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -5244,7 +5306,7 @@
         <v>1</v>
       </c>
       <c r="J57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -5261,16 +5323,16 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>182</v>
       </c>
       <c r="C58">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -5305,16 +5367,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="C59">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -5335,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="K59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L59">
         <v>0</v>
@@ -5355,10 +5417,10 @@
         <v>182</v>
       </c>
       <c r="C60">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -5399,10 +5461,10 @@
         <v>182</v>
       </c>
       <c r="C61">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5443,10 +5505,10 @@
         <v>182</v>
       </c>
       <c r="C62">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D62" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -5487,10 +5549,10 @@
         <v>182</v>
       </c>
       <c r="C63">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D63" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -5531,10 +5593,10 @@
         <v>182</v>
       </c>
       <c r="C64">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -5575,10 +5637,10 @@
         <v>182</v>
       </c>
       <c r="C65">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D65" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -5613,16 +5675,16 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C66">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -5657,16 +5719,16 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C67">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -5701,16 +5763,16 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C68">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -5745,16 +5807,16 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C69">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -5789,16 +5851,16 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C70">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -5833,16 +5895,16 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C71">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D71" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -5863,7 +5925,7 @@
         <v>0</v>
       </c>
       <c r="K71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L71">
         <v>0</v>
@@ -5877,16 +5939,16 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C72">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D72" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -5927,10 +5989,10 @@
         <v>184</v>
       </c>
       <c r="C73">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -5965,16 +6027,16 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C74">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D74" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -5989,7 +6051,7 @@
         <v>1</v>
       </c>
       <c r="I74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -6009,16 +6071,16 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C75">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D75" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -6039,7 +6101,7 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75">
         <v>0</v>
@@ -6053,16 +6115,16 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C76">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D76" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -6097,16 +6159,16 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B77" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C77">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="D77" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -6141,16 +6203,16 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C78">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D78" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -6165,7 +6227,7 @@
         <v>1</v>
       </c>
       <c r="I78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -6185,16 +6247,16 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B79" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C79">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D79" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -6229,16 +6291,16 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B80" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C80">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -6279,10 +6341,10 @@
         <v>187</v>
       </c>
       <c r="C81">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D81" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -6323,10 +6385,10 @@
         <v>187</v>
       </c>
       <c r="C82">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="D82" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -6361,16 +6423,16 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B83" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C83">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D83" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -6391,10 +6453,10 @@
         <v>0</v>
       </c>
       <c r="K83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83">
         <v>0</v>
@@ -6405,16 +6467,16 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B84" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C84">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D84" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -6435,10 +6497,10 @@
         <v>0</v>
       </c>
       <c r="K84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M84">
         <v>0</v>
@@ -6449,16 +6511,16 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B85" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C85">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D85" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -6479,10 +6541,10 @@
         <v>0</v>
       </c>
       <c r="K85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M85">
         <v>0</v>
@@ -6493,10 +6555,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B86" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C86">
         <v>42</v>
@@ -6523,10 +6585,10 @@
         <v>0</v>
       </c>
       <c r="K86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M86">
         <v>0</v>
@@ -6537,16 +6599,16 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B87" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C87">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D87" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -6581,16 +6643,16 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C88">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D88" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -6625,16 +6687,16 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C89">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="D89" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -6669,16 +6731,16 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="C90">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D90" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -6719,10 +6781,10 @@
         <v>189</v>
       </c>
       <c r="C91">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D91" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -6763,10 +6825,10 @@
         <v>189</v>
       </c>
       <c r="C92">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D92" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -6807,10 +6869,10 @@
         <v>189</v>
       </c>
       <c r="C93">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D93" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -6851,10 +6913,10 @@
         <v>189</v>
       </c>
       <c r="C94">
-        <v>78</v>
+        <v>42</v>
       </c>
       <c r="D94" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -6889,16 +6951,16 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C95">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D95" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -6910,7 +6972,7 @@
         <v>1</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -6933,16 +6995,16 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B96" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C96">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D96" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -6977,16 +7039,16 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C97">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D97" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -7021,16 +7083,16 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C98">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D98" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -7065,16 +7127,16 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B99" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C99">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D99" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -7086,7 +7148,7 @@
         <v>1</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99">
         <v>1</v>
@@ -7115,10 +7177,10 @@
         <v>191</v>
       </c>
       <c r="C100">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D100" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -7153,16 +7215,16 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C101">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D101" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -7197,16 +7259,16 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B102" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C102">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D102" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -7241,16 +7303,16 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B103" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C103">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D103" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -7285,10 +7347,10 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B104" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C104">
         <v>42</v>
@@ -7329,16 +7391,16 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B105" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C105">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>230</v>
+        <v>353</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -7373,16 +7435,16 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B106" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C106">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="D106" t="s">
-        <v>231</v>
+        <v>354</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -7417,16 +7479,16 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B107" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C107">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="D107" t="s">
-        <v>232</v>
+        <v>355</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -7461,16 +7523,16 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B108" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C108">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D108" t="s">
-        <v>206</v>
+        <v>114</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -7511,10 +7573,10 @@
         <v>193</v>
       </c>
       <c r="C109">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D109" t="s">
-        <v>353</v>
+        <v>116</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -7555,10 +7617,10 @@
         <v>193</v>
       </c>
       <c r="C110">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D110" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -7599,10 +7661,10 @@
         <v>193</v>
       </c>
       <c r="C111">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D111" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -7643,10 +7705,10 @@
         <v>193</v>
       </c>
       <c r="C112">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D112" t="s">
-        <v>114</v>
+        <v>358</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -7687,10 +7749,10 @@
         <v>193</v>
       </c>
       <c r="C113">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D113" t="s">
-        <v>116</v>
+        <v>359</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -7731,10 +7793,10 @@
         <v>193</v>
       </c>
       <c r="C114">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D114" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -7775,10 +7837,10 @@
         <v>193</v>
       </c>
       <c r="C115">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D115" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -7819,10 +7881,10 @@
         <v>193</v>
       </c>
       <c r="C116">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D116" t="s">
-        <v>358</v>
+        <v>206</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -7857,16 +7919,16 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C117">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D117" t="s">
-        <v>359</v>
+        <v>209</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -7901,16 +7963,16 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C118">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="D118" t="s">
-        <v>360</v>
+        <v>234</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -7945,16 +8007,16 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C119">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="D119" t="s">
-        <v>361</v>
+        <v>235</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -7989,16 +8051,16 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>193</v>
+        <v>95</v>
       </c>
       <c r="C120">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D120" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -8019,10 +8081,10 @@
         <v>0</v>
       </c>
       <c r="K120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -8039,10 +8101,10 @@
         <v>442</v>
       </c>
       <c r="C121">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="D121" t="s">
-        <v>449</v>
+        <v>172</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -8083,10 +8145,10 @@
         <v>442</v>
       </c>
       <c r="C122">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D122" t="s">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -8127,10 +8189,10 @@
         <v>442</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>93</v>
       </c>
       <c r="D123" t="s">
-        <v>98</v>
+        <v>449</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -8171,10 +8233,10 @@
         <v>442</v>
       </c>
       <c r="C124">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="D124" t="s">
-        <v>206</v>
+        <v>450</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -8215,10 +8277,10 @@
         <v>442</v>
       </c>
       <c r="C125">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="D125" t="s">
-        <v>221</v>
+        <v>451</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -8259,10 +8321,10 @@
         <v>442</v>
       </c>
       <c r="C126">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D126" t="s">
-        <v>86</v>
+        <v>452</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -8297,16 +8359,16 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B127" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C127">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="D127" t="s">
-        <v>445</v>
+        <v>172</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -8341,16 +8403,16 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B128" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C128">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D128" t="s">
-        <v>446</v>
+        <v>86</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -8385,16 +8447,16 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C129">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D129" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -8429,16 +8491,16 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B130" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C130">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D130" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -8473,16 +8535,16 @@
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B131" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C131">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D131" t="s">
-        <v>92</v>
+        <v>451</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -8523,10 +8585,10 @@
         <v>443</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="D132" t="s">
-        <v>98</v>
+        <v>452</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -8561,16 +8623,16 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B133" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C133">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D133" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -8605,16 +8667,16 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B134" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C134">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D134" t="s">
-        <v>221</v>
+        <v>86</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -8649,16 +8711,16 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C135">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D135" t="s">
-        <v>86</v>
+        <v>449</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -8693,16 +8755,16 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C136">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D136" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -8737,16 +8799,16 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C137">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D137" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -8781,16 +8843,16 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B138" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C138">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D138" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -8820,666 +8882,6 @@
         <v>1</v>
       </c>
       <c r="N138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A139">
-        <v>29</v>
-      </c>
-      <c r="B139" t="s">
-        <v>443</v>
-      </c>
-      <c r="C139">
-        <v>96</v>
-      </c>
-      <c r="D139" t="s">
-        <v>448</v>
-      </c>
-      <c r="E139">
-        <v>1</v>
-      </c>
-      <c r="F139">
-        <v>1</v>
-      </c>
-      <c r="G139">
-        <v>0</v>
-      </c>
-      <c r="H139">
-        <v>1</v>
-      </c>
-      <c r="I139">
-        <v>0</v>
-      </c>
-      <c r="J139">
-        <v>1</v>
-      </c>
-      <c r="K139">
-        <v>0</v>
-      </c>
-      <c r="L139">
-        <v>0</v>
-      </c>
-      <c r="M139">
-        <v>1</v>
-      </c>
-      <c r="N139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A140">
-        <v>29</v>
-      </c>
-      <c r="B140" t="s">
-        <v>443</v>
-      </c>
-      <c r="C140">
-        <v>97</v>
-      </c>
-      <c r="D140" t="s">
-        <v>92</v>
-      </c>
-      <c r="E140">
-        <v>1</v>
-      </c>
-      <c r="F140">
-        <v>1</v>
-      </c>
-      <c r="G140">
-        <v>0</v>
-      </c>
-      <c r="H140">
-        <v>1</v>
-      </c>
-      <c r="I140">
-        <v>0</v>
-      </c>
-      <c r="J140">
-        <v>1</v>
-      </c>
-      <c r="K140">
-        <v>0</v>
-      </c>
-      <c r="L140">
-        <v>0</v>
-      </c>
-      <c r="M140">
-        <v>1</v>
-      </c>
-      <c r="N140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A141">
-        <v>29</v>
-      </c>
-      <c r="B141" t="s">
-        <v>443</v>
-      </c>
-      <c r="C141">
-        <v>48</v>
-      </c>
-      <c r="D141" t="s">
-        <v>172</v>
-      </c>
-      <c r="E141">
-        <v>1</v>
-      </c>
-      <c r="F141">
-        <v>1</v>
-      </c>
-      <c r="G141">
-        <v>0</v>
-      </c>
-      <c r="H141">
-        <v>1</v>
-      </c>
-      <c r="I141">
-        <v>0</v>
-      </c>
-      <c r="J141">
-        <v>1</v>
-      </c>
-      <c r="K141">
-        <v>0</v>
-      </c>
-      <c r="L141">
-        <v>0</v>
-      </c>
-      <c r="M141">
-        <v>1</v>
-      </c>
-      <c r="N141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A142">
-        <v>29</v>
-      </c>
-      <c r="B142" t="s">
-        <v>443</v>
-      </c>
-      <c r="C142">
-        <v>98</v>
-      </c>
-      <c r="D142" t="s">
-        <v>449</v>
-      </c>
-      <c r="E142">
-        <v>1</v>
-      </c>
-      <c r="F142">
-        <v>1</v>
-      </c>
-      <c r="G142">
-        <v>0</v>
-      </c>
-      <c r="H142">
-        <v>1</v>
-      </c>
-      <c r="I142">
-        <v>0</v>
-      </c>
-      <c r="J142">
-        <v>1</v>
-      </c>
-      <c r="K142">
-        <v>0</v>
-      </c>
-      <c r="L142">
-        <v>0</v>
-      </c>
-      <c r="M142">
-        <v>1</v>
-      </c>
-      <c r="N142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A143">
-        <v>30</v>
-      </c>
-      <c r="B143" t="s">
-        <v>444</v>
-      </c>
-      <c r="C143">
-        <v>98</v>
-      </c>
-      <c r="D143" t="s">
-        <v>449</v>
-      </c>
-      <c r="E143">
-        <v>1</v>
-      </c>
-      <c r="F143">
-        <v>1</v>
-      </c>
-      <c r="G143">
-        <v>0</v>
-      </c>
-      <c r="H143">
-        <v>1</v>
-      </c>
-      <c r="I143">
-        <v>0</v>
-      </c>
-      <c r="J143">
-        <v>1</v>
-      </c>
-      <c r="K143">
-        <v>0</v>
-      </c>
-      <c r="L143">
-        <v>0</v>
-      </c>
-      <c r="M143">
-        <v>1</v>
-      </c>
-      <c r="N143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>30</v>
-      </c>
-      <c r="B144" t="s">
-        <v>444</v>
-      </c>
-      <c r="C144">
-        <v>48</v>
-      </c>
-      <c r="D144" t="s">
-        <v>172</v>
-      </c>
-      <c r="E144">
-        <v>1</v>
-      </c>
-      <c r="F144">
-        <v>1</v>
-      </c>
-      <c r="G144">
-        <v>0</v>
-      </c>
-      <c r="H144">
-        <v>1</v>
-      </c>
-      <c r="I144">
-        <v>0</v>
-      </c>
-      <c r="J144">
-        <v>1</v>
-      </c>
-      <c r="K144">
-        <v>0</v>
-      </c>
-      <c r="L144">
-        <v>0</v>
-      </c>
-      <c r="M144">
-        <v>1</v>
-      </c>
-      <c r="N144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>30</v>
-      </c>
-      <c r="B145" t="s">
-        <v>444</v>
-      </c>
-      <c r="C145">
-        <v>1</v>
-      </c>
-      <c r="D145" t="s">
-        <v>98</v>
-      </c>
-      <c r="E145">
-        <v>1</v>
-      </c>
-      <c r="F145">
-        <v>1</v>
-      </c>
-      <c r="G145">
-        <v>0</v>
-      </c>
-      <c r="H145">
-        <v>1</v>
-      </c>
-      <c r="I145">
-        <v>0</v>
-      </c>
-      <c r="J145">
-        <v>1</v>
-      </c>
-      <c r="K145">
-        <v>0</v>
-      </c>
-      <c r="L145">
-        <v>0</v>
-      </c>
-      <c r="M145">
-        <v>1</v>
-      </c>
-      <c r="N145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>30</v>
-      </c>
-      <c r="B146" t="s">
-        <v>444</v>
-      </c>
-      <c r="C146">
-        <v>62</v>
-      </c>
-      <c r="D146" t="s">
-        <v>206</v>
-      </c>
-      <c r="E146">
-        <v>1</v>
-      </c>
-      <c r="F146">
-        <v>1</v>
-      </c>
-      <c r="G146">
-        <v>0</v>
-      </c>
-      <c r="H146">
-        <v>1</v>
-      </c>
-      <c r="I146">
-        <v>0</v>
-      </c>
-      <c r="J146">
-        <v>1</v>
-      </c>
-      <c r="K146">
-        <v>0</v>
-      </c>
-      <c r="L146">
-        <v>0</v>
-      </c>
-      <c r="M146">
-        <v>1</v>
-      </c>
-      <c r="N146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>30</v>
-      </c>
-      <c r="B147" t="s">
-        <v>444</v>
-      </c>
-      <c r="C147">
-        <v>77</v>
-      </c>
-      <c r="D147" t="s">
-        <v>221</v>
-      </c>
-      <c r="E147">
-        <v>1</v>
-      </c>
-      <c r="F147">
-        <v>1</v>
-      </c>
-      <c r="G147">
-        <v>0</v>
-      </c>
-      <c r="H147">
-        <v>1</v>
-      </c>
-      <c r="I147">
-        <v>0</v>
-      </c>
-      <c r="J147">
-        <v>1</v>
-      </c>
-      <c r="K147">
-        <v>0</v>
-      </c>
-      <c r="L147">
-        <v>0</v>
-      </c>
-      <c r="M147">
-        <v>1</v>
-      </c>
-      <c r="N147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>30</v>
-      </c>
-      <c r="B148" t="s">
-        <v>444</v>
-      </c>
-      <c r="C148">
-        <v>92</v>
-      </c>
-      <c r="D148" t="s">
-        <v>86</v>
-      </c>
-      <c r="E148">
-        <v>1</v>
-      </c>
-      <c r="F148">
-        <v>1</v>
-      </c>
-      <c r="G148">
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <v>1</v>
-      </c>
-      <c r="I148">
-        <v>0</v>
-      </c>
-      <c r="J148">
-        <v>1</v>
-      </c>
-      <c r="K148">
-        <v>0</v>
-      </c>
-      <c r="L148">
-        <v>0</v>
-      </c>
-      <c r="M148">
-        <v>1</v>
-      </c>
-      <c r="N148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>30</v>
-      </c>
-      <c r="B149" t="s">
-        <v>444</v>
-      </c>
-      <c r="C149">
-        <v>93</v>
-      </c>
-      <c r="D149" t="s">
-        <v>445</v>
-      </c>
-      <c r="E149">
-        <v>1</v>
-      </c>
-      <c r="F149">
-        <v>1</v>
-      </c>
-      <c r="G149">
-        <v>0</v>
-      </c>
-      <c r="H149">
-        <v>1</v>
-      </c>
-      <c r="I149">
-        <v>0</v>
-      </c>
-      <c r="J149">
-        <v>1</v>
-      </c>
-      <c r="K149">
-        <v>0</v>
-      </c>
-      <c r="L149">
-        <v>0</v>
-      </c>
-      <c r="M149">
-        <v>1</v>
-      </c>
-      <c r="N149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>30</v>
-      </c>
-      <c r="B150" t="s">
-        <v>444</v>
-      </c>
-      <c r="C150">
-        <v>94</v>
-      </c>
-      <c r="D150" t="s">
-        <v>446</v>
-      </c>
-      <c r="E150">
-        <v>1</v>
-      </c>
-      <c r="F150">
-        <v>1</v>
-      </c>
-      <c r="G150">
-        <v>0</v>
-      </c>
-      <c r="H150">
-        <v>1</v>
-      </c>
-      <c r="I150">
-        <v>0</v>
-      </c>
-      <c r="J150">
-        <v>1</v>
-      </c>
-      <c r="K150">
-        <v>0</v>
-      </c>
-      <c r="L150">
-        <v>0</v>
-      </c>
-      <c r="M150">
-        <v>1</v>
-      </c>
-      <c r="N150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>30</v>
-      </c>
-      <c r="B151" t="s">
-        <v>444</v>
-      </c>
-      <c r="C151">
-        <v>95</v>
-      </c>
-      <c r="D151" t="s">
-        <v>447</v>
-      </c>
-      <c r="E151">
-        <v>1</v>
-      </c>
-      <c r="F151">
-        <v>1</v>
-      </c>
-      <c r="G151">
-        <v>0</v>
-      </c>
-      <c r="H151">
-        <v>1</v>
-      </c>
-      <c r="I151">
-        <v>0</v>
-      </c>
-      <c r="J151">
-        <v>1</v>
-      </c>
-      <c r="K151">
-        <v>0</v>
-      </c>
-      <c r="L151">
-        <v>0</v>
-      </c>
-      <c r="M151">
-        <v>1</v>
-      </c>
-      <c r="N151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>30</v>
-      </c>
-      <c r="B152" t="s">
-        <v>444</v>
-      </c>
-      <c r="C152">
-        <v>96</v>
-      </c>
-      <c r="D152" t="s">
-        <v>448</v>
-      </c>
-      <c r="E152">
-        <v>1</v>
-      </c>
-      <c r="F152">
-        <v>1</v>
-      </c>
-      <c r="G152">
-        <v>0</v>
-      </c>
-      <c r="H152">
-        <v>1</v>
-      </c>
-      <c r="I152">
-        <v>0</v>
-      </c>
-      <c r="J152">
-        <v>1</v>
-      </c>
-      <c r="K152">
-        <v>0</v>
-      </c>
-      <c r="L152">
-        <v>0</v>
-      </c>
-      <c r="M152">
-        <v>1</v>
-      </c>
-      <c r="N152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A153">
-        <v>30</v>
-      </c>
-      <c r="B153" t="s">
-        <v>444</v>
-      </c>
-      <c r="C153">
-        <v>97</v>
-      </c>
-      <c r="D153" t="s">
-        <v>92</v>
-      </c>
-      <c r="E153">
-        <v>1</v>
-      </c>
-      <c r="F153">
-        <v>1</v>
-      </c>
-      <c r="G153">
-        <v>0</v>
-      </c>
-      <c r="H153">
-        <v>1</v>
-      </c>
-      <c r="I153">
-        <v>0</v>
-      </c>
-      <c r="J153">
-        <v>1</v>
-      </c>
-      <c r="K153">
-        <v>0</v>
-      </c>
-      <c r="L153">
-        <v>0</v>
-      </c>
-      <c r="M153">
-        <v>1</v>
-      </c>
-      <c r="N153">
         <v>1</v>
       </c>
     </row>
@@ -14581,9 +13983,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15348,7 +14752,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -15356,7 +14760,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -15364,7 +14768,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -15372,23 +14776,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>97</v>
-      </c>
-      <c r="B99" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>98</v>
-      </c>
-      <c r="B100" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@11/19/2014 11:29:48 AM] Updates for ETS feed. SCR 13659. Internal version 10.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13810
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="9" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="471">
   <si>
     <t>SourceID</t>
   </si>
@@ -1397,6 +1397,51 @@
   </si>
   <si>
     <t>Added job_code WPWL51 (Manager, Regional)to Module_Submission table for submitting Supervisor ecls.</t>
+  </si>
+  <si>
+    <t>Added records for ETS feed functionality.</t>
+  </si>
+  <si>
+    <t>Excused absence, paid leave</t>
+  </si>
+  <si>
+    <t>Exempt OT Hours</t>
+  </si>
+  <si>
+    <t>Future hours</t>
+  </si>
+  <si>
+    <t>Future hours (Approver)</t>
+  </si>
+  <si>
+    <t>Holiday Hours</t>
+  </si>
+  <si>
+    <t>Holiday Hours (Approver)</t>
+  </si>
+  <si>
+    <t>Invalid time code – Direct</t>
+  </si>
+  <si>
+    <t>Invalid time code – Direct (Approver)</t>
+  </si>
+  <si>
+    <t>Invalid time code – Paid leave</t>
+  </si>
+  <si>
+    <t>Invalid time code – Paid leave (Approver)</t>
+  </si>
+  <si>
+    <t>Utilization</t>
+  </si>
+  <si>
+    <t>Utilization (Approver)</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on behalf of &lt;strong&gt; strPerson &lt;/strong&gt;  on &lt;strong&gt; strDateTime &lt;/strong&gt; that requires your action. Please click on the link below to review the eCoaching log.</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on behalf of  &lt;strong&gt; strPerson &lt;/strong&gt; on &lt;strong&gt;  strDateTime  &lt;/strong&gt; that requires your action. Please click on the link below to review the eCoaching log.</t>
   </si>
 </sst>
 </file>
@@ -1754,11 +1799,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1951,6 +1994,23 @@
       </c>
       <c r="E11" t="s">
         <v>455</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>41957</v>
+      </c>
+      <c r="C12" t="s">
+        <v>434</v>
+      </c>
+      <c r="D12">
+        <v>13659</v>
+      </c>
+      <c r="E12" t="s">
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -2809,7 +2869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A98" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8992,9 +9052,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10833,7 +10893,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
         <v>380</v>
@@ -10842,22 +10902,22 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>441</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="G53" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H53" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="I53" t="s">
-        <v>413</v>
+        <v>381</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -10868,31 +10928,31 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" t="s">
         <v>175</v>
       </c>
-      <c r="B54" t="s">
-        <v>380</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
-      </c>
-      <c r="F54" t="s">
-        <v>178</v>
-      </c>
-      <c r="G54" t="s">
-        <v>382</v>
-      </c>
       <c r="H54" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I54" t="s">
-        <v>414</v>
+        <v>469</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -10903,7 +10963,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
         <v>380</v>
@@ -10912,22 +10972,22 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G55" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H55" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I55" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -10938,7 +10998,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B56" t="s">
         <v>380</v>
@@ -10947,22 +11007,22 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G56" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H56" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I56" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -10973,7 +11033,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B57" t="s">
         <v>380</v>
@@ -10982,22 +11042,22 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G57" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H57" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I57" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -11008,7 +11068,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B58" t="s">
         <v>380</v>
@@ -11017,7 +11077,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -11032,7 +11092,7 @@
         <v>385</v>
       </c>
       <c r="I58" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -11043,7 +11103,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B59" t="s">
         <v>380</v>
@@ -11052,7 +11112,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -11067,7 +11127,7 @@
         <v>385</v>
       </c>
       <c r="I59" t="s">
-        <v>417</v>
+        <v>400</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -11078,7 +11138,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
         <v>380</v>
@@ -11087,7 +11147,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -11102,7 +11162,7 @@
         <v>385</v>
       </c>
       <c r="I60" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -11113,7 +11173,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B61" t="s">
         <v>380</v>
@@ -11122,7 +11182,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -11137,7 +11197,7 @@
         <v>385</v>
       </c>
       <c r="I61" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -11148,7 +11208,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B62" t="s">
         <v>380</v>
@@ -11157,7 +11217,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -11172,7 +11232,7 @@
         <v>385</v>
       </c>
       <c r="I62" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -11183,31 +11243,31 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
         <v>380</v>
       </c>
       <c r="C63" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G63" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H63" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I63" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -11218,31 +11278,31 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
         <v>380</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G64" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H64" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I64" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -11253,7 +11313,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
         <v>380</v>
@@ -11262,22 +11322,22 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G65" t="s">
         <v>175</v>
       </c>
       <c r="H65" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I65" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -11288,7 +11348,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
         <v>380</v>
@@ -11297,22 +11357,22 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>8</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G66" t="s">
         <v>175</v>
       </c>
       <c r="H66" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I66" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -11323,7 +11383,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
         <v>380</v>
@@ -11332,22 +11392,22 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G67" t="s">
         <v>175</v>
       </c>
       <c r="H67" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I67" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -11358,7 +11418,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B68" t="s">
         <v>380</v>
@@ -11367,22 +11427,22 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G68" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H68" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I68" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -11393,7 +11453,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
         <v>380</v>
@@ -11402,22 +11462,22 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G69" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H69" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I69" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -11428,7 +11488,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B70" t="s">
         <v>380</v>
@@ -11437,22 +11497,22 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G70" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H70" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I70" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -11463,7 +11523,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
         <v>380</v>
@@ -11472,22 +11532,22 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G71" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H71" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I71" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -11498,7 +11558,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B72" t="s">
         <v>380</v>
@@ -11507,22 +11567,22 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G72" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H72" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I72" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -11539,25 +11599,25 @@
         <v>380</v>
       </c>
       <c r="C73" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G73" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H73" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I73" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -11574,25 +11634,25 @@
         <v>380</v>
       </c>
       <c r="C74" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G74" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H74" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I74" t="s">
-        <v>400</v>
+        <v>425</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -11603,31 +11663,31 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B75" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G75" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H75" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I75" t="s">
-        <v>423</v>
+        <v>470</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -11638,7 +11698,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
         <v>380</v>
@@ -11647,22 +11707,22 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G76" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H76" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I76" t="s">
-        <v>400</v>
+        <v>413</v>
       </c>
       <c r="J76">
         <v>0</v>
@@ -11673,7 +11733,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B77" t="s">
         <v>380</v>
@@ -11682,22 +11742,22 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>170</v>
+        <v>13</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G77" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H77" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I77" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -11708,7 +11768,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
         <v>380</v>
@@ -11717,22 +11777,22 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G78" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H78" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I78" t="s">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -11743,7 +11803,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
         <v>380</v>
@@ -11752,22 +11812,22 @@
         <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G79" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H79" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I79" t="s">
-        <v>399</v>
+        <v>415</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -11778,7 +11838,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B80" t="s">
         <v>380</v>
@@ -11787,22 +11847,22 @@
         <v>5</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G80" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H80" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I80" t="s">
-        <v>400</v>
+        <v>414</v>
       </c>
       <c r="J80">
         <v>0</v>
@@ -11813,7 +11873,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B81" t="s">
         <v>380</v>
@@ -11822,7 +11882,7 @@
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -11837,7 +11897,7 @@
         <v>385</v>
       </c>
       <c r="I81" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -11848,7 +11908,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B82" t="s">
         <v>380</v>
@@ -11857,7 +11917,7 @@
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -11872,7 +11932,7 @@
         <v>385</v>
       </c>
       <c r="I82" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -11883,31 +11943,31 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
         <v>380</v>
       </c>
       <c r="C83" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G83" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H83" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I83" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="J83">
         <v>0</v>
@@ -11918,31 +11978,31 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B84" t="s">
         <v>380</v>
       </c>
       <c r="C84" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G84" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H84" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I84" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="J84">
         <v>0</v>
@@ -11953,31 +12013,31 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
         <v>380</v>
       </c>
       <c r="C85" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G85" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H85" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I85" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -11988,7 +12048,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B86" t="s">
         <v>380</v>
@@ -11997,22 +12057,22 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G86" t="s">
         <v>175</v>
       </c>
       <c r="H86" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I86" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -12023,7 +12083,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
         <v>380</v>
@@ -12032,22 +12092,22 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>170</v>
+        <v>13</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G87" t="s">
         <v>175</v>
       </c>
       <c r="H87" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I87" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -12058,7 +12118,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B88" t="s">
         <v>380</v>
@@ -12067,22 +12127,22 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G88" t="s">
         <v>175</v>
       </c>
       <c r="H88" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I88" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J88">
         <v>0</v>
@@ -12093,7 +12153,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
         <v>380</v>
@@ -12102,22 +12162,22 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G89" t="s">
         <v>175</v>
       </c>
       <c r="H89" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I89" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="J89">
         <v>0</v>
@@ -12128,7 +12188,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B90" t="s">
         <v>380</v>
@@ -12137,22 +12197,22 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G90" t="s">
         <v>175</v>
       </c>
       <c r="H90" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I90" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -12163,7 +12223,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B91" t="s">
         <v>380</v>
@@ -12172,22 +12232,22 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G91" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H91" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I91" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J91">
         <v>0</v>
@@ -12198,7 +12258,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B92" t="s">
         <v>380</v>
@@ -12207,22 +12267,22 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G92" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H92" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I92" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="J92">
         <v>0</v>
@@ -12233,36 +12293,106 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B93" t="s">
         <v>380</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>441</v>
+        <v>14</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="G93" t="s">
+        <v>382</v>
+      </c>
+      <c r="H93" t="s">
+        <v>391</v>
+      </c>
+      <c r="I93" t="s">
+        <v>415</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93" t="s">
         <v>381</v>
       </c>
-      <c r="H93" t="s">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>175</v>
+      </c>
+      <c r="B94" t="s">
+        <v>380</v>
+      </c>
+      <c r="C94" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" t="s">
+        <v>171</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
+        <v>178</v>
+      </c>
+      <c r="G94" t="s">
+        <v>382</v>
+      </c>
+      <c r="H94" t="s">
+        <v>391</v>
+      </c>
+      <c r="I94" t="s">
+        <v>415</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94" t="s">
         <v>381</v>
       </c>
-      <c r="I93" t="s">
-        <v>381</v>
-      </c>
-      <c r="J93">
-        <v>0</v>
-      </c>
-      <c r="K93" t="s">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" t="s">
+        <v>380</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>176</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="s">
+        <v>178</v>
+      </c>
+      <c r="G95" t="s">
+        <v>382</v>
+      </c>
+      <c r="H95" t="s">
+        <v>391</v>
+      </c>
+      <c r="I95" t="s">
+        <v>415</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95" t="s">
         <v>381</v>
       </c>
     </row>
@@ -12275,7 +12405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -12285,9 +12415,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12827,19 +12957,19 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>201</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>172</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -12850,13 +12980,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s">
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -12868,18 +12998,18 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -12896,13 +13026,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -12919,13 +13049,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -12942,13 +13072,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -12965,13 +13095,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -12988,13 +13118,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -13003,7 +13133,7 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -13011,13 +13141,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -13034,13 +13164,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -13057,36 +13187,36 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -13103,13 +13233,13 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -13126,13 +13256,13 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -13149,13 +13279,13 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -13172,13 +13302,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -13195,13 +13325,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -13218,70 +13348,116 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
         <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>220</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>441</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>221</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
         <v>0</v>
       </c>
     </row>
@@ -13983,11 +14159,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14777,6 +14951,102 @@
       </c>
       <c r="B98" t="s">
         <v>452</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -15334,7 +15604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@11/21/2014 4:23:16 PM] Internal version 11. Updated for SCR 13826.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13828
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="479">
   <si>
     <t>SourceID</t>
   </si>
@@ -1441,7 +1441,31 @@
     <t>A new eCoaching Log has been entered on behalf of &lt;strong&gt; strPerson &lt;/strong&gt;  on &lt;strong&gt; strDateTime &lt;/strong&gt; that requires your action. Please click on the link below to review the eCoaching log.</t>
   </si>
   <si>
-    <t>A new eCoaching Log has been entered on behalf of  &lt;strong&gt; strPerson &lt;/strong&gt; on &lt;strong&gt;  strDateTime  &lt;/strong&gt; that requires your action. Please click on the link below to review the eCoaching log.</t>
+    <t>Added additional sub sources for IQS feed.</t>
+  </si>
+  <si>
+    <t>LimeSurvey</t>
+  </si>
+  <si>
+    <t>Verint-GDIT</t>
+  </si>
+  <si>
+    <t>Verint-TQC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LimeSurvey </t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on behalf of &lt;strong&gt; strPerson &lt;/strong&gt;  on &lt;strong&gt; strDateTime &lt;/strong&gt; that requires your    action. Please click on the link below to review the eCoaching log.</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on behalf of  &lt;strong&gt; strPerson &lt;/strong&gt; on &lt;strong&gt;  strDateTime  &lt;/strong&gt; that requires your action.    Please click on the link below to review the eCoaching log.</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered on your behalf. Please click on the link below to review and verify the coaching opportunity received on &lt;strong&gt; strDateTime &lt;/strong&gt;.</t>
+  </si>
+  <si>
+    <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;strong&gt; strDateTime &lt;/strong&gt; for &lt;strong&gt; strPerson &lt;/strong&gt; is a valid Customer Service Escalation (CSE). Further directions are provided on the form.</t>
   </si>
 </sst>
 </file>
@@ -1799,9 +1823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2011,6 +2037,23 @@
       </c>
       <c r="E12" t="s">
         <v>456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>41964</v>
+      </c>
+      <c r="C13" t="s">
+        <v>434</v>
+      </c>
+      <c r="D13">
+        <v>13826</v>
+      </c>
+      <c r="E13" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -9052,9 +9095,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K95"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9467,22 +9510,22 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>441</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H12" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I12" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -9502,22 +9545,22 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -9537,10 +9580,10 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>177</v>
@@ -9549,10 +9592,10 @@
         <v>427</v>
       </c>
       <c r="H14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -9572,7 +9615,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -9607,7 +9650,7 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -9622,7 +9665,7 @@
         <v>385</v>
       </c>
       <c r="I16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -9642,7 +9685,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -9657,7 +9700,7 @@
         <v>385</v>
       </c>
       <c r="I17" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -9677,7 +9720,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -9712,7 +9755,7 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -9747,7 +9790,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -9762,7 +9805,7 @@
         <v>385</v>
       </c>
       <c r="I20" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -9782,7 +9825,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -9797,7 +9840,7 @@
         <v>385</v>
       </c>
       <c r="I21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -9817,7 +9860,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -9832,7 +9875,7 @@
         <v>385</v>
       </c>
       <c r="I22" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -9852,7 +9895,7 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -9884,25 +9927,25 @@
         <v>380</v>
       </c>
       <c r="C24" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G24" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H24" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I24" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -9922,7 +9965,7 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -9948,31 +9991,31 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
         <v>380</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="G26" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H26" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="I26" t="s">
-        <v>401</v>
+        <v>413</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -9983,31 +10026,31 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
         <v>380</v>
       </c>
       <c r="C27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="G27" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H27" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="I27" t="s">
-        <v>402</v>
+        <v>414</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -10018,31 +10061,31 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
         <v>380</v>
       </c>
       <c r="C28" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="G28" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H28" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="I28" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -10053,31 +10096,31 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s">
         <v>380</v>
       </c>
       <c r="C29" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="G29" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H29" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="I29" t="s">
-        <v>401</v>
+        <v>415</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -10088,31 +10131,31 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B30" t="s">
         <v>380</v>
       </c>
       <c r="C30" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="G30" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H30" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="I30" t="s">
-        <v>401</v>
+        <v>414</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -10123,13 +10166,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B31" t="s">
         <v>380</v>
       </c>
       <c r="C31" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -10138,16 +10181,16 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G31" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I31" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -10158,13 +10201,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B32" t="s">
         <v>380</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -10173,16 +10216,16 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G32" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I32" t="s">
-        <v>401</v>
+        <v>417</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -10193,13 +10236,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B33" t="s">
         <v>380</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
@@ -10208,16 +10251,16 @@
         <v>0</v>
       </c>
       <c r="F33" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G33" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H33" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I33" t="s">
-        <v>402</v>
+        <v>418</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -10228,13 +10271,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B34" t="s">
         <v>380</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
         <v>171</v>
@@ -10243,16 +10286,16 @@
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G34" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I34" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -10263,31 +10306,31 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
         <v>380</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G35" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H35" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I35" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -10298,7 +10341,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B36" t="s">
         <v>380</v>
@@ -10307,22 +10350,22 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F36" t="s">
         <v>27</v>
       </c>
       <c r="G36" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H36" t="s">
         <v>383</v>
       </c>
       <c r="I36" t="s">
-        <v>405</v>
+        <v>419</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -10342,22 +10385,22 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H37" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I37" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -10377,22 +10420,22 @@
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G38" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H38" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I38" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -10412,22 +10455,22 @@
         <v>3</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G39" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H39" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -10447,22 +10490,22 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G40" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H40" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I40" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -10482,22 +10525,22 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G41" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H41" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I41" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -10517,22 +10560,22 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G42" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H42" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I42" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -10552,22 +10595,22 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G43" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H43" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I43" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -10587,22 +10630,22 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G44" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H44" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I44" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -10622,22 +10665,22 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G45" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H45" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I45" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -10651,28 +10694,28 @@
         <v>174</v>
       </c>
       <c r="B46" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G46" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H46" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I46" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -10686,28 +10729,28 @@
         <v>174</v>
       </c>
       <c r="B47" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C47" t="s">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G47" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H47" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="I47" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -10721,28 +10764,28 @@
         <v>174</v>
       </c>
       <c r="B48" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G48" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H48" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I48" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -10753,31 +10796,31 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B49" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C49" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G49" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H49" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I49" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -10788,31 +10831,31 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="G50" t="s">
         <v>427</v>
       </c>
       <c r="H50" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I50" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -10823,31 +10866,31 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G51" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H51" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I51" t="s">
-        <v>411</v>
+        <v>423</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -10858,31 +10901,31 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C52" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G52" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="H52" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I52" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -10893,7 +10936,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
         <v>380</v>
@@ -10902,22 +10945,22 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>441</v>
+        <v>170</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="G53" t="s">
-        <v>381</v>
+        <v>427</v>
       </c>
       <c r="H53" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="I53" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -10928,31 +10971,31 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
-        <v>172</v>
+        <v>380</v>
       </c>
       <c r="C54" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>11</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G54" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H54" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I54" t="s">
-        <v>469</v>
+        <v>400</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -10972,7 +11015,7 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -10987,7 +11030,7 @@
         <v>385</v>
       </c>
       <c r="I55" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -11007,7 +11050,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -11042,7 +11085,7 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -11077,7 +11120,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -11092,7 +11135,7 @@
         <v>385</v>
       </c>
       <c r="I58" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -11109,25 +11152,25 @@
         <v>380</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>170</v>
+        <v>7</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G59" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H59" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I59" t="s">
-        <v>400</v>
+        <v>424</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -11144,25 +11187,25 @@
         <v>380</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G60" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H60" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I60" t="s">
-        <v>400</v>
+        <v>424</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -11179,25 +11222,25 @@
         <v>380</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G61" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H61" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="I61" t="s">
-        <v>399</v>
+        <v>425</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -11208,31 +11251,31 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B62" t="s">
         <v>380</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G62" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H62" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I62" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -11243,31 +11286,31 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B63" t="s">
         <v>380</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G63" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H63" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I63" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -11278,31 +11321,31 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B64" t="s">
         <v>380</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>171</v>
+        <v>10</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G64" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H64" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I64" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -11313,7 +11356,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
         <v>380</v>
@@ -11322,22 +11365,22 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G65" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H65" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I65" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -11348,7 +11391,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B66" t="s">
         <v>380</v>
@@ -11357,22 +11400,22 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G66" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H66" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I66" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -11383,7 +11426,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
         <v>380</v>
@@ -11392,22 +11435,22 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G67" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H67" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I67" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -11418,7 +11461,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B68" t="s">
         <v>380</v>
@@ -11427,22 +11470,22 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G68" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H68" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I68" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -11453,7 +11496,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B69" t="s">
         <v>380</v>
@@ -11462,22 +11505,22 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G69" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H69" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I69" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -11488,7 +11531,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B70" t="s">
         <v>380</v>
@@ -11497,22 +11540,22 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G70" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H70" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I70" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -11523,31 +11566,31 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B71" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C71" t="s">
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="G71" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H71" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I71" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -11558,31 +11601,31 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B72" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C72" t="s">
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
       <c r="G72" t="s">
         <v>175</v>
       </c>
       <c r="H72" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="I72" t="s">
-        <v>424</v>
+        <v>475</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -11593,31 +11636,31 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C73" t="s">
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="G73" t="s">
         <v>175</v>
       </c>
       <c r="H73" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="I73" t="s">
-        <v>425</v>
+        <v>476</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -11628,31 +11671,31 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B74" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C74" t="s">
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>171</v>
+        <v>16</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G74" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H74" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I74" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -11663,31 +11706,31 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B75" t="s">
-        <v>172</v>
+        <v>387</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G75" t="s">
         <v>175</v>
       </c>
       <c r="H75" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I75" t="s">
-        <v>470</v>
+        <v>408</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -11698,31 +11741,31 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C76" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G76" t="s">
         <v>382</v>
       </c>
       <c r="H76" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I76" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="J76">
         <v>0</v>
@@ -11733,31 +11776,31 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B77" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C77" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>178</v>
+        <v>26</v>
       </c>
       <c r="G77" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H77" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="I77" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -11768,31 +11811,31 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>28</v>
+      </c>
+      <c r="G78" t="s">
         <v>175</v>
       </c>
-      <c r="B78" t="s">
-        <v>380</v>
-      </c>
-      <c r="C78" t="s">
-        <v>5</v>
-      </c>
-      <c r="D78" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78" t="s">
-        <v>178</v>
-      </c>
-      <c r="G78" t="s">
-        <v>382</v>
-      </c>
       <c r="H78" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I78" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -11803,31 +11846,31 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B79" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>171</v>
+        <v>15</v>
       </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G79" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="H79" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I79" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -11844,25 +11887,25 @@
         <v>380</v>
       </c>
       <c r="C80" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G80" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H80" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I80" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="J80">
         <v>0</v>
@@ -11879,25 +11922,25 @@
         <v>380</v>
       </c>
       <c r="C81" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G81" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H81" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I81" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -11914,25 +11957,25 @@
         <v>380</v>
       </c>
       <c r="C82" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G82" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H82" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I82" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -11949,25 +11992,25 @@
         <v>380</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G83" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H83" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I83" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J83">
         <v>0</v>
@@ -11984,25 +12027,25 @@
         <v>380</v>
       </c>
       <c r="C84" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G84" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H84" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I84" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="J84">
         <v>0</v>
@@ -12019,25 +12062,25 @@
         <v>380</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F85" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G85" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H85" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I85" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -12057,22 +12100,22 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="G86" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H86" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="I86" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -12092,22 +12135,22 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="G87" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H87" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="I87" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -12127,22 +12170,22 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="G88" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H88" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="I88" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="J88">
         <v>0</v>
@@ -12153,7 +12196,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
         <v>380</v>
@@ -12162,22 +12205,22 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>171</v>
+        <v>10</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G89" t="s">
         <v>175</v>
       </c>
       <c r="H89" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I89" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="J89">
         <v>0</v>
@@ -12188,7 +12231,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
         <v>380</v>
@@ -12197,22 +12240,22 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G90" t="s">
         <v>175</v>
       </c>
       <c r="H90" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I90" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -12223,7 +12266,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B91" t="s">
         <v>380</v>
@@ -12232,22 +12275,22 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G91" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H91" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I91" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J91">
         <v>0</v>
@@ -12258,7 +12301,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
         <v>380</v>
@@ -12267,22 +12310,22 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G92" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H92" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I92" t="s">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="J92">
         <v>0</v>
@@ -12293,7 +12336,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>380</v>
@@ -12302,22 +12345,22 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G93" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H93" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I93" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="J93">
         <v>0</v>
@@ -12328,7 +12371,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>380</v>
@@ -12337,22 +12380,22 @@
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G94" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H94" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I94" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="J94">
         <v>0</v>
@@ -12363,7 +12406,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
         <v>380</v>
@@ -12372,27 +12415,342 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G95" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H95" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I95" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="J95">
         <v>0</v>
       </c>
       <c r="K95" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>174</v>
+      </c>
+      <c r="B96" t="s">
+        <v>15</v>
+      </c>
+      <c r="C96" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" t="s">
+        <v>471</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96" t="s">
+        <v>427</v>
+      </c>
+      <c r="H96" t="s">
+        <v>388</v>
+      </c>
+      <c r="I96" t="s">
+        <v>477</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" t="s">
+        <v>3</v>
+      </c>
+      <c r="D97" t="s">
+        <v>471</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" t="s">
+        <v>28</v>
+      </c>
+      <c r="G97" t="s">
+        <v>175</v>
+      </c>
+      <c r="H97" t="s">
+        <v>386</v>
+      </c>
+      <c r="I97" t="s">
+        <v>469</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>174</v>
+      </c>
+      <c r="B98" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" t="s">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
+        <v>471</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+      <c r="F98" t="s">
+        <v>27</v>
+      </c>
+      <c r="G98" t="s">
+        <v>390</v>
+      </c>
+      <c r="H98" t="s">
+        <v>383</v>
+      </c>
+      <c r="I98" t="s">
+        <v>478</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>174</v>
+      </c>
+      <c r="B99" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" t="s">
+        <v>3</v>
+      </c>
+      <c r="D99" t="s">
+        <v>472</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G99" t="s">
+        <v>427</v>
+      </c>
+      <c r="H99" t="s">
+        <v>388</v>
+      </c>
+      <c r="I99" t="s">
+        <v>477</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>174</v>
+      </c>
+      <c r="B100" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" t="s">
+        <v>472</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>28</v>
+      </c>
+      <c r="G100" t="s">
+        <v>175</v>
+      </c>
+      <c r="H100" t="s">
+        <v>386</v>
+      </c>
+      <c r="I100" t="s">
+        <v>469</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" t="s">
+        <v>472</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" t="s">
+        <v>27</v>
+      </c>
+      <c r="G101" t="s">
+        <v>390</v>
+      </c>
+      <c r="H101" t="s">
+        <v>383</v>
+      </c>
+      <c r="I101" t="s">
+        <v>478</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" t="s">
+        <v>473</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102" t="s">
+        <v>26</v>
+      </c>
+      <c r="G102" t="s">
+        <v>427</v>
+      </c>
+      <c r="H102" t="s">
+        <v>388</v>
+      </c>
+      <c r="I102" t="s">
+        <v>477</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>174</v>
+      </c>
+      <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>473</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103" t="s">
+        <v>28</v>
+      </c>
+      <c r="G103" t="s">
+        <v>175</v>
+      </c>
+      <c r="H103" t="s">
+        <v>386</v>
+      </c>
+      <c r="I103" t="s">
+        <v>469</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>174</v>
+      </c>
+      <c r="B104" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" t="s">
+        <v>473</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>27</v>
+      </c>
+      <c r="G104" t="s">
+        <v>390</v>
+      </c>
+      <c r="H104" t="s">
+        <v>383</v>
+      </c>
+      <c r="I104" t="s">
+        <v>478</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104" t="s">
         <v>381</v>
       </c>
     </row>
@@ -12405,7 +12763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -12415,9 +12773,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12980,19 +13338,19 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>201</v>
+        <v>122</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>471</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -13003,59 +13361,59 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>202</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>472</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>203</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>473</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -13067,18 +13425,18 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -13095,13 +13453,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -13118,13 +13476,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -13141,13 +13499,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -13156,7 +13514,7 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -13164,13 +13522,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -13179,7 +13537,7 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>1</v>
@@ -13187,13 +13545,13 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -13202,7 +13560,7 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -13210,82 +13568,82 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -13302,13 +13660,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -13325,13 +13683,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -13348,13 +13706,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -13371,36 +13729,36 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>171</v>
+        <v>19</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -13409,7 +13767,7 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -13417,13 +13775,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>441</v>
+        <v>21</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -13440,24 +13798,162 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>219</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>220</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>441</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>221</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
         <v>172</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>222</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>474</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>223</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>472</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>224</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>473</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@11/21/2014 6:23:18 PM] Internal version 12. Updated for SCR 13542 Supervisor warnings.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13832
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="480">
   <si>
     <t>SourceID</t>
   </si>
@@ -1466,6 +1466,9 @@
   </si>
   <si>
     <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;strong&gt; strDateTime &lt;/strong&gt; for &lt;strong&gt; strPerson &lt;/strong&gt; is a valid Customer Service Escalation (CSE). Further directions are provided on the form.</t>
+  </si>
+  <si>
+    <t>Enabled  supervisor flag for warnings coaching reasons in coaching reason selection table and added an email attribute entry for supervisor module and warning.</t>
   </si>
 </sst>
 </file>
@@ -1823,11 +1826,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1835,7 +1836,7 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="96.42578125" customWidth="1"/>
+    <col min="5" max="5" width="78" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2054,6 +2055,23 @@
       </c>
       <c r="E13" t="s">
         <v>470</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41964</v>
+      </c>
+      <c r="C14" t="s">
+        <v>434</v>
+      </c>
+      <c r="D14">
+        <v>13542</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -2912,7 +2930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N138"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0"/>
+    <sheetView topLeftCell="A92" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8231,7 +8249,7 @@
         <v>0</v>
       </c>
       <c r="L121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M121">
         <v>1</v>
@@ -8275,7 +8293,7 @@
         <v>0</v>
       </c>
       <c r="L122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M122">
         <v>1</v>
@@ -8319,7 +8337,7 @@
         <v>0</v>
       </c>
       <c r="L123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M123">
         <v>1</v>
@@ -8363,7 +8381,7 @@
         <v>0</v>
       </c>
       <c r="L124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M124">
         <v>1</v>
@@ -8407,7 +8425,7 @@
         <v>0</v>
       </c>
       <c r="L125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M125">
         <v>1</v>
@@ -8451,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="L126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M126">
         <v>1</v>
@@ -8495,7 +8513,7 @@
         <v>0</v>
       </c>
       <c r="L127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M127">
         <v>1</v>
@@ -8539,7 +8557,7 @@
         <v>0</v>
       </c>
       <c r="L128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M128">
         <v>1</v>
@@ -8583,7 +8601,7 @@
         <v>0</v>
       </c>
       <c r="L129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M129">
         <v>1</v>
@@ -8627,7 +8645,7 @@
         <v>0</v>
       </c>
       <c r="L130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M130">
         <v>1</v>
@@ -8671,7 +8689,7 @@
         <v>0</v>
       </c>
       <c r="L131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M131">
         <v>1</v>
@@ -8715,7 +8733,7 @@
         <v>0</v>
       </c>
       <c r="L132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M132">
         <v>1</v>
@@ -8759,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="L133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M133">
         <v>1</v>
@@ -8803,7 +8821,7 @@
         <v>0</v>
       </c>
       <c r="L134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M134">
         <v>1</v>
@@ -8847,7 +8865,7 @@
         <v>0</v>
       </c>
       <c r="L135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M135">
         <v>1</v>
@@ -8891,7 +8909,7 @@
         <v>0</v>
       </c>
       <c r="L136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M136">
         <v>1</v>
@@ -8935,7 +8953,7 @@
         <v>0</v>
       </c>
       <c r="L137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M137">
         <v>1</v>
@@ -8979,7 +8997,7 @@
         <v>0</v>
       </c>
       <c r="L138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M138">
         <v>1</v>
@@ -9095,9 +9113,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K104"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12751,6 +12769,41 @@
         <v>0</v>
       </c>
       <c r="K104" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>175</v>
+      </c>
+      <c r="B105" t="s">
+        <v>380</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>441</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G105" t="s">
+        <v>381</v>
+      </c>
+      <c r="H105" t="s">
+        <v>381</v>
+      </c>
+      <c r="I105" t="s">
+        <v>381</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105" t="s">
         <v>381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@12/18/2014 11:54:28 AM] Internal version 13. Updated for SCR 14028 new OMR report.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13863
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="482">
   <si>
     <t>SourceID</t>
   </si>
@@ -1469,6 +1469,12 @@
   </si>
   <si>
     <t>Enabled  supervisor flag for warnings coaching reasons in coaching reason selection table and added an email attribute entry for supervisor module and warning.</t>
+  </si>
+  <si>
+    <t>Added DIM values for noew TR2 OMR report in DIM Subcoahing reason and coaching reason selection tables</t>
+  </si>
+  <si>
+    <t>OMR: FFM T2 Transfers</t>
   </si>
 </sst>
 </file>
@@ -1826,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2072,6 +2078,23 @@
       </c>
       <c r="E14" s="3" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41991</v>
+      </c>
+      <c r="C15" t="s">
+        <v>434</v>
+      </c>
+      <c r="D15">
+        <v>14028</v>
+      </c>
+      <c r="E15" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -2928,9 +2951,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N138"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0"/>
+    <sheetView topLeftCell="A93" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2980,25 +3003,25 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>481</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3007,7 +3030,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3024,25 +3047,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>42</v>
+        <v>-1</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -3051,13 +3074,13 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -3068,16 +3091,16 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3101,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -3118,10 +3141,10 @@
         <v>85</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3162,10 +3185,10 @@
         <v>85</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3206,10 +3229,10 @@
         <v>85</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3250,10 +3273,10 @@
         <v>85</v>
       </c>
       <c r="C8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3294,10 +3317,10 @@
         <v>85</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3338,10 +3361,10 @@
         <v>85</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3382,10 +3405,10 @@
         <v>85</v>
       </c>
       <c r="C11">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3420,16 +3443,16 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3438,7 +3461,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -3470,10 +3493,10 @@
         <v>86</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -3482,7 +3505,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -3494,10 +3517,10 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3508,16 +3531,16 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -3538,7 +3561,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -3558,10 +3581,10 @@
         <v>181</v>
       </c>
       <c r="C15">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -3596,10 +3619,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="C16">
         <v>42</v>
@@ -3629,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3640,16 +3663,16 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3664,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -3673,13 +3696,13 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3690,10 +3713,10 @@
         <v>88</v>
       </c>
       <c r="C18">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>100</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3734,10 +3757,10 @@
         <v>88</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -3761,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -3778,10 +3801,10 @@
         <v>88</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -3805,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -3822,10 +3845,10 @@
         <v>88</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>346</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -3866,10 +3889,10 @@
         <v>88</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -3910,10 +3933,10 @@
         <v>88</v>
       </c>
       <c r="C23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>347</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -3954,10 +3977,10 @@
         <v>88</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>236</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -3998,10 +4021,10 @@
         <v>88</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -4042,10 +4065,10 @@
         <v>88</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>237</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -4086,10 +4109,10 @@
         <v>88</v>
       </c>
       <c r="C27">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>206</v>
+        <v>101</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -4124,16 +4147,16 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -4148,7 +4171,7 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -4157,13 +4180,13 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -4174,10 +4197,10 @@
         <v>89</v>
       </c>
       <c r="C29">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -4212,10 +4235,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30">
         <v>42</v>
@@ -4256,16 +4279,16 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -4306,10 +4329,10 @@
         <v>91</v>
       </c>
       <c r="C32">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -4350,10 +4373,10 @@
         <v>91</v>
       </c>
       <c r="C33">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -4394,10 +4417,10 @@
         <v>91</v>
       </c>
       <c r="C34">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -4438,10 +4461,10 @@
         <v>91</v>
       </c>
       <c r="C35">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>348</v>
+        <v>120</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -4482,10 +4505,10 @@
         <v>91</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -4526,10 +4549,10 @@
         <v>91</v>
       </c>
       <c r="C37">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -4570,10 +4593,10 @@
         <v>91</v>
       </c>
       <c r="C38">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -4614,10 +4637,10 @@
         <v>91</v>
       </c>
       <c r="C39">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -4658,10 +4681,10 @@
         <v>91</v>
       </c>
       <c r="C40">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D40" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -4702,10 +4725,10 @@
         <v>91</v>
       </c>
       <c r="C41">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>350</v>
+        <v>116</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -4746,10 +4769,10 @@
         <v>91</v>
       </c>
       <c r="C42">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -4790,10 +4813,10 @@
         <v>91</v>
       </c>
       <c r="C43">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -4828,16 +4851,16 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -4878,10 +4901,10 @@
         <v>92</v>
       </c>
       <c r="C45">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>352</v>
+        <v>140</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -4922,10 +4945,10 @@
         <v>92</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -4966,10 +4989,10 @@
         <v>92</v>
       </c>
       <c r="C47">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -5010,10 +5033,10 @@
         <v>92</v>
       </c>
       <c r="C48">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -5054,10 +5077,10 @@
         <v>92</v>
       </c>
       <c r="C49">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D49" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -5092,10 +5115,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50">
         <v>42</v>
@@ -5113,7 +5136,7 @@
         <v>1</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50">
         <v>1</v>
@@ -5122,7 +5145,7 @@
         <v>1</v>
       </c>
       <c r="K50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L50">
         <v>0</v>
@@ -5142,10 +5165,10 @@
         <v>93</v>
       </c>
       <c r="C51">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D51" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -5163,7 +5186,7 @@
         <v>1</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -5186,10 +5209,10 @@
         <v>93</v>
       </c>
       <c r="C52">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -5224,16 +5247,16 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -5245,19 +5268,19 @@
         <v>1</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53">
         <v>1</v>
       </c>
       <c r="J53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M53">
         <v>0</v>
@@ -5268,10 +5291,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54">
         <v>42</v>
@@ -5298,10 +5321,10 @@
         <v>1</v>
       </c>
       <c r="K54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -5312,16 +5335,16 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C55">
         <v>42</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -5339,10 +5362,10 @@
         <v>1</v>
       </c>
       <c r="J55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55">
         <v>0</v>
@@ -5356,16 +5379,16 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D56" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -5386,7 +5409,7 @@
         <v>0</v>
       </c>
       <c r="K56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L56">
         <v>0</v>
@@ -5406,10 +5429,10 @@
         <v>182</v>
       </c>
       <c r="C57">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -5450,10 +5473,10 @@
         <v>182</v>
       </c>
       <c r="C58">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -5494,10 +5517,10 @@
         <v>182</v>
       </c>
       <c r="C59">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -5538,10 +5561,10 @@
         <v>182</v>
       </c>
       <c r="C60">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -5582,10 +5605,10 @@
         <v>182</v>
       </c>
       <c r="C61">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5626,10 +5649,10 @@
         <v>182</v>
       </c>
       <c r="C62">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -5670,10 +5693,10 @@
         <v>182</v>
       </c>
       <c r="C63">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -5714,10 +5737,10 @@
         <v>182</v>
       </c>
       <c r="C64">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -5758,10 +5781,10 @@
         <v>182</v>
       </c>
       <c r="C65">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D65" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -5796,16 +5819,16 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C66">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D66" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -5846,10 +5869,10 @@
         <v>183</v>
       </c>
       <c r="C67">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -5890,10 +5913,10 @@
         <v>183</v>
       </c>
       <c r="C68">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -5928,16 +5951,16 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C69">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -5978,10 +6001,10 @@
         <v>184</v>
       </c>
       <c r="C70">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -6022,10 +6045,10 @@
         <v>184</v>
       </c>
       <c r="C71">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -6046,7 +6069,7 @@
         <v>0</v>
       </c>
       <c r="K71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L71">
         <v>0</v>
@@ -6066,10 +6089,10 @@
         <v>184</v>
       </c>
       <c r="C72">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D72" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -6090,7 +6113,7 @@
         <v>0</v>
       </c>
       <c r="K72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72">
         <v>0</v>
@@ -6110,10 +6133,10 @@
         <v>184</v>
       </c>
       <c r="C73">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D73" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -6148,10 +6171,10 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C74">
         <v>42</v>
@@ -6172,7 +6195,7 @@
         <v>1</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -6192,16 +6215,16 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C75">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D75" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -6216,7 +6239,7 @@
         <v>1</v>
       </c>
       <c r="I75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -6242,10 +6265,10 @@
         <v>186</v>
       </c>
       <c r="C76">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D76" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -6280,16 +6303,16 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C77">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D77" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -6330,10 +6353,10 @@
         <v>187</v>
       </c>
       <c r="C78">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -6374,10 +6397,10 @@
         <v>187</v>
       </c>
       <c r="C79">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -6418,10 +6441,10 @@
         <v>187</v>
       </c>
       <c r="C80">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -6462,10 +6485,10 @@
         <v>187</v>
       </c>
       <c r="C81">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -6506,10 +6529,10 @@
         <v>187</v>
       </c>
       <c r="C82">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D82" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -6544,16 +6567,16 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C83">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D83" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -6574,10 +6597,10 @@
         <v>0</v>
       </c>
       <c r="K83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M83">
         <v>0</v>
@@ -6594,10 +6617,10 @@
         <v>188</v>
       </c>
       <c r="C84">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -6638,10 +6661,10 @@
         <v>188</v>
       </c>
       <c r="C85">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D85" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -6676,10 +6699,10 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B86" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C86">
         <v>42</v>
@@ -6720,16 +6743,16 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C87">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D87" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -6770,10 +6793,10 @@
         <v>189</v>
       </c>
       <c r="C88">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D88" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -6814,10 +6837,10 @@
         <v>189</v>
       </c>
       <c r="C89">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D89" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -6858,10 +6881,10 @@
         <v>189</v>
       </c>
       <c r="C90">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -6902,10 +6925,10 @@
         <v>189</v>
       </c>
       <c r="C91">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D91" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -6946,10 +6969,10 @@
         <v>189</v>
       </c>
       <c r="C92">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D92" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -6990,10 +7013,10 @@
         <v>189</v>
       </c>
       <c r="C93">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E93">
         <v>1</v>
@@ -7034,10 +7057,10 @@
         <v>189</v>
       </c>
       <c r="C94">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D94" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -7072,10 +7095,10 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B95" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C95">
         <v>42</v>
@@ -7093,7 +7116,7 @@
         <v>1</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95">
         <v>1</v>
@@ -7116,16 +7139,16 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B96" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C96">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D96" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -7137,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96">
         <v>1</v>
@@ -7166,10 +7189,10 @@
         <v>191</v>
       </c>
       <c r="C97">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -7210,10 +7233,10 @@
         <v>191</v>
       </c>
       <c r="C98">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D98" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -7254,10 +7277,10 @@
         <v>191</v>
       </c>
       <c r="C99">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D99" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -7298,10 +7321,10 @@
         <v>191</v>
       </c>
       <c r="C100">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D100" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -7336,16 +7359,16 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C101">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D101" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -7386,10 +7409,10 @@
         <v>192</v>
       </c>
       <c r="C102">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -7430,10 +7453,10 @@
         <v>192</v>
       </c>
       <c r="C103">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D103" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -7474,10 +7497,10 @@
         <v>192</v>
       </c>
       <c r="C104">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D104" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -7512,16 +7535,16 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B105" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C105">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D105" t="s">
-        <v>353</v>
+        <v>206</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -7562,10 +7585,10 @@
         <v>193</v>
       </c>
       <c r="C106">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D106" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -7606,10 +7629,10 @@
         <v>193</v>
       </c>
       <c r="C107">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D107" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -7650,10 +7673,10 @@
         <v>193</v>
       </c>
       <c r="C108">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D108" t="s">
-        <v>114</v>
+        <v>355</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -7694,10 +7717,10 @@
         <v>193</v>
       </c>
       <c r="C109">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D109" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -7738,10 +7761,10 @@
         <v>193</v>
       </c>
       <c r="C110">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D110" t="s">
-        <v>356</v>
+        <v>116</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -7782,10 +7805,10 @@
         <v>193</v>
       </c>
       <c r="C111">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D111" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -7826,10 +7849,10 @@
         <v>193</v>
       </c>
       <c r="C112">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D112" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -7870,10 +7893,10 @@
         <v>193</v>
       </c>
       <c r="C113">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D113" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -7914,10 +7937,10 @@
         <v>193</v>
       </c>
       <c r="C114">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D114" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -7958,10 +7981,10 @@
         <v>193</v>
       </c>
       <c r="C115">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D115" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -8002,10 +8025,10 @@
         <v>193</v>
       </c>
       <c r="C116">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D116" t="s">
-        <v>206</v>
+        <v>361</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -8040,16 +8063,16 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C117">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D117" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -8090,10 +8113,10 @@
         <v>181</v>
       </c>
       <c r="C118">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D118" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -8134,10 +8157,10 @@
         <v>181</v>
       </c>
       <c r="C119">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D119" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -8172,16 +8195,16 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C120">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D120" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -8202,10 +8225,10 @@
         <v>0</v>
       </c>
       <c r="K120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -8216,16 +8239,16 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>442</v>
+        <v>95</v>
       </c>
       <c r="C121">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="D121" t="s">
-        <v>172</v>
+        <v>220</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -8234,28 +8257,28 @@
         <v>1</v>
       </c>
       <c r="G121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H121">
         <v>1</v>
       </c>
       <c r="I121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
@@ -8266,10 +8289,10 @@
         <v>442</v>
       </c>
       <c r="C122">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="D122" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -8310,10 +8333,10 @@
         <v>442</v>
       </c>
       <c r="C123">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D123" t="s">
-        <v>449</v>
+        <v>86</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -8354,10 +8377,10 @@
         <v>442</v>
       </c>
       <c r="C124">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D124" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -8398,10 +8421,10 @@
         <v>442</v>
       </c>
       <c r="C125">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D125" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -8442,10 +8465,10 @@
         <v>442</v>
       </c>
       <c r="C126">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D126" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -8480,16 +8503,16 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B127" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C127">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="D127" t="s">
-        <v>172</v>
+        <v>452</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -8530,10 +8553,10 @@
         <v>443</v>
       </c>
       <c r="C128">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="D128" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -8574,10 +8597,10 @@
         <v>443</v>
       </c>
       <c r="C129">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D129" t="s">
-        <v>449</v>
+        <v>86</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -8618,10 +8641,10 @@
         <v>443</v>
       </c>
       <c r="C130">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D130" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -8662,10 +8685,10 @@
         <v>443</v>
       </c>
       <c r="C131">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D131" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -8706,10 +8729,10 @@
         <v>443</v>
       </c>
       <c r="C132">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D132" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -8744,16 +8767,16 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B133" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C133">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="D133" t="s">
-        <v>172</v>
+        <v>452</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -8794,10 +8817,10 @@
         <v>444</v>
       </c>
       <c r="C134">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="D134" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -8838,10 +8861,10 @@
         <v>444</v>
       </c>
       <c r="C135">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D135" t="s">
-        <v>449</v>
+        <v>86</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -8882,10 +8905,10 @@
         <v>444</v>
       </c>
       <c r="C136">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D136" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -8926,10 +8949,10 @@
         <v>444</v>
       </c>
       <c r="C137">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D137" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -8970,39 +8993,83 @@
         <v>444</v>
       </c>
       <c r="C138">
+        <v>95</v>
+      </c>
+      <c r="D138" t="s">
+        <v>451</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+      <c r="H138">
+        <v>1</v>
+      </c>
+      <c r="I138">
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>1</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>1</v>
+      </c>
+      <c r="M138">
+        <v>1</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>30</v>
+      </c>
+      <c r="B139" t="s">
+        <v>444</v>
+      </c>
+      <c r="C139">
         <v>96</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D139" t="s">
         <v>452</v>
       </c>
-      <c r="E138">
-        <v>1</v>
-      </c>
-      <c r="F138">
-        <v>1</v>
-      </c>
-      <c r="G138">
-        <v>0</v>
-      </c>
-      <c r="H138">
-        <v>1</v>
-      </c>
-      <c r="I138">
-        <v>0</v>
-      </c>
-      <c r="J138">
-        <v>1</v>
-      </c>
-      <c r="K138">
-        <v>0</v>
-      </c>
-      <c r="L138">
-        <v>1</v>
-      </c>
-      <c r="M138">
-        <v>1</v>
-      </c>
-      <c r="N138">
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>1</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139">
+        <v>1</v>
+      </c>
+      <c r="N139">
         <v>1</v>
       </c>
     </row>
@@ -14708,7 +14775,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -15596,6 +15663,14 @@
       </c>
       <c r="B110" t="s">
         <v>468</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>481</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@1/15/2015 4:02:18 PM] Internal Version 15. Additional updates for SCR 14031.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13894
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="550">
   <si>
     <t>SourceID</t>
   </si>
@@ -1673,6 +1673,12 @@
   </si>
   <si>
     <t>Changes for incorporating ETS Compliance Reports</t>
+  </si>
+  <si>
+    <t>Additional Changes for incorporating ETS Compliance Reports</t>
+  </si>
+  <si>
+    <t>Outstanding Action (Employee)</t>
   </si>
 </sst>
 </file>
@@ -2030,7 +2036,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2327,6 +2333,23 @@
       </c>
       <c r="E17" t="s">
         <v>547</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>42013</v>
+      </c>
+      <c r="C18" t="s">
+        <v>434</v>
+      </c>
+      <c r="D18">
+        <v>14031</v>
+      </c>
+      <c r="E18" t="s">
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -10576,7 +10599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A69" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16994,9 +17017,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0"/>
+    <sheetView topLeftCell="A86" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17970,6 +17993,22 @@
       </c>
       <c r="B121" t="s">
         <v>502</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@1/20/2015 12:30:26 PM] Internal version 16. Updated per SCR 14139.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13912
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="551">
   <si>
     <t>SourceID</t>
   </si>
@@ -1679,6 +1679,9 @@
   </si>
   <si>
     <t>Outstanding Action (Employee)</t>
+  </si>
+  <si>
+    <t>Updated to add WPPT* job codes to submit LSA ecls per scr 14139.</t>
   </si>
 </sst>
 </file>
@@ -2036,7 +2039,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2352,6 +2355,23 @@
         <v>548</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1">
+        <v>42024</v>
+      </c>
+      <c r="C19" t="s">
+        <v>434</v>
+      </c>
+      <c r="D19">
+        <v>14139</v>
+      </c>
+      <c r="E19" t="s">
+        <v>550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2362,7 +2382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2963,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2983,7 +3003,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -3003,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@2/5/2015 2:12:42 PM] Internal version 17. Updated per scr 14252.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13928
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="554">
   <si>
     <t>SourceID</t>
   </si>
@@ -1682,6 +1682,15 @@
   </si>
   <si>
     <t>Updated to add WPPT* job codes to submit LSA ecls per scr 14139.</t>
+  </si>
+  <si>
+    <t>Updated to add WISA12 job code to submit LSA ecls per scr 14252.</t>
+  </si>
+  <si>
+    <t>WISA12</t>
+  </si>
+  <si>
+    <t>Administrator, Systems</t>
   </si>
 </sst>
 </file>
@@ -2039,9 +2048,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2372,6 +2383,23 @@
         <v>550</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1">
+        <v>42040</v>
+      </c>
+      <c r="C20" t="s">
+        <v>434</v>
+      </c>
+      <c r="D20">
+        <v>14252</v>
+      </c>
+      <c r="E20" t="s">
+        <v>551</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2380,9 +2408,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3363,6 +3391,26 @@
         <v>0</v>
       </c>
       <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>552</v>
+      </c>
+      <c r="B50" t="s">
+        <v>553</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[VM:Susmitha.palacherla@3/31/2015 1:36:10 PM] Internal version 18. Updated per scr 14422.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13996
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -23,12 +23,16 @@
     <sheet name="Email_Notifications" sheetId="13" r:id="rId14"/>
     <sheet name="ETS_Description" sheetId="15" r:id="rId15"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DIM_Source!$A$1:$H$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Email_Notifications!$A$1:$K$115</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2056" uniqueCount="555">
   <si>
     <t>SourceID</t>
   </si>
@@ -1691,6 +1695,9 @@
   </si>
   <si>
     <t>Administrator, Systems</t>
+  </si>
+  <si>
+    <t>Updated DIM_Source to inactivate 'CMS Reported issue' for LSA and use 'CMS Reported Item' and in Email_notifications table updated subsource  'CMS Reported issue' to 'CMS Reported Item' for LSA module.</t>
   </si>
 </sst>
 </file>
@@ -2048,11 +2055,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2400,6 +2405,23 @@
         <v>551</v>
       </c>
     </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <v>42094</v>
+      </c>
+      <c r="C21" t="s">
+        <v>434</v>
+      </c>
+      <c r="D21">
+        <v>14422</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2410,7 +2432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10667,7 +10689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13355,7 +13377,7 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>492</v>
+        <v>170</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -13530,7 +13552,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>492</v>
+        <v>170</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -14896,7 +14918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15136,7 +15158,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -15644,7 +15666,7 @@
         <v>492</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -15656,7 +15678,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -15838,7 +15860,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -16346,7 +16368,7 @@
         <v>492</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -16358,7 +16380,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revision 23. Updates for SCR 15008 to add additional job codes for sup submission.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C32328
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2836" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="709">
   <si>
     <t>SourceID</t>
   </si>
@@ -2147,6 +2147,21 @@
   </si>
   <si>
     <t>Set supervisor =1 for 5 new AHT subcoaching reasons in Coaching_Reason_selection table.</t>
+  </si>
+  <si>
+    <t>Additional job codes for sup module submission</t>
+  </si>
+  <si>
+    <t>WISO12</t>
+  </si>
+  <si>
+    <t>Engineer, Software</t>
+  </si>
+  <si>
+    <t>WPOP11</t>
+  </si>
+  <si>
+    <t>Associate Analyst, Operations</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2939,6 +2954,23 @@
         <v>703</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>42163</v>
+      </c>
+      <c r="C26" t="s">
+        <v>434</v>
+      </c>
+      <c r="D26">
+        <v>15008</v>
+      </c>
+      <c r="E26" t="s">
+        <v>704</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2947,9 +2979,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3364,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3493,7 +3525,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -3916,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3939,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3962,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -4123,7 +4155,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -4146,7 +4178,53 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>705</v>
+      </c>
+      <c r="B53" t="s">
+        <v>706</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>707</v>
+      </c>
+      <c r="B54" t="s">
+        <v>708</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal revision 27. TFS 604.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C32836
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2879" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2884" uniqueCount="719">
   <si>
     <t>SourceID</t>
   </si>
@@ -2186,6 +2186,12 @@
   </si>
   <si>
     <t>A new eCoaching Log has been entered and requires your action. Please click on the link below to review and verify that the eCL entered on &lt;strong&gt;strDateTime&lt;/strong&gt; for &lt;strong&gt;strPerson&lt;/strong&gt; is a valid Customer Service Escalation (CSE). Further directions are provided on the form.</t>
+  </si>
+  <si>
+    <t>Added 1 new sub coach reason under AHT for CSR and SUP Modules in tables DIM_subCoaching_Reason and Coaching_Reason_selection.</t>
+  </si>
+  <si>
+    <t>Appropriate use of hold</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2549,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3044,6 +3050,23 @@
       </c>
       <c r="E29" t="s">
         <v>712</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>42248</v>
+      </c>
+      <c r="C30" t="s">
+        <v>434</v>
+      </c>
+      <c r="D30">
+        <v>604</v>
+      </c>
+      <c r="E30" t="s">
+        <v>717</v>
       </c>
     </row>
   </sheetData>
@@ -4377,9 +4400,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P292"/>
+  <dimension ref="A1:P293"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A251" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11888,25 +11911,25 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="C151">
-        <v>-1</v>
+        <v>230</v>
       </c>
       <c r="D151" t="s">
-        <v>4</v>
+        <v>718</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H151">
         <v>1</v>
@@ -11915,13 +11938,13 @@
         <v>1</v>
       </c>
       <c r="J151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K151">
         <v>0</v>
       </c>
       <c r="L151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M151">
         <v>0</v>
@@ -11938,25 +11961,25 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B152" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C152">
-        <v>42</v>
+        <v>-1</v>
       </c>
       <c r="D152" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H152">
         <v>1</v>
@@ -11965,13 +11988,13 @@
         <v>1</v>
       </c>
       <c r="J152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K152">
         <v>0</v>
       </c>
       <c r="L152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M152">
         <v>0</v>
@@ -11988,16 +12011,16 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B153" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C153">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D153" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -12021,7 +12044,7 @@
         <v>0</v>
       </c>
       <c r="L153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M153">
         <v>0</v>
@@ -12044,10 +12067,10 @@
         <v>85</v>
       </c>
       <c r="C154">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D154" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E154">
         <v>1</v>
@@ -12094,10 +12117,10 @@
         <v>85</v>
       </c>
       <c r="C155">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D155" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -12144,10 +12167,10 @@
         <v>85</v>
       </c>
       <c r="C156">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D156" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -12194,10 +12217,10 @@
         <v>85</v>
       </c>
       <c r="C157">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D157" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -12244,10 +12267,10 @@
         <v>85</v>
       </c>
       <c r="C158">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D158" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -12294,10 +12317,10 @@
         <v>85</v>
       </c>
       <c r="C159">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D159" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -12344,10 +12367,10 @@
         <v>85</v>
       </c>
       <c r="C160">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D160" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -12388,16 +12411,16 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B161" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C161">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D161" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -12406,7 +12429,7 @@
         <v>1</v>
       </c>
       <c r="G161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161">
         <v>1</v>
@@ -12444,10 +12467,10 @@
         <v>86</v>
       </c>
       <c r="C162">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D162" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -12456,7 +12479,7 @@
         <v>1</v>
       </c>
       <c r="G162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H162">
         <v>1</v>
@@ -12468,10 +12491,10 @@
         <v>1</v>
       </c>
       <c r="K162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M162">
         <v>0</v>
@@ -12480,24 +12503,24 @@
         <v>0</v>
       </c>
       <c r="O162">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B163" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="C163">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D163" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -12518,7 +12541,7 @@
         <v>1</v>
       </c>
       <c r="K163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L163">
         <v>1</v>
@@ -12530,10 +12553,10 @@
         <v>0</v>
       </c>
       <c r="O163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P163">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
@@ -12544,10 +12567,10 @@
         <v>181</v>
       </c>
       <c r="C164">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -12588,10 +12611,10 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="C165">
         <v>42</v>
@@ -12621,7 +12644,7 @@
         <v>0</v>
       </c>
       <c r="L165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M165">
         <v>0</v>
@@ -12638,16 +12661,16 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C166">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D166" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -12662,7 +12685,7 @@
         <v>1</v>
       </c>
       <c r="I166">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J166">
         <v>1</v>
@@ -12671,13 +12694,13 @@
         <v>0</v>
       </c>
       <c r="L166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N166">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O166">
         <v>0</v>
@@ -12694,10 +12717,10 @@
         <v>88</v>
       </c>
       <c r="C167">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D167" t="s">
-        <v>344</v>
+        <v>100</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -12744,10 +12767,10 @@
         <v>88</v>
       </c>
       <c r="C168">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D168" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -12771,7 +12794,7 @@
         <v>0</v>
       </c>
       <c r="L168">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M168">
         <v>1</v>
@@ -12794,10 +12817,10 @@
         <v>88</v>
       </c>
       <c r="C169">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D169" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -12821,7 +12844,7 @@
         <v>0</v>
       </c>
       <c r="L169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M169">
         <v>1</v>
@@ -12844,10 +12867,10 @@
         <v>88</v>
       </c>
       <c r="C170">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D170" t="s">
-        <v>103</v>
+        <v>346</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -12894,10 +12917,10 @@
         <v>88</v>
       </c>
       <c r="C171">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D171" t="s">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -12944,10 +12967,10 @@
         <v>88</v>
       </c>
       <c r="C172">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D172" t="s">
-        <v>105</v>
+        <v>347</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -12994,10 +13017,10 @@
         <v>88</v>
       </c>
       <c r="C173">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D173" t="s">
-        <v>236</v>
+        <v>105</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -13044,10 +13067,10 @@
         <v>88</v>
       </c>
       <c r="C174">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D174" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13094,10 +13117,10 @@
         <v>88</v>
       </c>
       <c r="C175">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D175" t="s">
-        <v>101</v>
+        <v>237</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13144,10 +13167,10 @@
         <v>88</v>
       </c>
       <c r="C176">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D176" t="s">
-        <v>206</v>
+        <v>101</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -13183,21 +13206,21 @@
         <v>0</v>
       </c>
       <c r="P176">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B177" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C177">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D177" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -13212,7 +13235,7 @@
         <v>1</v>
       </c>
       <c r="I177">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J177">
         <v>1</v>
@@ -13221,19 +13244,19 @@
         <v>0</v>
       </c>
       <c r="L177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N177">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O177">
         <v>0</v>
       </c>
       <c r="P177">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
@@ -13244,10 +13267,10 @@
         <v>89</v>
       </c>
       <c r="C178">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D178" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -13288,10 +13311,10 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B179" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C179">
         <v>42</v>
@@ -13338,16 +13361,16 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B180" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C180">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D180" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -13394,10 +13417,10 @@
         <v>91</v>
       </c>
       <c r="C181">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D181" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -13444,10 +13467,10 @@
         <v>91</v>
       </c>
       <c r="C182">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D182" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -13494,10 +13517,10 @@
         <v>91</v>
       </c>
       <c r="C183">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D183" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -13544,10 +13567,10 @@
         <v>91</v>
       </c>
       <c r="C184">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D184" t="s">
-        <v>348</v>
+        <v>120</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -13594,10 +13617,10 @@
         <v>91</v>
       </c>
       <c r="C185">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D185" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -13644,10 +13667,10 @@
         <v>91</v>
       </c>
       <c r="C186">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D186" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -13694,10 +13717,10 @@
         <v>91</v>
       </c>
       <c r="C187">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D187" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -13744,10 +13767,10 @@
         <v>91</v>
       </c>
       <c r="C188">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D188" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -13794,10 +13817,10 @@
         <v>91</v>
       </c>
       <c r="C189">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D189" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -13844,10 +13867,10 @@
         <v>91</v>
       </c>
       <c r="C190">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D190" t="s">
-        <v>350</v>
+        <v>116</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -13894,10 +13917,10 @@
         <v>91</v>
       </c>
       <c r="C191">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D191" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -13944,10 +13967,10 @@
         <v>91</v>
       </c>
       <c r="C192">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D192" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -13988,16 +14011,16 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C193">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D193" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -14044,10 +14067,10 @@
         <v>92</v>
       </c>
       <c r="C194">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D194" t="s">
-        <v>352</v>
+        <v>140</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -14094,10 +14117,10 @@
         <v>92</v>
       </c>
       <c r="C195">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D195" t="s">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -14144,10 +14167,10 @@
         <v>92</v>
       </c>
       <c r="C196">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D196" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -14194,10 +14217,10 @@
         <v>92</v>
       </c>
       <c r="C197">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D197" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -14244,10 +14267,10 @@
         <v>92</v>
       </c>
       <c r="C198">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D198" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -14280,7 +14303,7 @@
         <v>0</v>
       </c>
       <c r="O198">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P198">
         <v>0</v>
@@ -14288,10 +14311,10 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B199" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C199">
         <v>42</v>
@@ -14309,7 +14332,7 @@
         <v>1</v>
       </c>
       <c r="H199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I199">
         <v>1</v>
@@ -14318,7 +14341,7 @@
         <v>1</v>
       </c>
       <c r="K199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L199">
         <v>0</v>
@@ -14333,7 +14356,7 @@
         <v>1</v>
       </c>
       <c r="P199">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
@@ -14344,10 +14367,10 @@
         <v>93</v>
       </c>
       <c r="C200">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D200" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -14365,7 +14388,7 @@
         <v>1</v>
       </c>
       <c r="J200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K200">
         <v>1</v>
@@ -14383,7 +14406,7 @@
         <v>1</v>
       </c>
       <c r="P200">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
@@ -14394,10 +14417,10 @@
         <v>93</v>
       </c>
       <c r="C201">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D201" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -14430,7 +14453,7 @@
         <v>0</v>
       </c>
       <c r="O201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P201">
         <v>0</v>
@@ -14438,16 +14461,16 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B202" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C202">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D202" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -14459,19 +14482,19 @@
         <v>1</v>
       </c>
       <c r="H202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I202">
         <v>1</v>
       </c>
       <c r="J202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K202">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M202">
         <v>0</v>
@@ -14488,10 +14511,10 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B203" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C203">
         <v>42</v>
@@ -14518,10 +14541,10 @@
         <v>1</v>
       </c>
       <c r="K203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M203">
         <v>0</v>
@@ -14530,24 +14553,24 @@
         <v>0</v>
       </c>
       <c r="O203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P203">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B204" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C204">
         <v>42</v>
       </c>
       <c r="D204" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="E204">
         <v>1</v>
@@ -14565,10 +14588,10 @@
         <v>1</v>
       </c>
       <c r="J204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L204">
         <v>0</v>
@@ -14580,24 +14603,24 @@
         <v>0</v>
       </c>
       <c r="O204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P204">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B205" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C205">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D205" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="E205">
         <v>1</v>
@@ -14618,7 +14641,7 @@
         <v>0</v>
       </c>
       <c r="K205">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L205">
         <v>0</v>
@@ -14644,10 +14667,10 @@
         <v>182</v>
       </c>
       <c r="C206">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D206" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E206">
         <v>1</v>
@@ -14694,10 +14717,10 @@
         <v>182</v>
       </c>
       <c r="C207">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D207" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E207">
         <v>1</v>
@@ -14744,10 +14767,10 @@
         <v>182</v>
       </c>
       <c r="C208">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D208" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -14794,10 +14817,10 @@
         <v>182</v>
       </c>
       <c r="C209">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D209" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -14844,10 +14867,10 @@
         <v>182</v>
       </c>
       <c r="C210">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D210" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E210">
         <v>1</v>
@@ -14894,10 +14917,10 @@
         <v>182</v>
       </c>
       <c r="C211">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D211" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E211">
         <v>1</v>
@@ -14944,10 +14967,10 @@
         <v>182</v>
       </c>
       <c r="C212">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D212" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -14994,10 +15017,10 @@
         <v>182</v>
       </c>
       <c r="C213">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D213" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E213">
         <v>1</v>
@@ -15044,10 +15067,10 @@
         <v>182</v>
       </c>
       <c r="C214">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D214" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -15088,16 +15111,16 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B215" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C215">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D215" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E215">
         <v>1</v>
@@ -15144,10 +15167,10 @@
         <v>183</v>
       </c>
       <c r="C216">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D216" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -15194,10 +15217,10 @@
         <v>183</v>
       </c>
       <c r="C217">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D217" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E217">
         <v>1</v>
@@ -15238,16 +15261,16 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B218" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C218">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D218" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -15280,7 +15303,7 @@
         <v>0</v>
       </c>
       <c r="O218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P218">
         <v>0</v>
@@ -15294,10 +15317,10 @@
         <v>184</v>
       </c>
       <c r="C219">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D219" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E219">
         <v>1</v>
@@ -15330,7 +15353,7 @@
         <v>0</v>
       </c>
       <c r="O219">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P219">
         <v>0</v>
@@ -15344,10 +15367,10 @@
         <v>184</v>
       </c>
       <c r="C220">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D220" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -15368,7 +15391,7 @@
         <v>0</v>
       </c>
       <c r="K220">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L220">
         <v>0</v>
@@ -15394,10 +15417,10 @@
         <v>184</v>
       </c>
       <c r="C221">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D221" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -15418,7 +15441,7 @@
         <v>0</v>
       </c>
       <c r="K221">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L221">
         <v>0</v>
@@ -15444,10 +15467,10 @@
         <v>184</v>
       </c>
       <c r="C222">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D222" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -15480,7 +15503,7 @@
         <v>0</v>
       </c>
       <c r="O222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P222">
         <v>0</v>
@@ -15488,10 +15511,10 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B223" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C223">
         <v>42</v>
@@ -15512,7 +15535,7 @@
         <v>1</v>
       </c>
       <c r="I223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J223">
         <v>0</v>
@@ -15530,7 +15553,7 @@
         <v>0</v>
       </c>
       <c r="O223">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P223">
         <v>0</v>
@@ -15538,16 +15561,16 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B224" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C224">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D224" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -15562,7 +15585,7 @@
         <v>1</v>
       </c>
       <c r="I224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J224">
         <v>0</v>
@@ -15580,7 +15603,7 @@
         <v>0</v>
       </c>
       <c r="O224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P224">
         <v>0</v>
@@ -15594,10 +15617,10 @@
         <v>186</v>
       </c>
       <c r="C225">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D225" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -15638,16 +15661,16 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B226" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C226">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D226" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -15680,7 +15703,7 @@
         <v>0</v>
       </c>
       <c r="O226">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P226">
         <v>0</v>
@@ -15694,10 +15717,10 @@
         <v>187</v>
       </c>
       <c r="C227">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D227" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -15744,10 +15767,10 @@
         <v>187</v>
       </c>
       <c r="C228">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D228" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -15794,10 +15817,10 @@
         <v>187</v>
       </c>
       <c r="C229">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D229" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -15844,10 +15867,10 @@
         <v>187</v>
       </c>
       <c r="C230">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D230" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -15894,10 +15917,10 @@
         <v>187</v>
       </c>
       <c r="C231">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D231" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -15930,7 +15953,7 @@
         <v>0</v>
       </c>
       <c r="O231">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P231">
         <v>0</v>
@@ -15938,16 +15961,16 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B232" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C232">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D232" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -15968,10 +15991,10 @@
         <v>0</v>
       </c>
       <c r="K232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L232">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M232">
         <v>0</v>
@@ -15980,7 +16003,7 @@
         <v>0</v>
       </c>
       <c r="O232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P232">
         <v>0</v>
@@ -15994,10 +16017,10 @@
         <v>188</v>
       </c>
       <c r="C233">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D233" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -16044,10 +16067,10 @@
         <v>188</v>
       </c>
       <c r="C234">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D234" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -16088,10 +16111,10 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B235" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C235">
         <v>42</v>
@@ -16133,21 +16156,21 @@
         <v>0</v>
       </c>
       <c r="P235">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B236" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C236">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D236" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -16183,7 +16206,7 @@
         <v>0</v>
       </c>
       <c r="P236">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
@@ -16194,10 +16217,10 @@
         <v>189</v>
       </c>
       <c r="C237">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D237" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -16244,10 +16267,10 @@
         <v>189</v>
       </c>
       <c r="C238">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D238" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -16294,10 +16317,10 @@
         <v>189</v>
       </c>
       <c r="C239">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D239" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -16344,10 +16367,10 @@
         <v>189</v>
       </c>
       <c r="C240">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D240" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -16394,10 +16417,10 @@
         <v>189</v>
       </c>
       <c r="C241">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D241" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -16444,10 +16467,10 @@
         <v>189</v>
       </c>
       <c r="C242">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D242" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -16494,10 +16517,10 @@
         <v>189</v>
       </c>
       <c r="C243">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D243" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -16538,10 +16561,10 @@
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B244" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C244">
         <v>42</v>
@@ -16559,7 +16582,7 @@
         <v>1</v>
       </c>
       <c r="H244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I244">
         <v>1</v>
@@ -16588,16 +16611,16 @@
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B245" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C245">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D245" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -16609,7 +16632,7 @@
         <v>1</v>
       </c>
       <c r="H245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I245">
         <v>1</v>
@@ -16644,10 +16667,10 @@
         <v>191</v>
       </c>
       <c r="C246">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D246" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -16694,10 +16717,10 @@
         <v>191</v>
       </c>
       <c r="C247">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D247" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -16744,10 +16767,10 @@
         <v>191</v>
       </c>
       <c r="C248">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D248" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -16794,10 +16817,10 @@
         <v>191</v>
       </c>
       <c r="C249">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D249" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -16838,16 +16861,16 @@
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B250" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C250">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D250" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -16894,10 +16917,10 @@
         <v>192</v>
       </c>
       <c r="C251">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D251" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -16944,10 +16967,10 @@
         <v>192</v>
       </c>
       <c r="C252">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D252" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -16994,10 +17017,10 @@
         <v>192</v>
       </c>
       <c r="C253">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D253" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -17038,16 +17061,16 @@
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B254" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C254">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D254" t="s">
-        <v>353</v>
+        <v>206</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -17094,10 +17117,10 @@
         <v>193</v>
       </c>
       <c r="C255">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D255" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -17144,10 +17167,10 @@
         <v>193</v>
       </c>
       <c r="C256">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D256" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -17194,10 +17217,10 @@
         <v>193</v>
       </c>
       <c r="C257">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D257" t="s">
-        <v>114</v>
+        <v>355</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -17244,10 +17267,10 @@
         <v>193</v>
       </c>
       <c r="C258">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D258" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -17294,10 +17317,10 @@
         <v>193</v>
       </c>
       <c r="C259">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D259" t="s">
-        <v>356</v>
+        <v>116</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -17344,10 +17367,10 @@
         <v>193</v>
       </c>
       <c r="C260">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D260" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E260">
         <v>1</v>
@@ -17394,10 +17417,10 @@
         <v>193</v>
       </c>
       <c r="C261">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D261" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E261">
         <v>1</v>
@@ -17444,10 +17467,10 @@
         <v>193</v>
       </c>
       <c r="C262">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D262" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E262">
         <v>1</v>
@@ -17494,10 +17517,10 @@
         <v>193</v>
       </c>
       <c r="C263">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D263" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -17544,10 +17567,10 @@
         <v>193</v>
       </c>
       <c r="C264">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D264" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E264">
         <v>1</v>
@@ -17594,10 +17617,10 @@
         <v>193</v>
       </c>
       <c r="C265">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D265" t="s">
-        <v>206</v>
+        <v>361</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -17638,16 +17661,16 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B266" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C266">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D266" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -17694,10 +17717,10 @@
         <v>181</v>
       </c>
       <c r="C267">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D267" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -17744,10 +17767,10 @@
         <v>181</v>
       </c>
       <c r="C268">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D268" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -17788,16 +17811,16 @@
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B269" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C269">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D269" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -17818,10 +17841,10 @@
         <v>0</v>
       </c>
       <c r="K269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L269">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M269">
         <v>0</v>
@@ -17830,7 +17853,7 @@
         <v>0</v>
       </c>
       <c r="O269">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P269">
         <v>0</v>
@@ -17838,16 +17861,16 @@
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B270" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C270">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="D270" t="s">
-        <v>645</v>
+        <v>220</v>
       </c>
       <c r="E270">
         <v>1</v>
@@ -17868,7 +17891,7 @@
         <v>0</v>
       </c>
       <c r="K270">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L270">
         <v>0</v>
@@ -17880,10 +17903,10 @@
         <v>0</v>
       </c>
       <c r="O270">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P270">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.25">
@@ -17894,10 +17917,10 @@
         <v>172</v>
       </c>
       <c r="C271">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D271" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -17944,10 +17967,10 @@
         <v>172</v>
       </c>
       <c r="C272">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D272" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -17988,16 +18011,16 @@
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B273" t="s">
-        <v>574</v>
+        <v>172</v>
       </c>
       <c r="C273">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="D273" t="s">
-        <v>649</v>
+        <v>689</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -18044,10 +18067,10 @@
         <v>574</v>
       </c>
       <c r="C274">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D274" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E274">
         <v>1</v>
@@ -18094,10 +18117,10 @@
         <v>574</v>
       </c>
       <c r="C275">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D275" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -18144,10 +18167,10 @@
         <v>574</v>
       </c>
       <c r="C276">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D276" t="s">
-        <v>206</v>
+        <v>651</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -18188,16 +18211,16 @@
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B277" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C277">
-        <v>182</v>
+        <v>42</v>
       </c>
       <c r="D277" t="s">
-        <v>643</v>
+        <v>206</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -18244,10 +18267,10 @@
         <v>575</v>
       </c>
       <c r="C278">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D278" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -18294,10 +18317,10 @@
         <v>575</v>
       </c>
       <c r="C279">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D279" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -18344,10 +18367,10 @@
         <v>575</v>
       </c>
       <c r="C280">
-        <v>42</v>
+        <v>213</v>
       </c>
       <c r="D280" t="s">
-        <v>206</v>
+        <v>674</v>
       </c>
       <c r="E280">
         <v>1</v>
@@ -18388,16 +18411,16 @@
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281">
+        <v>41</v>
+      </c>
+      <c r="B281" t="s">
+        <v>575</v>
+      </c>
+      <c r="C281">
         <v>42</v>
       </c>
-      <c r="B281" t="s">
-        <v>576</v>
-      </c>
-      <c r="C281">
-        <v>156</v>
-      </c>
       <c r="D281" t="s">
-        <v>617</v>
+        <v>206</v>
       </c>
       <c r="E281">
         <v>1</v>
@@ -18444,10 +18467,10 @@
         <v>576</v>
       </c>
       <c r="C282">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D282" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -18494,10 +18517,10 @@
         <v>576</v>
       </c>
       <c r="C283">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D283" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -18544,10 +18567,10 @@
         <v>576</v>
       </c>
       <c r="C284">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="D284" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
       <c r="E284">
         <v>1</v>
@@ -18594,10 +18617,10 @@
         <v>576</v>
       </c>
       <c r="C285">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D285" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="E285">
         <v>1</v>
@@ -18644,10 +18667,10 @@
         <v>576</v>
       </c>
       <c r="C286">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D286" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="E286">
         <v>1</v>
@@ -18694,10 +18717,10 @@
         <v>576</v>
       </c>
       <c r="C287">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="D287" t="s">
-        <v>206</v>
+        <v>690</v>
       </c>
       <c r="E287">
         <v>1</v>
@@ -18738,16 +18761,16 @@
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B288" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C288">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="D288" t="s">
-        <v>611</v>
+        <v>206</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -18794,10 +18817,10 @@
         <v>577</v>
       </c>
       <c r="C289">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="D289" t="s">
-        <v>206</v>
+        <v>611</v>
       </c>
       <c r="E289">
         <v>1</v>
@@ -18838,16 +18861,16 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B290" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C290">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="D290" t="s">
-        <v>590</v>
+        <v>206</v>
       </c>
       <c r="E290">
         <v>1</v>
@@ -18894,10 +18917,10 @@
         <v>578</v>
       </c>
       <c r="C291">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D291" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="E291">
         <v>1</v>
@@ -18944,45 +18967,95 @@
         <v>578</v>
       </c>
       <c r="C292">
+        <v>152</v>
+      </c>
+      <c r="D292" t="s">
+        <v>613</v>
+      </c>
+      <c r="E292">
+        <v>1</v>
+      </c>
+      <c r="F292">
+        <v>1</v>
+      </c>
+      <c r="G292">
+        <v>1</v>
+      </c>
+      <c r="H292">
+        <v>1</v>
+      </c>
+      <c r="I292">
+        <v>1</v>
+      </c>
+      <c r="J292">
+        <v>0</v>
+      </c>
+      <c r="K292">
+        <v>0</v>
+      </c>
+      <c r="L292">
+        <v>0</v>
+      </c>
+      <c r="M292">
+        <v>0</v>
+      </c>
+      <c r="N292">
+        <v>0</v>
+      </c>
+      <c r="O292">
+        <v>0</v>
+      </c>
+      <c r="P292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>44</v>
+      </c>
+      <c r="B293" t="s">
+        <v>578</v>
+      </c>
+      <c r="C293">
         <v>154</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D293" t="s">
         <v>615</v>
       </c>
-      <c r="E292">
-        <v>1</v>
-      </c>
-      <c r="F292">
-        <v>1</v>
-      </c>
-      <c r="G292">
-        <v>1</v>
-      </c>
-      <c r="H292">
-        <v>1</v>
-      </c>
-      <c r="I292">
-        <v>1</v>
-      </c>
-      <c r="J292">
-        <v>0</v>
-      </c>
-      <c r="K292">
-        <v>0</v>
-      </c>
-      <c r="L292">
-        <v>0</v>
-      </c>
-      <c r="M292">
-        <v>0</v>
-      </c>
-      <c r="N292">
-        <v>0</v>
-      </c>
-      <c r="O292">
-        <v>0</v>
-      </c>
-      <c r="P292">
+      <c r="E293">
+        <v>1</v>
+      </c>
+      <c r="F293">
+        <v>1</v>
+      </c>
+      <c r="G293">
+        <v>1</v>
+      </c>
+      <c r="H293">
+        <v>1</v>
+      </c>
+      <c r="I293">
+        <v>1</v>
+      </c>
+      <c r="J293">
+        <v>0</v>
+      </c>
+      <c r="K293">
+        <v>0</v>
+      </c>
+      <c r="L293">
+        <v>0</v>
+      </c>
+      <c r="M293">
+        <v>0</v>
+      </c>
+      <c r="N293">
+        <v>0</v>
+      </c>
+      <c r="O293">
+        <v>0</v>
+      </c>
+      <c r="P293">
         <v>1</v>
       </c>
     </row>
@@ -27488,9 +27561,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B231"/>
+  <dimension ref="A1:B232"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0"/>
+    <sheetView topLeftCell="A190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29344,6 +29417,14 @@
       </c>
       <c r="B231" t="s">
         <v>690</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>230</v>
+      </c>
+      <c r="B232" t="s">
+        <v>718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 28. TFS 667.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C32844
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2884" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="722">
   <si>
     <t>SourceID</t>
   </si>
@@ -2192,6 +2192,15 @@
   </si>
   <si>
     <t>Appropriate use of hold</t>
+  </si>
+  <si>
+    <t>Allow submission of all modules to job code WPOP70</t>
+  </si>
+  <si>
+    <t>WPOP70</t>
+  </si>
+  <si>
+    <t>Director, Operations</t>
   </si>
 </sst>
 </file>
@@ -2549,7 +2558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3069,6 +3078,23 @@
         <v>717</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1">
+        <v>42249</v>
+      </c>
+      <c r="C31" t="s">
+        <v>434</v>
+      </c>
+      <c r="D31">
+        <v>667</v>
+      </c>
+      <c r="E31" t="s">
+        <v>719</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3077,9 +3103,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3494,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4046,7 +4072,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4069,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -4092,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -4253,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -4276,7 +4302,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -4323,6 +4349,29 @@
       </c>
       <c r="G54">
         <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>720</v>
+      </c>
+      <c r="B55" t="s">
+        <v>721</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 29. Updates for TFS 549 and 644.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33172
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -23,6 +23,10 @@
     <sheet name="Email_Notifications" sheetId="13" r:id="rId14"/>
     <sheet name="ETS_Description" sheetId="15" r:id="rId15"/>
     <sheet name="DIM_Behavior" sheetId="16" r:id="rId16"/>
+    <sheet name="Survey_DIM_Type" sheetId="17" r:id="rId17"/>
+    <sheet name="Sirvey_DIM_Question" sheetId="18" r:id="rId18"/>
+    <sheet name="Survey_DIM_Response" sheetId="19" r:id="rId19"/>
+    <sheet name="Survey_DIM_QAnswer" sheetId="20" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="758">
   <si>
     <t>SourceID</t>
   </si>
@@ -2201,12 +2205,123 @@
   </si>
   <si>
     <t>Director, Operations</t>
+  </si>
+  <si>
+    <t>SurveyTypeID</t>
+  </si>
+  <si>
+    <t>Decsription</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>LastUpdateDate</t>
+  </si>
+  <si>
+    <t>Employee Survey</t>
+  </si>
+  <si>
+    <t>QuestionID</t>
+  </si>
+  <si>
+    <t>ResponseID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>1 - Very Ineffective</t>
+  </si>
+  <si>
+    <t>2 - Ineffective</t>
+  </si>
+  <si>
+    <t>3 - Neither</t>
+  </si>
+  <si>
+    <t>4 - Effective</t>
+  </si>
+  <si>
+    <t>5 - Very Effective</t>
+  </si>
+  <si>
+    <t>1 - Very Dissatisfied</t>
+  </si>
+  <si>
+    <t>2 - Dissatisfied</t>
+  </si>
+  <si>
+    <t>4 - Satisfied</t>
+  </si>
+  <si>
+    <t>5 - Very Satisfied</t>
+  </si>
+  <si>
+    <t>QuestionNumber</t>
+  </si>
+  <si>
+    <t>ResponseValue</t>
+  </si>
+  <si>
+    <t>ResponseType</t>
+  </si>
+  <si>
+    <t>isHotTopic</t>
+  </si>
+  <si>
+    <t>Radio Button</t>
+  </si>
+  <si>
+    <t>CSR Survey. Added 4 new Tabs for CSR Survey DIM tables.</t>
+  </si>
+  <si>
+    <t>ARC Escalations OMR feeds.Updated SubCoachingReason tab to add new record and set CSR to 0 in Coaching_Reason_selection table for IAE.</t>
+  </si>
+  <si>
+    <t>OMR: Inappropriate ARC Transfer</t>
+  </si>
+  <si>
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>Was the call played back for you during your last coaching session? (If applicable). |     If no, what reason was provided?</t>
+  </si>
+  <si>
+    <t>Will you be able to apply the information from your last coaching session? |    If yes, how?  If no, why  not?</t>
+  </si>
+  <si>
+    <t>Please rate the effectiveness of the coaching notes provided in the eCL. |   Please explain below.</t>
+  </si>
+  <si>
+    <t>Please rate your overall coaching experience. |   Please explain below.</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Did you find the coaching session valuable/effective? |   If yes, what specifically.  If no, why not?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss:mss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2250,13 +2365,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2558,9 +2674,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2908,7 +3026,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -3093,6 +3211,40 @@
       </c>
       <c r="E31" t="s">
         <v>719</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>42261</v>
+      </c>
+      <c r="C32" t="s">
+        <v>434</v>
+      </c>
+      <c r="D32">
+        <v>549</v>
+      </c>
+      <c r="E32" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>29.1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>42268</v>
+      </c>
+      <c r="C33" t="s">
+        <v>434</v>
+      </c>
+      <c r="D33">
+        <v>644</v>
+      </c>
+      <c r="E33" t="s">
+        <v>749</v>
       </c>
     </row>
   </sheetData>
@@ -13887,7 +14039,7 @@
         <v>1</v>
       </c>
       <c r="J189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K189">
         <v>0</v>
@@ -24880,6 +25032,513 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="23.28515625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B1" t="s">
+        <v>723</v>
+      </c>
+      <c r="C1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D1" t="s">
+        <v>725</v>
+      </c>
+      <c r="E1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" t="s">
+        <v>481</v>
+      </c>
+      <c r="J1" t="s">
+        <v>561</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>727</v>
+      </c>
+      <c r="C2">
+        <v>20150901</v>
+      </c>
+      <c r="D2">
+        <v>99991231</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>728</v>
+      </c>
+      <c r="B1" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D1" t="s">
+        <v>724</v>
+      </c>
+      <c r="E1" t="s">
+        <v>725</v>
+      </c>
+      <c r="F1" t="s">
+        <v>746</v>
+      </c>
+      <c r="G1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>20150901</v>
+      </c>
+      <c r="E2">
+        <v>99991231</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>752</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>20150901</v>
+      </c>
+      <c r="E3">
+        <v>99991231</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>753</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>20150901</v>
+      </c>
+      <c r="E4">
+        <v>99991231</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>757</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>20150901</v>
+      </c>
+      <c r="E5">
+        <v>99991231</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>754</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>20150901</v>
+      </c>
+      <c r="E6">
+        <v>99991231</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>20150901</v>
+      </c>
+      <c r="E7">
+        <v>99991231</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>729</v>
+      </c>
+      <c r="B1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>756</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>731</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>732</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>733</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>734</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>735</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>736</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>737</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>738</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>739</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>740</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>741</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>742</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
@@ -26722,6 +27381,653 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="24" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>722</v>
+      </c>
+      <c r="B1" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D1" t="s">
+        <v>729</v>
+      </c>
+      <c r="E1" t="s">
+        <v>744</v>
+      </c>
+      <c r="F1" t="s">
+        <v>745</v>
+      </c>
+      <c r="G1" t="s">
+        <v>746</v>
+      </c>
+      <c r="H1" t="s">
+        <v>724</v>
+      </c>
+      <c r="I1" t="s">
+        <v>725</v>
+      </c>
+      <c r="J1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>731</v>
+      </c>
+      <c r="F2" t="s">
+        <v>747</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>20150901</v>
+      </c>
+      <c r="I2">
+        <v>99991231</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>732</v>
+      </c>
+      <c r="F3" t="s">
+        <v>747</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>20150901</v>
+      </c>
+      <c r="I3">
+        <v>99991231</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>733</v>
+      </c>
+      <c r="F4" t="s">
+        <v>747</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>20150901</v>
+      </c>
+      <c r="I4">
+        <v>99991231</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>731</v>
+      </c>
+      <c r="F5" t="s">
+        <v>747</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>20150901</v>
+      </c>
+      <c r="I5">
+        <v>99991231</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>732</v>
+      </c>
+      <c r="F6" t="s">
+        <v>747</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>20150901</v>
+      </c>
+      <c r="I6">
+        <v>99991231</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>731</v>
+      </c>
+      <c r="F7" t="s">
+        <v>747</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>20150901</v>
+      </c>
+      <c r="I7">
+        <v>99991231</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>732</v>
+      </c>
+      <c r="F8" t="s">
+        <v>747</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>20150901</v>
+      </c>
+      <c r="I8">
+        <v>99991231</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>734</v>
+      </c>
+      <c r="F9" t="s">
+        <v>747</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>20150901</v>
+      </c>
+      <c r="I9">
+        <v>99991231</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>735</v>
+      </c>
+      <c r="F10" t="s">
+        <v>747</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>20150901</v>
+      </c>
+      <c r="I10">
+        <v>99991231</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>736</v>
+      </c>
+      <c r="F11" t="s">
+        <v>747</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>20150901</v>
+      </c>
+      <c r="I11">
+        <v>99991231</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>737</v>
+      </c>
+      <c r="F12" t="s">
+        <v>747</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>20150901</v>
+      </c>
+      <c r="I12">
+        <v>99991231</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>738</v>
+      </c>
+      <c r="F13" t="s">
+        <v>747</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>20150901</v>
+      </c>
+      <c r="I13">
+        <v>99991231</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>739</v>
+      </c>
+      <c r="F14" t="s">
+        <v>747</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>20150901</v>
+      </c>
+      <c r="I14">
+        <v>99991231</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>740</v>
+      </c>
+      <c r="F15" t="s">
+        <v>747</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>20150901</v>
+      </c>
+      <c r="I15">
+        <v>99991231</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>736</v>
+      </c>
+      <c r="F16" t="s">
+        <v>747</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>20150901</v>
+      </c>
+      <c r="I16">
+        <v>99991231</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>741</v>
+      </c>
+      <c r="F17" t="s">
+        <v>747</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>20150901</v>
+      </c>
+      <c r="I17">
+        <v>99991231</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>742</v>
+      </c>
+      <c r="F18" t="s">
+        <v>747</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>20150901</v>
+      </c>
+      <c r="I18">
+        <v>99991231</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4">
+        <v>42248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27610,9 +28916,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B232"/>
+  <dimension ref="A1:B233"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0"/>
+    <sheetView topLeftCell="A191" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29474,6 +30780,14 @@
       </c>
       <c r="B232" t="s">
         <v>718</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>231</v>
+      </c>
+      <c r="B233" t="s">
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 30. TFS 841.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33228
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840" firstSheet="14" activeTab="19"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="759">
   <si>
     <t>SourceID</t>
   </si>
@@ -2313,6 +2313,9 @@
   </si>
   <si>
     <t>Did you find the coaching session valuable/effective? |   If yes, what specifically.  If no, why not?</t>
+  </si>
+  <si>
+    <t>Enable sup modukle submissions for job code WACQ13. Updated Module_submission tab.</t>
   </si>
 </sst>
 </file>
@@ -2674,11 +2677,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3247,6 +3248,23 @@
         <v>749</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>42283</v>
+      </c>
+      <c r="C34" t="s">
+        <v>434</v>
+      </c>
+      <c r="D34">
+        <v>841</v>
+      </c>
+      <c r="E34" t="s">
+        <v>758</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3257,7 +3275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3364,7 +3382,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3649,7 +3667,7 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3672,7 +3690,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -4178,7 +4196,7 @@
         <v>1</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -4224,7 +4242,7 @@
         <v>0</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -4247,7 +4265,7 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -4270,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -4431,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -4454,7 +4472,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -27388,7 +27406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Internal Version 31. TFS 861.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33364
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="760">
   <si>
     <t>SourceID</t>
   </si>
@@ -2315,7 +2315,10 @@
     <t>Did you find the coaching session valuable/effective? |   If yes, what specifically.  If no, why not?</t>
   </si>
   <si>
-    <t>Enable sup modukle submissions for job code WACQ13. Updated Module_submission tab.</t>
+    <t>Enable sup module submissions for job code WACQ13. Updated Module_submission tab.</t>
+  </si>
+  <si>
+    <t>Open Warnings for all Modules (LSA, Training and Quality Modules)Updated Coaching_Reason_Selection and Email_Notification tabs</t>
   </si>
 </sst>
 </file>
@@ -2677,7 +2680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3263,6 +3266,23 @@
       </c>
       <c r="E34" t="s">
         <v>758</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>42298</v>
+      </c>
+      <c r="C35" t="s">
+        <v>434</v>
+      </c>
+      <c r="D35">
+        <v>861</v>
+      </c>
+      <c r="E35" t="s">
+        <v>759</v>
       </c>
     </row>
   </sheetData>
@@ -4621,7 +4641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P293"/>
   <sheetViews>
-    <sheetView topLeftCell="A251" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4710,7 +4730,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -4722,10 +4742,10 @@
         <v>1</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -4760,7 +4780,7 @@
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -4772,10 +4792,10 @@
         <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4810,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -4822,10 +4842,10 @@
         <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4860,7 +4880,7 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -4872,10 +4892,10 @@
         <v>1</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4910,7 +4930,7 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -4922,10 +4942,10 @@
         <v>1</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4960,7 +4980,7 @@
         <v>1</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -4972,10 +4992,10 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -5010,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -5022,10 +5042,10 @@
         <v>1</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -5060,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -5072,10 +5092,10 @@
         <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5110,7 +5130,7 @@
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -5122,10 +5142,10 @@
         <v>1</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -5160,7 +5180,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -5172,10 +5192,10 @@
         <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5210,7 +5230,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -5222,10 +5242,10 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -5260,7 +5280,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -5272,10 +5292,10 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5310,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -5322,10 +5342,10 @@
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -5360,7 +5380,7 @@
         <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -5372,10 +5392,10 @@
         <v>1</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -5410,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -5422,10 +5442,10 @@
         <v>1</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -5460,7 +5480,7 @@
         <v>1</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -5472,10 +5492,10 @@
         <v>1</v>
       </c>
       <c r="O17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -5510,7 +5530,7 @@
         <v>1</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -5522,10 +5542,10 @@
         <v>1</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -5560,7 +5580,7 @@
         <v>1</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -5572,10 +5592,10 @@
         <v>1</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -19413,7 +19433,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K154"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -20624,31 +20644,31 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>561</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>711</v>
+        <v>441</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G35" t="s">
-        <v>427</v>
+        <v>381</v>
       </c>
       <c r="H35" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="I35" t="s">
-        <v>475</v>
+        <v>381</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -20674,16 +20694,16 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G36" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H36" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I36" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -20706,19 +20726,19 @@
         <v>711</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H37" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I37" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -20732,28 +20752,28 @@
         <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>711</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G38" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="H38" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I38" t="s">
-        <v>381</v>
+        <v>716</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -20764,7 +20784,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B39" t="s">
         <v>380</v>
@@ -20773,22 +20793,22 @@
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>441</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H39" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I39" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -20808,22 +20828,22 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H40" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I40" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -20843,7 +20863,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -20858,7 +20878,7 @@
         <v>383</v>
       </c>
       <c r="I41" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -20878,7 +20898,7 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -20913,7 +20933,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -20928,7 +20948,7 @@
         <v>383</v>
       </c>
       <c r="I43" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -20948,7 +20968,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -20983,7 +21003,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -20998,7 +21018,7 @@
         <v>383</v>
       </c>
       <c r="I45" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -21018,7 +21038,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -21053,7 +21073,7 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -21068,7 +21088,7 @@
         <v>383</v>
       </c>
       <c r="I47" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -21088,22 +21108,22 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>441</v>
+        <v>13</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G48" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H48" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I48" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -21123,7 +21143,7 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -21138,7 +21158,7 @@
         <v>383</v>
       </c>
       <c r="I49" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -21158,22 +21178,22 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>441</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>177</v>
+        <v>24</v>
       </c>
       <c r="G50" t="s">
-        <v>427</v>
+        <v>381</v>
       </c>
       <c r="H50" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I50" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -21184,7 +21204,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B51" t="s">
         <v>380</v>
@@ -21193,22 +21213,22 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>441</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>177</v>
+        <v>24</v>
       </c>
       <c r="G51" t="s">
-        <v>427</v>
+        <v>381</v>
       </c>
       <c r="H51" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="I51" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -21228,22 +21248,22 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G52" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H52" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I52" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -21263,10 +21283,10 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
         <v>177</v>
@@ -21275,10 +21295,10 @@
         <v>427</v>
       </c>
       <c r="H53" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I53" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -21298,7 +21318,7 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -21333,7 +21353,7 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -21368,7 +21388,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -21383,7 +21403,7 @@
         <v>385</v>
       </c>
       <c r="I56" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -21403,7 +21423,7 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -21418,7 +21438,7 @@
         <v>385</v>
       </c>
       <c r="I57" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -21438,7 +21458,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -21473,7 +21493,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -21488,7 +21508,7 @@
         <v>385</v>
       </c>
       <c r="I59" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -21508,7 +21528,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -21523,7 +21543,7 @@
         <v>385</v>
       </c>
       <c r="I60" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -21540,25 +21560,25 @@
         <v>380</v>
       </c>
       <c r="C61" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H61" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I61" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -21569,7 +21589,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B62" t="s">
         <v>380</v>
@@ -21578,22 +21598,22 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G62" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H62" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I62" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -21604,7 +21624,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B63" t="s">
         <v>380</v>
@@ -21613,22 +21633,22 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G63" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H63" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I63" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -21639,31 +21659,31 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B64" t="s">
         <v>380</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
       <c r="G64" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H64" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I64" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -21683,7 +21703,7 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -21698,7 +21718,7 @@
         <v>391</v>
       </c>
       <c r="I65" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -21718,7 +21738,7 @@
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -21753,22 +21773,22 @@
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G67" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H67" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I67" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -21788,22 +21808,22 @@
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G68" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H68" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I68" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -21823,22 +21843,22 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G69" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H69" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I69" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -21858,7 +21878,7 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -21873,7 +21893,7 @@
         <v>385</v>
       </c>
       <c r="I70" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -21893,7 +21913,7 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -21908,7 +21928,7 @@
         <v>385</v>
       </c>
       <c r="I71" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -21925,25 +21945,25 @@
         <v>380</v>
       </c>
       <c r="C72" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G72" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H72" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I72" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -21954,31 +21974,31 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
         <v>380</v>
       </c>
       <c r="C73" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G73" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H73" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I73" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -21989,31 +22009,31 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B74" t="s">
         <v>380</v>
       </c>
       <c r="C74" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G74" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H74" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I74" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -22024,7 +22044,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B75" t="s">
         <v>380</v>
@@ -22033,22 +22053,22 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G75" t="s">
         <v>175</v>
       </c>
       <c r="H75" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I75" t="s">
-        <v>402</v>
+        <v>419</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -22068,7 +22088,7 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -22103,7 +22123,7 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -22138,7 +22158,7 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -22153,7 +22173,7 @@
         <v>386</v>
       </c>
       <c r="I78" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -22173,7 +22193,7 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -22188,7 +22208,7 @@
         <v>386</v>
       </c>
       <c r="I79" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -22208,7 +22228,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -22243,7 +22263,7 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -22258,7 +22278,7 @@
         <v>386</v>
       </c>
       <c r="I81" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -22278,7 +22298,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -22293,7 +22313,7 @@
         <v>386</v>
       </c>
       <c r="I82" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -22313,22 +22333,22 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G83" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H83" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I83" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J83">
         <v>0</v>
@@ -22348,22 +22368,22 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G84" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H84" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I84" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="J84">
         <v>0</v>
@@ -22374,31 +22394,31 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B85" t="s">
         <v>380</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G85" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H85" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I85" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -22409,31 +22429,31 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
         <v>380</v>
       </c>
       <c r="C86" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G86" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H86" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I86" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -22444,31 +22464,31 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B87" t="s">
         <v>380</v>
       </c>
       <c r="C87" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G87" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H87" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I87" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -22488,7 +22508,7 @@
         <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -22523,7 +22543,7 @@
         <v>5</v>
       </c>
       <c r="D89" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -22558,7 +22578,7 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -22573,7 +22593,7 @@
         <v>385</v>
       </c>
       <c r="I90" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -22593,7 +22613,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -22608,7 +22628,7 @@
         <v>385</v>
       </c>
       <c r="I91" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J91">
         <v>0</v>
@@ -22628,7 +22648,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -22663,7 +22683,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -22678,7 +22698,7 @@
         <v>385</v>
       </c>
       <c r="I93" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J93">
         <v>0</v>
@@ -22698,7 +22718,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -22713,7 +22733,7 @@
         <v>385</v>
       </c>
       <c r="I94" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="J94">
         <v>0</v>
@@ -22730,25 +22750,25 @@
         <v>380</v>
       </c>
       <c r="C95" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G95" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H95" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I95" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J95">
         <v>0</v>
@@ -22765,25 +22785,25 @@
         <v>380</v>
       </c>
       <c r="C96" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G96" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H96" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I96" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J96">
         <v>0</v>
@@ -22800,25 +22820,25 @@
         <v>380</v>
       </c>
       <c r="C97" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G97" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H97" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I97" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J97">
         <v>0</v>
@@ -22829,7 +22849,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B98" t="s">
         <v>380</v>
@@ -22838,22 +22858,22 @@
         <v>3</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G98" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H98" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I98" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="J98">
         <v>0</v>
@@ -22864,7 +22884,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B99" t="s">
         <v>380</v>
@@ -22873,22 +22893,22 @@
         <v>3</v>
       </c>
       <c r="D99" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G99" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H99" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I99" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
       <c r="J99">
         <v>0</v>
@@ -22899,7 +22919,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B100" t="s">
         <v>380</v>
@@ -22908,22 +22928,22 @@
         <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G100" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H100" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I100" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="J100">
         <v>0</v>
@@ -22943,7 +22963,7 @@
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -22958,7 +22978,7 @@
         <v>383</v>
       </c>
       <c r="I101" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J101">
         <v>0</v>
@@ -22978,7 +22998,7 @@
         <v>3</v>
       </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -22993,7 +23013,7 @@
         <v>383</v>
       </c>
       <c r="I102" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="J102">
         <v>0</v>
@@ -23013,7 +23033,7 @@
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -23028,7 +23048,7 @@
         <v>383</v>
       </c>
       <c r="I103" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J103">
         <v>0</v>
@@ -23048,7 +23068,7 @@
         <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -23083,7 +23103,7 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -23098,7 +23118,7 @@
         <v>383</v>
       </c>
       <c r="I105" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="J105">
         <v>0</v>
@@ -23118,7 +23138,7 @@
         <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -23133,7 +23153,7 @@
         <v>383</v>
       </c>
       <c r="I106" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J106">
         <v>0</v>
@@ -23147,28 +23167,28 @@
         <v>174</v>
       </c>
       <c r="B107" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C107" t="s">
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G107" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H107" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I107" t="s">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="J107">
         <v>0</v>
@@ -23182,28 +23202,28 @@
         <v>174</v>
       </c>
       <c r="B108" t="s">
-        <v>172</v>
+        <v>380</v>
       </c>
       <c r="C108" t="s">
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G108" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H108" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I108" t="s">
-        <v>503</v>
+        <v>404</v>
       </c>
       <c r="J108">
         <v>0</v>
@@ -23214,31 +23234,31 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B109" t="s">
-        <v>172</v>
+        <v>380</v>
       </c>
       <c r="C109" t="s">
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" t="s">
         <v>27</v>
       </c>
       <c r="G109" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H109" t="s">
         <v>383</v>
       </c>
       <c r="I109" t="s">
-        <v>504</v>
+        <v>404</v>
       </c>
       <c r="J109">
         <v>0</v>
@@ -23249,31 +23269,31 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>481</v>
+        <v>174</v>
       </c>
       <c r="B110" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C110" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110" t="s">
-        <v>177</v>
+        <v>26</v>
       </c>
       <c r="G110" t="s">
         <v>427</v>
       </c>
       <c r="H110" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="I110" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J110">
         <v>0</v>
@@ -23284,31 +23304,31 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>481</v>
+        <v>174</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C111" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G111" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H111" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I111" t="s">
-        <v>400</v>
+        <v>503</v>
       </c>
       <c r="J111">
         <v>0</v>
@@ -23319,31 +23339,31 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>481</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>491</v>
+        <v>172</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G112" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H112" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I112" t="s">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="J112">
         <v>0</v>
@@ -23363,7 +23383,7 @@
         <v>5</v>
       </c>
       <c r="D113" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -23398,7 +23418,7 @@
         <v>5</v>
       </c>
       <c r="D114" t="s">
-        <v>493</v>
+        <v>12</v>
       </c>
       <c r="E114">
         <v>0</v>
@@ -23430,25 +23450,25 @@
         <v>380</v>
       </c>
       <c r="C115" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>8</v>
+        <v>491</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G115" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H115" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I115" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J115">
         <v>0</v>
@@ -23465,25 +23485,25 @@
         <v>380</v>
       </c>
       <c r="C116" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G116" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H116" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I116" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J116">
         <v>0</v>
@@ -23500,25 +23520,25 @@
         <v>380</v>
       </c>
       <c r="C117" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="F117" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G117" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H117" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I117" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J117">
         <v>0</v>
@@ -23538,7 +23558,7 @@
         <v>3</v>
       </c>
       <c r="D118" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -23573,7 +23593,7 @@
         <v>3</v>
       </c>
       <c r="D119" t="s">
-        <v>493</v>
+        <v>12</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -23599,31 +23619,31 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B120" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C120" t="s">
         <v>3</v>
       </c>
       <c r="D120" t="s">
-        <v>16</v>
+        <v>491</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G120" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H120" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I120" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="J120">
         <v>0</v>
@@ -23634,16 +23654,16 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B121" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C121" t="s">
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -23658,7 +23678,7 @@
         <v>386</v>
       </c>
       <c r="I121" t="s">
-        <v>408</v>
+        <v>424</v>
       </c>
       <c r="J121">
         <v>0</v>
@@ -23669,31 +23689,31 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B122" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C122" t="s">
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>16</v>
+        <v>493</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
       <c r="F122" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G122" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H122" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I122" t="s">
-        <v>409</v>
+        <v>424</v>
       </c>
       <c r="J122">
         <v>0</v>
@@ -23707,28 +23727,28 @@
         <v>174</v>
       </c>
       <c r="B123" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C123" t="s">
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="G123" t="s">
         <v>427</v>
       </c>
       <c r="H123" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I123" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="J123">
         <v>0</v>
@@ -23742,13 +23762,13 @@
         <v>174</v>
       </c>
       <c r="B124" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C124" t="s">
         <v>3</v>
       </c>
       <c r="D124" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -23763,7 +23783,7 @@
         <v>386</v>
       </c>
       <c r="I124" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="J124">
         <v>0</v>
@@ -23777,28 +23797,28 @@
         <v>174</v>
       </c>
       <c r="B125" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C125" t="s">
         <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F125" t="s">
         <v>27</v>
       </c>
       <c r="G125" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="H125" t="s">
         <v>383</v>
       </c>
       <c r="I125" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="J125">
         <v>0</v>
@@ -23809,31 +23829,31 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B126" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C126" t="s">
         <v>3</v>
       </c>
       <c r="D126" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G126" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H126" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I126" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="J126">
         <v>0</v>
@@ -23844,31 +23864,31 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B127" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C127" t="s">
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
       <c r="F127" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G127" t="s">
         <v>175</v>
       </c>
       <c r="H127" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I127" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="J127">
         <v>0</v>
@@ -23879,31 +23899,31 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B128" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C128" t="s">
         <v>3</v>
       </c>
       <c r="D128" t="s">
-        <v>171</v>
+        <v>15</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F128" t="s">
         <v>27</v>
       </c>
       <c r="G128" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H128" t="s">
         <v>383</v>
       </c>
       <c r="I128" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -23923,7 +23943,7 @@
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -23958,22 +23978,22 @@
         <v>3</v>
       </c>
       <c r="D130" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F130" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G130" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H130" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I130" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J130">
         <v>0</v>
@@ -23993,22 +24013,22 @@
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F131" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G131" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H131" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I131" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="J131">
         <v>0</v>
@@ -24028,22 +24048,22 @@
         <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G132" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H132" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I132" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="J132">
         <v>0</v>
@@ -24063,7 +24083,7 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -24078,7 +24098,7 @@
         <v>391</v>
       </c>
       <c r="I133" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="J133">
         <v>0</v>
@@ -24098,7 +24118,7 @@
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>176</v>
+        <v>13</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -24113,7 +24133,7 @@
         <v>391</v>
       </c>
       <c r="I134" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J134">
         <v>0</v>
@@ -24124,7 +24144,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B135" t="s">
         <v>380</v>
@@ -24133,22 +24153,22 @@
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G135" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H135" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I135" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J135">
         <v>0</v>
@@ -24159,7 +24179,7 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B136" t="s">
         <v>380</v>
@@ -24168,22 +24188,22 @@
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G136" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H136" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I136" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J136">
         <v>0</v>
@@ -24194,7 +24214,7 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B137" t="s">
         <v>380</v>
@@ -24203,22 +24223,22 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F137" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G137" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H137" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I137" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J137">
         <v>0</v>
@@ -24238,7 +24258,7 @@
         <v>3</v>
       </c>
       <c r="D138" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E138">
         <v>0</v>
@@ -24253,7 +24273,7 @@
         <v>392</v>
       </c>
       <c r="I138" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J138">
         <v>0</v>
@@ -24273,7 +24293,7 @@
         <v>3</v>
       </c>
       <c r="D139" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="E139">
         <v>0</v>
@@ -24308,7 +24328,7 @@
         <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -24323,7 +24343,7 @@
         <v>392</v>
       </c>
       <c r="I140" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J140">
         <v>0</v>
@@ -24343,7 +24363,7 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -24358,7 +24378,7 @@
         <v>392</v>
       </c>
       <c r="I141" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="J141">
         <v>0</v>
@@ -24369,31 +24389,31 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B142" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C142" t="s">
         <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>471</v>
+        <v>13</v>
       </c>
       <c r="E142">
         <v>0</v>
       </c>
       <c r="F142" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="G142" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H142" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="I142" t="s">
-        <v>475</v>
+        <v>424</v>
       </c>
       <c r="J142">
         <v>0</v>
@@ -24404,31 +24424,31 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B143" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C143" t="s">
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>471</v>
+        <v>14</v>
       </c>
       <c r="E143">
         <v>0</v>
       </c>
       <c r="F143" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="G143" t="s">
         <v>175</v>
       </c>
       <c r="H143" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I143" t="s">
-        <v>469</v>
+        <v>425</v>
       </c>
       <c r="J143">
         <v>0</v>
@@ -24439,31 +24459,31 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B144" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C144" t="s">
         <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>471</v>
+        <v>171</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F144" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G144" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H144" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I144" t="s">
-        <v>476</v>
+        <v>425</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -24483,7 +24503,7 @@
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -24518,7 +24538,7 @@
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E146">
         <v>0</v>
@@ -24553,7 +24573,7 @@
         <v>3</v>
       </c>
       <c r="D147" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -24588,7 +24608,7 @@
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E148">
         <v>0</v>
@@ -24623,7 +24643,7 @@
         <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E149">
         <v>0</v>
@@ -24658,7 +24678,7 @@
         <v>3</v>
       </c>
       <c r="D150" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -24684,31 +24704,31 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B151" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C151" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D151" t="s">
-        <v>441</v>
+        <v>473</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G151" t="s">
-        <v>381</v>
+        <v>427</v>
       </c>
       <c r="H151" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="I151" t="s">
-        <v>381</v>
+        <v>475</v>
       </c>
       <c r="J151">
         <v>0</v>
@@ -24719,31 +24739,31 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>561</v>
+        <v>174</v>
       </c>
       <c r="B152" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C152" t="s">
         <v>3</v>
       </c>
       <c r="D152" t="s">
-        <v>8</v>
+        <v>473</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F152" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G152" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H152" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I152" t="s">
-        <v>716</v>
+        <v>469</v>
       </c>
       <c r="J152">
         <v>0</v>
@@ -24754,16 +24774,16 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>561</v>
+        <v>174</v>
       </c>
       <c r="B153" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C153" t="s">
         <v>3</v>
       </c>
       <c r="D153" t="s">
-        <v>10</v>
+        <v>473</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -24772,13 +24792,13 @@
         <v>27</v>
       </c>
       <c r="G153" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="H153" t="s">
         <v>383</v>
       </c>
       <c r="I153" t="s">
-        <v>716</v>
+        <v>476</v>
       </c>
       <c r="J153">
         <v>0</v>
@@ -24789,36 +24809,141 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>561</v>
+        <v>175</v>
       </c>
       <c r="B154" t="s">
         <v>380</v>
       </c>
       <c r="C154" t="s">
+        <v>5</v>
+      </c>
+      <c r="D154" t="s">
+        <v>441</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154" t="s">
+        <v>24</v>
+      </c>
+      <c r="G154" t="s">
+        <v>381</v>
+      </c>
+      <c r="H154" t="s">
+        <v>381</v>
+      </c>
+      <c r="I154" t="s">
+        <v>381</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>561</v>
+      </c>
+      <c r="B155" t="s">
+        <v>380</v>
+      </c>
+      <c r="C155" t="s">
         <v>3</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D155" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155">
+        <v>1</v>
+      </c>
+      <c r="F155" t="s">
+        <v>27</v>
+      </c>
+      <c r="G155" t="s">
+        <v>382</v>
+      </c>
+      <c r="H155" t="s">
+        <v>383</v>
+      </c>
+      <c r="I155" t="s">
+        <v>716</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>561</v>
+      </c>
+      <c r="B156" t="s">
+        <v>380</v>
+      </c>
+      <c r="C156" t="s">
+        <v>3</v>
+      </c>
+      <c r="D156" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>27</v>
+      </c>
+      <c r="G156" t="s">
+        <v>382</v>
+      </c>
+      <c r="H156" t="s">
+        <v>383</v>
+      </c>
+      <c r="I156" t="s">
+        <v>716</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>561</v>
+      </c>
+      <c r="B157" t="s">
+        <v>380</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3</v>
+      </c>
+      <c r="D157" t="s">
         <v>7</v>
       </c>
-      <c r="E154">
-        <v>1</v>
-      </c>
-      <c r="F154" t="s">
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157" t="s">
         <v>27</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G157" t="s">
         <v>382</v>
       </c>
-      <c r="H154" t="s">
+      <c r="H157" t="s">
         <v>383</v>
       </c>
-      <c r="I154" t="s">
+      <c r="I157" t="s">
         <v>716</v>
       </c>
-      <c r="J154">
-        <v>0</v>
-      </c>
-      <c r="K154" t="s">
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157" t="s">
         <v>381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Internal version 32. Updated for TFS 1013 new Direct source for Sup Module.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33413
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="762">
   <si>
     <t>SourceID</t>
   </si>
@@ -2319,6 +2319,12 @@
   </si>
   <si>
     <t>Open Warnings for all Modules (LSA, Training and Quality Modules)Updated Coaching_Reason_Selection and Email_Notification tabs</t>
+  </si>
+  <si>
+    <t>Add new Direct Source for Supervisor Module UI Submissions. Updated Dim_Source and Email_Notifications tabs</t>
+  </si>
+  <si>
+    <t>Coach the coach</t>
   </si>
 </sst>
 </file>
@@ -2680,7 +2686,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3283,6 +3289,23 @@
       </c>
       <c r="E35" t="s">
         <v>759</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36" s="1">
+        <v>42307</v>
+      </c>
+      <c r="C36" t="s">
+        <v>434</v>
+      </c>
+      <c r="D36">
+        <v>1013</v>
+      </c>
+      <c r="E36" t="s">
+        <v>760</v>
       </c>
     </row>
   </sheetData>
@@ -19433,9 +19456,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A117" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20819,7 +20842,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B40" t="s">
         <v>380</v>
@@ -20828,22 +20851,22 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>761</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="G40" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H40" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="I40" t="s">
-        <v>381</v>
+        <v>413</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -20854,7 +20877,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B41" t="s">
         <v>380</v>
@@ -20863,22 +20886,22 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>761</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G41" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H41" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I41" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -20898,22 +20921,22 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G42" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H42" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I42" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -20933,7 +20956,7 @@
         <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -20948,7 +20971,7 @@
         <v>383</v>
       </c>
       <c r="I43" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -20968,7 +20991,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -21003,7 +21026,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -21018,7 +21041,7 @@
         <v>383</v>
       </c>
       <c r="I45" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -21038,7 +21061,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -21073,7 +21096,7 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -21088,7 +21111,7 @@
         <v>383</v>
       </c>
       <c r="I47" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -21108,7 +21131,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -21143,7 +21166,7 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -21158,7 +21181,7 @@
         <v>383</v>
       </c>
       <c r="I49" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -21178,22 +21201,22 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>441</v>
+        <v>13</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G50" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H50" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I50" t="s">
-        <v>381</v>
+        <v>394</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -21204,7 +21227,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
         <v>380</v>
@@ -21213,22 +21236,22 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>441</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G51" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H51" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I51" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -21248,22 +21271,22 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>171</v>
+        <v>441</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G52" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H52" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I52" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -21274,7 +21297,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
         <v>380</v>
@@ -21283,22 +21306,22 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>441</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>177</v>
+        <v>24</v>
       </c>
       <c r="G53" t="s">
-        <v>427</v>
+        <v>381</v>
       </c>
       <c r="H53" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="I53" t="s">
-        <v>398</v>
+        <v>381</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -21318,22 +21341,22 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G54" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H54" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I54" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -21356,7 +21379,7 @@
         <v>8</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="s">
         <v>177</v>
@@ -21365,10 +21388,10 @@
         <v>427</v>
       </c>
       <c r="H55" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I55" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -21388,7 +21411,7 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -21403,7 +21426,7 @@
         <v>385</v>
       </c>
       <c r="I56" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -21423,7 +21446,7 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -21458,7 +21481,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -21473,7 +21496,7 @@
         <v>385</v>
       </c>
       <c r="I58" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -21493,7 +21516,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -21528,7 +21551,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -21543,7 +21566,7 @@
         <v>385</v>
       </c>
       <c r="I60" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -21563,7 +21586,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -21598,7 +21621,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -21613,7 +21636,7 @@
         <v>385</v>
       </c>
       <c r="I62" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -21633,7 +21656,7 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -21648,7 +21671,7 @@
         <v>385</v>
       </c>
       <c r="I63" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -21665,25 +21688,25 @@
         <v>380</v>
       </c>
       <c r="C64" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G64" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H64" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -21694,7 +21717,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
         <v>380</v>
@@ -21703,22 +21726,22 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G65" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H65" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="I65" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -21729,31 +21752,31 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B66" t="s">
         <v>380</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
       <c r="G66" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H66" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I66" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -21773,7 +21796,7 @@
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -21788,7 +21811,7 @@
         <v>391</v>
       </c>
       <c r="I67" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -21808,7 +21831,7 @@
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -21823,7 +21846,7 @@
         <v>391</v>
       </c>
       <c r="I68" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -21843,7 +21866,7 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -21858,7 +21881,7 @@
         <v>391</v>
       </c>
       <c r="I69" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -21878,22 +21901,22 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G70" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H70" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I70" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -21913,22 +21936,22 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G71" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H71" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I71" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -21948,7 +21971,7 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -21963,7 +21986,7 @@
         <v>385</v>
       </c>
       <c r="I72" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -21983,7 +22006,7 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -21998,7 +22021,7 @@
         <v>385</v>
       </c>
       <c r="I73" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -22018,7 +22041,7 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -22050,25 +22073,25 @@
         <v>380</v>
       </c>
       <c r="C75" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G75" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H75" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I75" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -22079,31 +22102,31 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
         <v>380</v>
       </c>
       <c r="C76" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>7</v>
+        <v>176</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G76" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H76" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I76" t="s">
-        <v>401</v>
+        <v>418</v>
       </c>
       <c r="J76">
         <v>0</v>
@@ -22114,7 +22137,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B77" t="s">
         <v>380</v>
@@ -22123,22 +22146,22 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G77" t="s">
         <v>175</v>
       </c>
       <c r="H77" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I77" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -22158,7 +22181,7 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -22173,7 +22196,7 @@
         <v>386</v>
       </c>
       <c r="I78" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -22193,7 +22216,7 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -22228,7 +22251,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -22243,7 +22266,7 @@
         <v>386</v>
       </c>
       <c r="I80" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J80">
         <v>0</v>
@@ -22263,7 +22286,7 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -22298,7 +22321,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -22313,7 +22336,7 @@
         <v>386</v>
       </c>
       <c r="I82" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -22333,7 +22356,7 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -22368,7 +22391,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -22383,7 +22406,7 @@
         <v>386</v>
       </c>
       <c r="I84" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J84">
         <v>0</v>
@@ -22403,7 +22426,7 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -22438,22 +22461,22 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G86" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H86" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I86" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -22473,22 +22496,22 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G87" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H87" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I87" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -22499,31 +22522,31 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
         <v>380</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G88" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H88" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I88" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="J88">
         <v>0</v>
@@ -22534,31 +22557,31 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B89" t="s">
         <v>380</v>
       </c>
       <c r="C89" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G89" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H89" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I89" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="J89">
         <v>0</v>
@@ -22578,7 +22601,7 @@
         <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -22593,7 +22616,7 @@
         <v>385</v>
       </c>
       <c r="I90" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -22613,7 +22636,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -22648,7 +22671,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -22663,7 +22686,7 @@
         <v>385</v>
       </c>
       <c r="I92" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="J92">
         <v>0</v>
@@ -22683,7 +22706,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -22718,7 +22741,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -22733,7 +22756,7 @@
         <v>385</v>
       </c>
       <c r="I94" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J94">
         <v>0</v>
@@ -22753,7 +22776,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -22788,7 +22811,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -22803,7 +22826,7 @@
         <v>385</v>
       </c>
       <c r="I96" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="J96">
         <v>0</v>
@@ -22823,7 +22846,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -22838,7 +22861,7 @@
         <v>385</v>
       </c>
       <c r="I97" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J97">
         <v>0</v>
@@ -22855,25 +22878,25 @@
         <v>380</v>
       </c>
       <c r="C98" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G98" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H98" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I98" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J98">
         <v>0</v>
@@ -22890,25 +22913,25 @@
         <v>380</v>
       </c>
       <c r="C99" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G99" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H99" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I99" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J99">
         <v>0</v>
@@ -22928,7 +22951,7 @@
         <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -22943,7 +22966,7 @@
         <v>392</v>
       </c>
       <c r="I100" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J100">
         <v>0</v>
@@ -22954,7 +22977,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B101" t="s">
         <v>380</v>
@@ -22966,19 +22989,19 @@
         <v>8</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G101" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H101" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I101" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="J101">
         <v>0</v>
@@ -22989,7 +23012,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
         <v>380</v>
@@ -23001,19 +23024,19 @@
         <v>9</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G102" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H102" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I102" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
       <c r="J102">
         <v>0</v>
@@ -23033,7 +23056,7 @@
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -23048,7 +23071,7 @@
         <v>383</v>
       </c>
       <c r="I103" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J103">
         <v>0</v>
@@ -23068,7 +23091,7 @@
         <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -23083,7 +23106,7 @@
         <v>383</v>
       </c>
       <c r="I104" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J104">
         <v>0</v>
@@ -23103,7 +23126,7 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -23118,7 +23141,7 @@
         <v>383</v>
       </c>
       <c r="I105" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J105">
         <v>0</v>
@@ -23138,7 +23161,7 @@
         <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -23153,7 +23176,7 @@
         <v>383</v>
       </c>
       <c r="I106" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="J106">
         <v>0</v>
@@ -23173,7 +23196,7 @@
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -23188,7 +23211,7 @@
         <v>383</v>
       </c>
       <c r="I107" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="J107">
         <v>0</v>
@@ -23208,7 +23231,7 @@
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -23223,7 +23246,7 @@
         <v>383</v>
       </c>
       <c r="I108" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="J108">
         <v>0</v>
@@ -23243,7 +23266,7 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -23258,7 +23281,7 @@
         <v>383</v>
       </c>
       <c r="I109" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J109">
         <v>0</v>
@@ -23272,28 +23295,28 @@
         <v>174</v>
       </c>
       <c r="B110" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C110" t="s">
         <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G110" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H110" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I110" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J110">
         <v>0</v>
@@ -23307,28 +23330,28 @@
         <v>174</v>
       </c>
       <c r="B111" t="s">
-        <v>172</v>
+        <v>380</v>
       </c>
       <c r="C111" t="s">
         <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G111" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H111" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I111" t="s">
-        <v>503</v>
+        <v>404</v>
       </c>
       <c r="J111">
         <v>0</v>
@@ -23339,31 +23362,31 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B112" t="s">
-        <v>172</v>
+        <v>387</v>
       </c>
       <c r="C112" t="s">
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G112" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H112" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I112" t="s">
-        <v>504</v>
+        <v>399</v>
       </c>
       <c r="J112">
         <v>0</v>
@@ -23374,31 +23397,31 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>481</v>
+        <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G113" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H113" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I113" t="s">
-        <v>400</v>
+        <v>503</v>
       </c>
       <c r="J113">
         <v>0</v>
@@ -23409,31 +23432,31 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>481</v>
+        <v>175</v>
       </c>
       <c r="B114" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>172</v>
       </c>
       <c r="E114">
         <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G114" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H114" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I114" t="s">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="J114">
         <v>0</v>
@@ -23453,7 +23476,7 @@
         <v>5</v>
       </c>
       <c r="D115" t="s">
-        <v>491</v>
+        <v>8</v>
       </c>
       <c r="E115">
         <v>0</v>
@@ -23488,7 +23511,7 @@
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -23523,7 +23546,7 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -23555,25 +23578,25 @@
         <v>380</v>
       </c>
       <c r="C118" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="F118" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G118" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H118" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I118" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J118">
         <v>0</v>
@@ -23590,25 +23613,25 @@
         <v>380</v>
       </c>
       <c r="C119" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>12</v>
+        <v>493</v>
       </c>
       <c r="E119">
         <v>0</v>
       </c>
       <c r="F119" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G119" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H119" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I119" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J119">
         <v>0</v>
@@ -23628,7 +23651,7 @@
         <v>3</v>
       </c>
       <c r="D120" t="s">
-        <v>491</v>
+        <v>8</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -23663,7 +23686,7 @@
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -23698,7 +23721,7 @@
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -23724,31 +23747,31 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B123" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C123" t="s">
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>16</v>
+        <v>170</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="F123" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G123" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H123" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I123" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="J123">
         <v>0</v>
@@ -23759,16 +23782,16 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B124" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C124" t="s">
         <v>3</v>
       </c>
       <c r="D124" t="s">
-        <v>16</v>
+        <v>493</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -23783,7 +23806,7 @@
         <v>386</v>
       </c>
       <c r="I124" t="s">
-        <v>408</v>
+        <v>424</v>
       </c>
       <c r="J124">
         <v>0</v>
@@ -23809,16 +23832,16 @@
         <v>0</v>
       </c>
       <c r="F125" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G125" t="s">
-        <v>382</v>
+        <v>427</v>
       </c>
       <c r="H125" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="I125" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="J125">
         <v>0</v>
@@ -23832,28 +23855,28 @@
         <v>174</v>
       </c>
       <c r="B126" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C126" t="s">
         <v>3</v>
       </c>
       <c r="D126" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G126" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H126" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I126" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="J126">
         <v>0</v>
@@ -23867,28 +23890,28 @@
         <v>174</v>
       </c>
       <c r="B127" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C127" t="s">
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E127">
         <v>0</v>
       </c>
       <c r="F127" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G127" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H127" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I127" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="J127">
         <v>0</v>
@@ -23911,19 +23934,19 @@
         <v>15</v>
       </c>
       <c r="E128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G128" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="H128" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I128" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -23934,31 +23957,31 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B129" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C129" t="s">
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E129">
         <v>0</v>
       </c>
       <c r="F129" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G129" t="s">
         <v>175</v>
       </c>
       <c r="H129" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I129" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="J129">
         <v>0</v>
@@ -23969,31 +23992,31 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B130" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C130" t="s">
         <v>3</v>
       </c>
       <c r="D130" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130" t="s">
         <v>27</v>
       </c>
       <c r="G130" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H130" t="s">
         <v>383</v>
       </c>
       <c r="I130" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="J130">
         <v>0</v>
@@ -24013,7 +24036,7 @@
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E131">
         <v>0</v>
@@ -24048,7 +24071,7 @@
         <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -24063,7 +24086,7 @@
         <v>383</v>
       </c>
       <c r="I132" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J132">
         <v>0</v>
@@ -24083,22 +24106,22 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="E133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F133" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G133" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H133" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I133" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J133">
         <v>0</v>
@@ -24118,22 +24141,22 @@
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>13</v>
+        <v>176</v>
       </c>
       <c r="E134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F134" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G134" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H134" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I134" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="J134">
         <v>0</v>
@@ -24153,7 +24176,7 @@
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -24168,7 +24191,7 @@
         <v>391</v>
       </c>
       <c r="I135" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="J135">
         <v>0</v>
@@ -24188,7 +24211,7 @@
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -24203,7 +24226,7 @@
         <v>391</v>
       </c>
       <c r="I136" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J136">
         <v>0</v>
@@ -24223,7 +24246,7 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -24249,7 +24272,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B138" t="s">
         <v>380</v>
@@ -24258,22 +24281,22 @@
         <v>3</v>
       </c>
       <c r="D138" t="s">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G138" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H138" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I138" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J138">
         <v>0</v>
@@ -24284,7 +24307,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B139" t="s">
         <v>380</v>
@@ -24293,22 +24316,22 @@
         <v>3</v>
       </c>
       <c r="D139" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F139" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G139" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H139" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I139" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J139">
         <v>0</v>
@@ -24328,7 +24351,7 @@
         <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E140">
         <v>0</v>
@@ -24363,7 +24386,7 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>12</v>
+        <v>170</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -24378,7 +24401,7 @@
         <v>392</v>
       </c>
       <c r="I141" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J141">
         <v>0</v>
@@ -24398,7 +24421,7 @@
         <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -24433,7 +24456,7 @@
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -24448,7 +24471,7 @@
         <v>392</v>
       </c>
       <c r="I143" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="J143">
         <v>0</v>
@@ -24468,7 +24491,7 @@
         <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -24483,7 +24506,7 @@
         <v>392</v>
       </c>
       <c r="I144" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -24494,31 +24517,31 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B145" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C145" t="s">
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>471</v>
+        <v>14</v>
       </c>
       <c r="E145">
         <v>0</v>
       </c>
       <c r="F145" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="G145" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H145" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="I145" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="J145">
         <v>0</v>
@@ -24529,31 +24552,31 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B146" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C146" t="s">
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>471</v>
+        <v>171</v>
       </c>
       <c r="E146">
         <v>0</v>
       </c>
       <c r="F146" t="s">
-        <v>28</v>
+        <v>179</v>
       </c>
       <c r="G146" t="s">
         <v>175</v>
       </c>
       <c r="H146" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="I146" t="s">
-        <v>469</v>
+        <v>425</v>
       </c>
       <c r="J146">
         <v>0</v>
@@ -24576,19 +24599,19 @@
         <v>471</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G147" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="H147" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I147" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J147">
         <v>0</v>
@@ -24608,22 +24631,22 @@
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E148">
         <v>0</v>
       </c>
       <c r="F148" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G148" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H148" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I148" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="J148">
         <v>0</v>
@@ -24643,22 +24666,22 @@
         <v>3</v>
       </c>
       <c r="D149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F149" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G149" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H149" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I149" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="J149">
         <v>0</v>
@@ -24681,19 +24704,19 @@
         <v>472</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F150" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G150" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="H150" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I150" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J150">
         <v>0</v>
@@ -24713,22 +24736,22 @@
         <v>3</v>
       </c>
       <c r="D151" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G151" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H151" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I151" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="J151">
         <v>0</v>
@@ -24748,22 +24771,22 @@
         <v>3</v>
       </c>
       <c r="D152" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G152" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H152" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I152" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="J152">
         <v>0</v>
@@ -24786,19 +24809,19 @@
         <v>473</v>
       </c>
       <c r="E153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G153" t="s">
-        <v>390</v>
+        <v>427</v>
       </c>
       <c r="H153" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="I153" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J153">
         <v>0</v>
@@ -24809,31 +24832,31 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>174</v>
+      </c>
+      <c r="B154" t="s">
+        <v>15</v>
+      </c>
+      <c r="C154" t="s">
+        <v>3</v>
+      </c>
+      <c r="D154" t="s">
+        <v>473</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154" t="s">
+        <v>28</v>
+      </c>
+      <c r="G154" t="s">
         <v>175</v>
       </c>
-      <c r="B154" t="s">
-        <v>380</v>
-      </c>
-      <c r="C154" t="s">
-        <v>5</v>
-      </c>
-      <c r="D154" t="s">
-        <v>441</v>
-      </c>
-      <c r="E154">
-        <v>0</v>
-      </c>
-      <c r="F154" t="s">
-        <v>24</v>
-      </c>
-      <c r="G154" t="s">
-        <v>381</v>
-      </c>
       <c r="H154" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="I154" t="s">
-        <v>381</v>
+        <v>469</v>
       </c>
       <c r="J154">
         <v>0</v>
@@ -24844,16 +24867,16 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>561</v>
+        <v>174</v>
       </c>
       <c r="B155" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C155" t="s">
         <v>3</v>
       </c>
       <c r="D155" t="s">
-        <v>8</v>
+        <v>473</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -24862,13 +24885,13 @@
         <v>27</v>
       </c>
       <c r="G155" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="H155" t="s">
         <v>383</v>
       </c>
       <c r="I155" t="s">
-        <v>716</v>
+        <v>476</v>
       </c>
       <c r="J155">
         <v>0</v>
@@ -24879,31 +24902,31 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>561</v>
+        <v>175</v>
       </c>
       <c r="B156" t="s">
         <v>380</v>
       </c>
       <c r="C156" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D156" t="s">
-        <v>10</v>
+        <v>441</v>
       </c>
       <c r="E156">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F156" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G156" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H156" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I156" t="s">
-        <v>716</v>
+        <v>381</v>
       </c>
       <c r="J156">
         <v>0</v>
@@ -24923,7 +24946,7 @@
         <v>3</v>
       </c>
       <c r="D157" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -24944,6 +24967,76 @@
         <v>0</v>
       </c>
       <c r="K157" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>561</v>
+      </c>
+      <c r="B158" t="s">
+        <v>380</v>
+      </c>
+      <c r="C158" t="s">
+        <v>3</v>
+      </c>
+      <c r="D158" t="s">
+        <v>10</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158" t="s">
+        <v>27</v>
+      </c>
+      <c r="G158" t="s">
+        <v>382</v>
+      </c>
+      <c r="H158" t="s">
+        <v>383</v>
+      </c>
+      <c r="I158" t="s">
+        <v>716</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>561</v>
+      </c>
+      <c r="B159" t="s">
+        <v>380</v>
+      </c>
+      <c r="C159" t="s">
+        <v>3</v>
+      </c>
+      <c r="D159" t="s">
+        <v>7</v>
+      </c>
+      <c r="E159">
+        <v>1</v>
+      </c>
+      <c r="F159" t="s">
+        <v>27</v>
+      </c>
+      <c r="G159" t="s">
+        <v>382</v>
+      </c>
+      <c r="H159" t="s">
+        <v>383</v>
+      </c>
+      <c r="I159" t="s">
+        <v>716</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159" t="s">
         <v>381</v>
       </c>
     </row>
@@ -25684,9 +25777,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0"/>
+    <sheetView topLeftCell="A23" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26654,22 +26747,22 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>761</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -26683,13 +26776,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -26701,24 +26794,24 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -26733,7 +26826,7 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -26741,13 +26834,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -26762,21 +26855,21 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -26794,18 +26887,18 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -26820,7 +26913,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39">
         <v>1</v>
@@ -26828,13 +26921,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -26849,7 +26942,7 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -26857,13 +26950,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -26872,27 +26965,27 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B42" t="s">
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -26907,21 +27000,21 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -26939,30 +27032,30 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -26973,13 +27066,13 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B45" t="s">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -27002,13 +27095,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B46" t="s">
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -27031,13 +27124,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -27060,13 +27153,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -27089,13 +27182,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -27118,13 +27211,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -27147,71 +27240,71 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B51" t="s">
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>21</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>441</v>
+        <v>176</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -27220,7 +27313,7 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -27234,13 +27327,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>441</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -27263,13 +27356,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B55" t="s">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>474</v>
+        <v>172</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -27292,13 +27385,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B56" t="s">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -27321,13 +27414,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B57" t="s">
         <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -27350,13 +27443,13 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B58" t="s">
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -27371,7 +27464,7 @@
         <v>0</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -27379,16 +27472,16 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B59" t="s">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -27400,7 +27493,7 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -27408,16 +27501,16 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -27429,7 +27522,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -27437,13 +27530,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B61" t="s">
         <v>3</v>
       </c>
       <c r="C61" t="s">
-        <v>563</v>
+        <v>493</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -27458,21 +27551,21 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B62" t="s">
         <v>3</v>
       </c>
       <c r="C62" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -27495,30 +27588,88 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B63" t="s">
         <v>3</v>
       </c>
       <c r="C63" t="s">
+        <v>564</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>230</v>
+      </c>
+      <c r="B64" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
         <v>711</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>231</v>
+      </c>
+      <c r="B65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>761</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Internal version 33 Updated for TFS 1016 new SCR under CCI for CSR Module
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33415
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="764">
   <si>
     <t>SourceID</t>
   </si>
@@ -2325,6 +2325,12 @@
   </si>
   <si>
     <t>Coach the coach</t>
+  </si>
+  <si>
+    <t>Added 1 new sub coach reason under CCI for CSR  Module in tables DIM_subCoaching_Reason and Coaching_Reason_selection.</t>
+  </si>
+  <si>
+    <t>Short Duration Reporting</t>
   </si>
 </sst>
 </file>
@@ -2686,7 +2692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3306,6 +3312,23 @@
       </c>
       <c r="E36" t="s">
         <v>760</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37" s="1">
+        <v>42307</v>
+      </c>
+      <c r="C37" t="s">
+        <v>434</v>
+      </c>
+      <c r="D37">
+        <v>1016</v>
+      </c>
+      <c r="E37" t="s">
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -4662,9 +4685,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P293"/>
+  <dimension ref="A1:P294"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A252" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12223,25 +12246,25 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="B152" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="C152">
-        <v>-1</v>
+        <v>232</v>
       </c>
       <c r="D152" t="s">
-        <v>4</v>
+        <v>763</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H152">
         <v>1</v>
@@ -12250,7 +12273,7 @@
         <v>1</v>
       </c>
       <c r="J152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K152">
         <v>0</v>
@@ -12273,25 +12296,25 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B153" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C153">
-        <v>42</v>
+        <v>-1</v>
       </c>
       <c r="D153" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H153">
         <v>1</v>
@@ -12300,13 +12323,13 @@
         <v>1</v>
       </c>
       <c r="J153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K153">
         <v>0</v>
       </c>
       <c r="L153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M153">
         <v>0</v>
@@ -12323,16 +12346,16 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B154" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C154">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D154" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="E154">
         <v>1</v>
@@ -12356,7 +12379,7 @@
         <v>0</v>
       </c>
       <c r="L154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M154">
         <v>0</v>
@@ -12379,10 +12402,10 @@
         <v>85</v>
       </c>
       <c r="C155">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D155" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -12429,10 +12452,10 @@
         <v>85</v>
       </c>
       <c r="C156">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D156" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -12479,10 +12502,10 @@
         <v>85</v>
       </c>
       <c r="C157">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D157" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -12529,10 +12552,10 @@
         <v>85</v>
       </c>
       <c r="C158">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D158" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -12579,10 +12602,10 @@
         <v>85</v>
       </c>
       <c r="C159">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D159" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -12629,10 +12652,10 @@
         <v>85</v>
       </c>
       <c r="C160">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D160" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -12679,10 +12702,10 @@
         <v>85</v>
       </c>
       <c r="C161">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D161" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -12723,16 +12746,16 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B162" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C162">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D162" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -12741,7 +12764,7 @@
         <v>1</v>
       </c>
       <c r="G162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H162">
         <v>1</v>
@@ -12779,10 +12802,10 @@
         <v>86</v>
       </c>
       <c r="C163">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D163" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -12791,7 +12814,7 @@
         <v>1</v>
       </c>
       <c r="G163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H163">
         <v>1</v>
@@ -12803,10 +12826,10 @@
         <v>1</v>
       </c>
       <c r="K163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M163">
         <v>0</v>
@@ -12815,24 +12838,24 @@
         <v>0</v>
       </c>
       <c r="O163">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B164" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D164" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -12853,7 +12876,7 @@
         <v>1</v>
       </c>
       <c r="K164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L164">
         <v>1</v>
@@ -12865,10 +12888,10 @@
         <v>0</v>
       </c>
       <c r="O164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P164">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
@@ -12879,10 +12902,10 @@
         <v>181</v>
       </c>
       <c r="C165">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D165" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -12923,10 +12946,10 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="C166">
         <v>42</v>
@@ -12956,7 +12979,7 @@
         <v>0</v>
       </c>
       <c r="L166">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M166">
         <v>0</v>
@@ -12973,16 +12996,16 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B167" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C167">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D167" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -12997,7 +13020,7 @@
         <v>1</v>
       </c>
       <c r="I167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J167">
         <v>1</v>
@@ -13006,13 +13029,13 @@
         <v>0</v>
       </c>
       <c r="L167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M167">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N167">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O167">
         <v>0</v>
@@ -13029,10 +13052,10 @@
         <v>88</v>
       </c>
       <c r="C168">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D168" t="s">
-        <v>344</v>
+        <v>100</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -13079,10 +13102,10 @@
         <v>88</v>
       </c>
       <c r="C169">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D169" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -13106,7 +13129,7 @@
         <v>0</v>
       </c>
       <c r="L169">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M169">
         <v>1</v>
@@ -13129,10 +13152,10 @@
         <v>88</v>
       </c>
       <c r="C170">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D170" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -13156,7 +13179,7 @@
         <v>0</v>
       </c>
       <c r="L170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M170">
         <v>1</v>
@@ -13179,10 +13202,10 @@
         <v>88</v>
       </c>
       <c r="C171">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D171" t="s">
-        <v>103</v>
+        <v>346</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -13229,10 +13252,10 @@
         <v>88</v>
       </c>
       <c r="C172">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D172" t="s">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -13279,10 +13302,10 @@
         <v>88</v>
       </c>
       <c r="C173">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D173" t="s">
-        <v>105</v>
+        <v>347</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -13329,10 +13352,10 @@
         <v>88</v>
       </c>
       <c r="C174">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D174" t="s">
-        <v>236</v>
+        <v>105</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13379,10 +13402,10 @@
         <v>88</v>
       </c>
       <c r="C175">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D175" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13429,10 +13452,10 @@
         <v>88</v>
       </c>
       <c r="C176">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D176" t="s">
-        <v>101</v>
+        <v>237</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -13479,10 +13502,10 @@
         <v>88</v>
       </c>
       <c r="C177">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D177" t="s">
-        <v>206</v>
+        <v>101</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -13518,21 +13541,21 @@
         <v>0</v>
       </c>
       <c r="P177">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B178" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C178">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D178" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -13547,7 +13570,7 @@
         <v>1</v>
       </c>
       <c r="I178">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J178">
         <v>1</v>
@@ -13556,19 +13579,19 @@
         <v>0</v>
       </c>
       <c r="L178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N178">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O178">
         <v>0</v>
       </c>
       <c r="P178">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
@@ -13579,10 +13602,10 @@
         <v>89</v>
       </c>
       <c r="C179">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D179" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -13623,10 +13646,10 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B180" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C180">
         <v>42</v>
@@ -13673,16 +13696,16 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B181" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C181">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D181" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -13729,10 +13752,10 @@
         <v>91</v>
       </c>
       <c r="C182">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D182" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -13779,10 +13802,10 @@
         <v>91</v>
       </c>
       <c r="C183">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D183" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -13829,10 +13852,10 @@
         <v>91</v>
       </c>
       <c r="C184">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D184" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -13879,10 +13902,10 @@
         <v>91</v>
       </c>
       <c r="C185">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D185" t="s">
-        <v>348</v>
+        <v>120</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -13929,10 +13952,10 @@
         <v>91</v>
       </c>
       <c r="C186">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D186" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -13979,10 +14002,10 @@
         <v>91</v>
       </c>
       <c r="C187">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D187" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -14029,10 +14052,10 @@
         <v>91</v>
       </c>
       <c r="C188">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D188" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -14079,10 +14102,10 @@
         <v>91</v>
       </c>
       <c r="C189">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D189" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -14100,7 +14123,7 @@
         <v>1</v>
       </c>
       <c r="J189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K189">
         <v>0</v>
@@ -14129,10 +14152,10 @@
         <v>91</v>
       </c>
       <c r="C190">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D190" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -14150,7 +14173,7 @@
         <v>1</v>
       </c>
       <c r="J190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K190">
         <v>0</v>
@@ -14179,10 +14202,10 @@
         <v>91</v>
       </c>
       <c r="C191">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D191" t="s">
-        <v>350</v>
+        <v>116</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -14229,10 +14252,10 @@
         <v>91</v>
       </c>
       <c r="C192">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D192" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -14279,10 +14302,10 @@
         <v>91</v>
       </c>
       <c r="C193">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D193" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -14323,16 +14346,16 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B194" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C194">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D194" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -14379,10 +14402,10 @@
         <v>92</v>
       </c>
       <c r="C195">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D195" t="s">
-        <v>352</v>
+        <v>140</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -14429,10 +14452,10 @@
         <v>92</v>
       </c>
       <c r="C196">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D196" t="s">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -14479,10 +14502,10 @@
         <v>92</v>
       </c>
       <c r="C197">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D197" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -14529,10 +14552,10 @@
         <v>92</v>
       </c>
       <c r="C198">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D198" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -14579,10 +14602,10 @@
         <v>92</v>
       </c>
       <c r="C199">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D199" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -14615,7 +14638,7 @@
         <v>0</v>
       </c>
       <c r="O199">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P199">
         <v>0</v>
@@ -14623,10 +14646,10 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B200" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C200">
         <v>42</v>
@@ -14644,7 +14667,7 @@
         <v>1</v>
       </c>
       <c r="H200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I200">
         <v>1</v>
@@ -14653,7 +14676,7 @@
         <v>1</v>
       </c>
       <c r="K200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L200">
         <v>0</v>
@@ -14668,7 +14691,7 @@
         <v>1</v>
       </c>
       <c r="P200">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
@@ -14679,10 +14702,10 @@
         <v>93</v>
       </c>
       <c r="C201">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D201" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -14700,7 +14723,7 @@
         <v>1</v>
       </c>
       <c r="J201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K201">
         <v>1</v>
@@ -14718,7 +14741,7 @@
         <v>1</v>
       </c>
       <c r="P201">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
@@ -14729,10 +14752,10 @@
         <v>93</v>
       </c>
       <c r="C202">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D202" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -14765,7 +14788,7 @@
         <v>0</v>
       </c>
       <c r="O202">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P202">
         <v>0</v>
@@ -14773,16 +14796,16 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B203" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C203">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D203" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -14794,19 +14817,19 @@
         <v>1</v>
       </c>
       <c r="H203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I203">
         <v>1</v>
       </c>
       <c r="J203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L203">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M203">
         <v>0</v>
@@ -14823,10 +14846,10 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B204" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C204">
         <v>42</v>
@@ -14853,10 +14876,10 @@
         <v>1</v>
       </c>
       <c r="K204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M204">
         <v>0</v>
@@ -14865,24 +14888,24 @@
         <v>0</v>
       </c>
       <c r="O204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P204">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B205" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C205">
         <v>42</v>
       </c>
       <c r="D205" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="E205">
         <v>1</v>
@@ -14900,10 +14923,10 @@
         <v>1</v>
       </c>
       <c r="J205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L205">
         <v>0</v>
@@ -14915,24 +14938,24 @@
         <v>0</v>
       </c>
       <c r="O205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P205">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B206" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C206">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D206" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="E206">
         <v>1</v>
@@ -14953,7 +14976,7 @@
         <v>0</v>
       </c>
       <c r="K206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L206">
         <v>0</v>
@@ -14979,10 +15002,10 @@
         <v>182</v>
       </c>
       <c r="C207">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D207" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E207">
         <v>1</v>
@@ -15029,10 +15052,10 @@
         <v>182</v>
       </c>
       <c r="C208">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D208" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -15079,10 +15102,10 @@
         <v>182</v>
       </c>
       <c r="C209">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D209" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -15129,10 +15152,10 @@
         <v>182</v>
       </c>
       <c r="C210">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D210" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E210">
         <v>1</v>
@@ -15179,10 +15202,10 @@
         <v>182</v>
       </c>
       <c r="C211">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D211" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E211">
         <v>1</v>
@@ -15229,10 +15252,10 @@
         <v>182</v>
       </c>
       <c r="C212">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D212" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -15279,10 +15302,10 @@
         <v>182</v>
       </c>
       <c r="C213">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D213" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E213">
         <v>1</v>
@@ -15329,10 +15352,10 @@
         <v>182</v>
       </c>
       <c r="C214">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D214" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -15379,10 +15402,10 @@
         <v>182</v>
       </c>
       <c r="C215">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D215" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E215">
         <v>1</v>
@@ -15423,16 +15446,16 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B216" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C216">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D216" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -15479,10 +15502,10 @@
         <v>183</v>
       </c>
       <c r="C217">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D217" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E217">
         <v>1</v>
@@ -15529,10 +15552,10 @@
         <v>183</v>
       </c>
       <c r="C218">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D218" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -15573,16 +15596,16 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B219" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C219">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D219" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E219">
         <v>1</v>
@@ -15615,7 +15638,7 @@
         <v>0</v>
       </c>
       <c r="O219">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P219">
         <v>0</v>
@@ -15629,10 +15652,10 @@
         <v>184</v>
       </c>
       <c r="C220">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D220" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -15665,7 +15688,7 @@
         <v>0</v>
       </c>
       <c r="O220">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P220">
         <v>0</v>
@@ -15679,10 +15702,10 @@
         <v>184</v>
       </c>
       <c r="C221">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D221" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -15703,7 +15726,7 @@
         <v>0</v>
       </c>
       <c r="K221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L221">
         <v>0</v>
@@ -15729,10 +15752,10 @@
         <v>184</v>
       </c>
       <c r="C222">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D222" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -15753,7 +15776,7 @@
         <v>0</v>
       </c>
       <c r="K222">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L222">
         <v>0</v>
@@ -15779,10 +15802,10 @@
         <v>184</v>
       </c>
       <c r="C223">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D223" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E223">
         <v>1</v>
@@ -15815,7 +15838,7 @@
         <v>0</v>
       </c>
       <c r="O223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P223">
         <v>0</v>
@@ -15823,10 +15846,10 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B224" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C224">
         <v>42</v>
@@ -15847,7 +15870,7 @@
         <v>1</v>
       </c>
       <c r="I224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J224">
         <v>0</v>
@@ -15865,7 +15888,7 @@
         <v>0</v>
       </c>
       <c r="O224">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P224">
         <v>0</v>
@@ -15873,16 +15896,16 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B225" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C225">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D225" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -15897,7 +15920,7 @@
         <v>1</v>
       </c>
       <c r="I225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J225">
         <v>0</v>
@@ -15915,7 +15938,7 @@
         <v>0</v>
       </c>
       <c r="O225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P225">
         <v>0</v>
@@ -15929,10 +15952,10 @@
         <v>186</v>
       </c>
       <c r="C226">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D226" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -15973,16 +15996,16 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B227" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C227">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D227" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -16015,7 +16038,7 @@
         <v>0</v>
       </c>
       <c r="O227">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P227">
         <v>0</v>
@@ -16029,10 +16052,10 @@
         <v>187</v>
       </c>
       <c r="C228">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D228" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -16079,10 +16102,10 @@
         <v>187</v>
       </c>
       <c r="C229">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D229" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -16129,10 +16152,10 @@
         <v>187</v>
       </c>
       <c r="C230">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D230" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -16179,10 +16202,10 @@
         <v>187</v>
       </c>
       <c r="C231">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D231" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -16229,10 +16252,10 @@
         <v>187</v>
       </c>
       <c r="C232">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D232" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -16265,7 +16288,7 @@
         <v>0</v>
       </c>
       <c r="O232">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P232">
         <v>0</v>
@@ -16273,16 +16296,16 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B233" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C233">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D233" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -16303,10 +16326,10 @@
         <v>0</v>
       </c>
       <c r="K233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M233">
         <v>0</v>
@@ -16315,7 +16338,7 @@
         <v>0</v>
       </c>
       <c r="O233">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P233">
         <v>0</v>
@@ -16329,10 +16352,10 @@
         <v>188</v>
       </c>
       <c r="C234">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D234" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -16379,10 +16402,10 @@
         <v>188</v>
       </c>
       <c r="C235">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D235" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E235">
         <v>1</v>
@@ -16423,10 +16446,10 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B236" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C236">
         <v>42</v>
@@ -16468,21 +16491,21 @@
         <v>0</v>
       </c>
       <c r="P236">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B237" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C237">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D237" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -16518,7 +16541,7 @@
         <v>0</v>
       </c>
       <c r="P237">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
@@ -16529,10 +16552,10 @@
         <v>189</v>
       </c>
       <c r="C238">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D238" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -16579,10 +16602,10 @@
         <v>189</v>
       </c>
       <c r="C239">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D239" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -16629,10 +16652,10 @@
         <v>189</v>
       </c>
       <c r="C240">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D240" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -16679,10 +16702,10 @@
         <v>189</v>
       </c>
       <c r="C241">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D241" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -16729,10 +16752,10 @@
         <v>189</v>
       </c>
       <c r="C242">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D242" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -16779,10 +16802,10 @@
         <v>189</v>
       </c>
       <c r="C243">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D243" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -16829,10 +16852,10 @@
         <v>189</v>
       </c>
       <c r="C244">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D244" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -16873,10 +16896,10 @@
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B245" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C245">
         <v>42</v>
@@ -16894,7 +16917,7 @@
         <v>1</v>
       </c>
       <c r="H245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I245">
         <v>1</v>
@@ -16923,16 +16946,16 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B246" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C246">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D246" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -16944,7 +16967,7 @@
         <v>1</v>
       </c>
       <c r="H246">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I246">
         <v>1</v>
@@ -16979,10 +17002,10 @@
         <v>191</v>
       </c>
       <c r="C247">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D247" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -17029,10 +17052,10 @@
         <v>191</v>
       </c>
       <c r="C248">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D248" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -17079,10 +17102,10 @@
         <v>191</v>
       </c>
       <c r="C249">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D249" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -17129,10 +17152,10 @@
         <v>191</v>
       </c>
       <c r="C250">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D250" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -17173,16 +17196,16 @@
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B251" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C251">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D251" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -17229,10 +17252,10 @@
         <v>192</v>
       </c>
       <c r="C252">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D252" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -17279,10 +17302,10 @@
         <v>192</v>
       </c>
       <c r="C253">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D253" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -17329,10 +17352,10 @@
         <v>192</v>
       </c>
       <c r="C254">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D254" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -17373,16 +17396,16 @@
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B255" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C255">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D255" t="s">
-        <v>353</v>
+        <v>206</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -17429,10 +17452,10 @@
         <v>193</v>
       </c>
       <c r="C256">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D256" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -17479,10 +17502,10 @@
         <v>193</v>
       </c>
       <c r="C257">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D257" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -17529,10 +17552,10 @@
         <v>193</v>
       </c>
       <c r="C258">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D258" t="s">
-        <v>114</v>
+        <v>355</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -17579,10 +17602,10 @@
         <v>193</v>
       </c>
       <c r="C259">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D259" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -17629,10 +17652,10 @@
         <v>193</v>
       </c>
       <c r="C260">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D260" t="s">
-        <v>356</v>
+        <v>116</v>
       </c>
       <c r="E260">
         <v>1</v>
@@ -17679,10 +17702,10 @@
         <v>193</v>
       </c>
       <c r="C261">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D261" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E261">
         <v>1</v>
@@ -17729,10 +17752,10 @@
         <v>193</v>
       </c>
       <c r="C262">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D262" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E262">
         <v>1</v>
@@ -17779,10 +17802,10 @@
         <v>193</v>
       </c>
       <c r="C263">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D263" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -17829,10 +17852,10 @@
         <v>193</v>
       </c>
       <c r="C264">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D264" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E264">
         <v>1</v>
@@ -17879,10 +17902,10 @@
         <v>193</v>
       </c>
       <c r="C265">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D265" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -17929,10 +17952,10 @@
         <v>193</v>
       </c>
       <c r="C266">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D266" t="s">
-        <v>206</v>
+        <v>361</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -17973,16 +17996,16 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B267" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C267">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D267" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -18029,10 +18052,10 @@
         <v>181</v>
       </c>
       <c r="C268">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D268" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -18079,10 +18102,10 @@
         <v>181</v>
       </c>
       <c r="C269">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D269" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -18123,16 +18146,16 @@
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B270" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C270">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D270" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E270">
         <v>1</v>
@@ -18153,10 +18176,10 @@
         <v>0</v>
       </c>
       <c r="K270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L270">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M270">
         <v>0</v>
@@ -18165,7 +18188,7 @@
         <v>0</v>
       </c>
       <c r="O270">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P270">
         <v>0</v>
@@ -18173,16 +18196,16 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B271" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C271">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="D271" t="s">
-        <v>645</v>
+        <v>220</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -18203,7 +18226,7 @@
         <v>0</v>
       </c>
       <c r="K271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L271">
         <v>0</v>
@@ -18215,10 +18238,10 @@
         <v>0</v>
       </c>
       <c r="O271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P271">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.25">
@@ -18229,10 +18252,10 @@
         <v>172</v>
       </c>
       <c r="C272">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D272" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -18279,10 +18302,10 @@
         <v>172</v>
       </c>
       <c r="C273">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D273" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -18323,16 +18346,16 @@
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B274" t="s">
-        <v>574</v>
+        <v>172</v>
       </c>
       <c r="C274">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="D274" t="s">
-        <v>649</v>
+        <v>689</v>
       </c>
       <c r="E274">
         <v>1</v>
@@ -18379,10 +18402,10 @@
         <v>574</v>
       </c>
       <c r="C275">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D275" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -18429,10 +18452,10 @@
         <v>574</v>
       </c>
       <c r="C276">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D276" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -18479,10 +18502,10 @@
         <v>574</v>
       </c>
       <c r="C277">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D277" t="s">
-        <v>206</v>
+        <v>651</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -18523,16 +18546,16 @@
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B278" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C278">
-        <v>182</v>
+        <v>42</v>
       </c>
       <c r="D278" t="s">
-        <v>643</v>
+        <v>206</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -18579,10 +18602,10 @@
         <v>575</v>
       </c>
       <c r="C279">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D279" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -18629,10 +18652,10 @@
         <v>575</v>
       </c>
       <c r="C280">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D280" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="E280">
         <v>1</v>
@@ -18679,10 +18702,10 @@
         <v>575</v>
       </c>
       <c r="C281">
-        <v>42</v>
+        <v>213</v>
       </c>
       <c r="D281" t="s">
-        <v>206</v>
+        <v>674</v>
       </c>
       <c r="E281">
         <v>1</v>
@@ -18723,16 +18746,16 @@
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282">
+        <v>41</v>
+      </c>
+      <c r="B282" t="s">
+        <v>575</v>
+      </c>
+      <c r="C282">
         <v>42</v>
       </c>
-      <c r="B282" t="s">
-        <v>576</v>
-      </c>
-      <c r="C282">
-        <v>156</v>
-      </c>
       <c r="D282" t="s">
-        <v>617</v>
+        <v>206</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -18779,10 +18802,10 @@
         <v>576</v>
       </c>
       <c r="C283">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D283" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -18829,10 +18852,10 @@
         <v>576</v>
       </c>
       <c r="C284">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D284" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="E284">
         <v>1</v>
@@ -18879,10 +18902,10 @@
         <v>576</v>
       </c>
       <c r="C285">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="D285" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
       <c r="E285">
         <v>1</v>
@@ -18929,10 +18952,10 @@
         <v>576</v>
       </c>
       <c r="C286">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D286" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="E286">
         <v>1</v>
@@ -18979,10 +19002,10 @@
         <v>576</v>
       </c>
       <c r="C287">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D287" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="E287">
         <v>1</v>
@@ -19029,10 +19052,10 @@
         <v>576</v>
       </c>
       <c r="C288">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="D288" t="s">
-        <v>206</v>
+        <v>690</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -19073,16 +19096,16 @@
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B289" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C289">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="D289" t="s">
-        <v>611</v>
+        <v>206</v>
       </c>
       <c r="E289">
         <v>1</v>
@@ -19129,10 +19152,10 @@
         <v>577</v>
       </c>
       <c r="C290">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="D290" t="s">
-        <v>206</v>
+        <v>611</v>
       </c>
       <c r="E290">
         <v>1</v>
@@ -19173,16 +19196,16 @@
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B291" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C291">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="D291" t="s">
-        <v>590</v>
+        <v>206</v>
       </c>
       <c r="E291">
         <v>1</v>
@@ -19229,10 +19252,10 @@
         <v>578</v>
       </c>
       <c r="C292">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D292" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="E292">
         <v>1</v>
@@ -19279,45 +19302,95 @@
         <v>578</v>
       </c>
       <c r="C293">
+        <v>152</v>
+      </c>
+      <c r="D293" t="s">
+        <v>613</v>
+      </c>
+      <c r="E293">
+        <v>1</v>
+      </c>
+      <c r="F293">
+        <v>1</v>
+      </c>
+      <c r="G293">
+        <v>1</v>
+      </c>
+      <c r="H293">
+        <v>1</v>
+      </c>
+      <c r="I293">
+        <v>1</v>
+      </c>
+      <c r="J293">
+        <v>0</v>
+      </c>
+      <c r="K293">
+        <v>0</v>
+      </c>
+      <c r="L293">
+        <v>0</v>
+      </c>
+      <c r="M293">
+        <v>0</v>
+      </c>
+      <c r="N293">
+        <v>0</v>
+      </c>
+      <c r="O293">
+        <v>0</v>
+      </c>
+      <c r="P293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>44</v>
+      </c>
+      <c r="B294" t="s">
+        <v>578</v>
+      </c>
+      <c r="C294">
         <v>154</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D294" t="s">
         <v>615</v>
       </c>
-      <c r="E293">
-        <v>1</v>
-      </c>
-      <c r="F293">
-        <v>1</v>
-      </c>
-      <c r="G293">
-        <v>1</v>
-      </c>
-      <c r="H293">
-        <v>1</v>
-      </c>
-      <c r="I293">
-        <v>1</v>
-      </c>
-      <c r="J293">
-        <v>0</v>
-      </c>
-      <c r="K293">
-        <v>0</v>
-      </c>
-      <c r="L293">
-        <v>0</v>
-      </c>
-      <c r="M293">
-        <v>0</v>
-      </c>
-      <c r="N293">
-        <v>0</v>
-      </c>
-      <c r="O293">
-        <v>0</v>
-      </c>
-      <c r="P293">
+      <c r="E294">
+        <v>1</v>
+      </c>
+      <c r="F294">
+        <v>1</v>
+      </c>
+      <c r="G294">
+        <v>1</v>
+      </c>
+      <c r="H294">
+        <v>1</v>
+      </c>
+      <c r="I294">
+        <v>1</v>
+      </c>
+      <c r="J294">
+        <v>0</v>
+      </c>
+      <c r="K294">
+        <v>0</v>
+      </c>
+      <c r="L294">
+        <v>0</v>
+      </c>
+      <c r="M294">
+        <v>0</v>
+      </c>
+      <c r="N294">
+        <v>0</v>
+      </c>
+      <c r="O294">
+        <v>0</v>
+      </c>
+      <c r="P294">
         <v>1</v>
       </c>
     </row>
@@ -29210,9 +29283,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B233"/>
+  <dimension ref="A1:B234"/>
   <sheetViews>
-    <sheetView topLeftCell="A191" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B234"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31082,6 +31157,14 @@
       </c>
       <c r="B233" t="s">
         <v>750</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>232</v>
+      </c>
+      <c r="B234" t="s">
+        <v>763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 34. TFS 1555
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33659
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3041" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="771">
   <si>
     <t>SourceID</t>
   </si>
@@ -2331,6 +2331,27 @@
   </si>
   <si>
     <t>Short Duration Reporting</t>
+  </si>
+  <si>
+    <t>Added additional job codes for LSA Module in Employee_Selection and Module_Submission tabs</t>
+  </si>
+  <si>
+    <t>WIHD40</t>
+  </si>
+  <si>
+    <t>Supervisor, Help Desk</t>
+  </si>
+  <si>
+    <t>WIHD50</t>
+  </si>
+  <si>
+    <t>Manager, Help Desk</t>
+  </si>
+  <si>
+    <t>WABA11</t>
+  </si>
+  <si>
+    <t>Assoc Administrator, Business</t>
   </si>
 </sst>
 </file>
@@ -2692,9 +2713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3331,6 +3354,23 @@
         <v>762</v>
       </c>
     </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1">
+        <v>42370</v>
+      </c>
+      <c r="C38" t="s">
+        <v>434</v>
+      </c>
+      <c r="D38">
+        <v>1555</v>
+      </c>
+      <c r="E38" t="s">
+        <v>764</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3339,9 +3379,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4552,13 +4592,13 @@
         <v>1</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -4608,6 +4648,75 @@
       </c>
       <c r="G55">
         <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>765</v>
+      </c>
+      <c r="B56" t="s">
+        <v>766</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>767</v>
+      </c>
+      <c r="B57" t="s">
+        <v>768</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>769</v>
+      </c>
+      <c r="B58" t="s">
+        <v>770</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>1</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -28507,7 +28616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31873,7 +31984,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -32037,7 +32148,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -32268,6 +32379,98 @@
       </c>
       <c r="G17">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>327</v>
+      </c>
+      <c r="B18" t="s">
+        <v>328</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>765</v>
+      </c>
+      <c r="B19" t="s">
+        <v>766</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>767</v>
+      </c>
+      <c r="B20" t="s">
+        <v>768</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>769</v>
+      </c>
+      <c r="B21" t="s">
+        <v>770</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 35. TFS 1555
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33664
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="772">
   <si>
     <t>SourceID</t>
   </si>
@@ -2352,6 +2352,9 @@
   </si>
   <si>
     <t>Assoc Administrator, Business</t>
+  </si>
+  <si>
+    <t>Upadted to remove newly added LSA job codes from internal version 34 from Employee_Selection tab</t>
   </si>
 </sst>
 </file>
@@ -2713,11 +2716,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3369,6 +3370,23 @@
       </c>
       <c r="E38" t="s">
         <v>764</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1">
+        <v>42370</v>
+      </c>
+      <c r="C39" t="s">
+        <v>434</v>
+      </c>
+      <c r="D39">
+        <v>1555</v>
+      </c>
+      <c r="E39" t="s">
+        <v>771</v>
       </c>
     </row>
   </sheetData>
@@ -31984,9 +32002,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -32404,75 +32424,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>765</v>
-      </c>
-      <c r="B19" t="s">
-        <v>766</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>767</v>
-      </c>
-      <c r="B20" t="s">
-        <v>768</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>769</v>
-      </c>
-      <c r="B21" t="s">
-        <v>770</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Survey Questions text for TFS 2249
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34058
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -24,7 +24,7 @@
     <sheet name="ETS_Description" sheetId="15" r:id="rId15"/>
     <sheet name="DIM_Behavior" sheetId="16" r:id="rId16"/>
     <sheet name="Survey_DIM_Type" sheetId="17" r:id="rId17"/>
-    <sheet name="Sirvey_DIM_Question" sheetId="18" r:id="rId18"/>
+    <sheet name="Survey_DIM_Question" sheetId="18" r:id="rId18"/>
     <sheet name="Survey_DIM_Response" sheetId="19" r:id="rId19"/>
     <sheet name="Survey_DIM_QAnswer" sheetId="20" r:id="rId20"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="773">
   <si>
     <t>SourceID</t>
   </si>
@@ -2300,9 +2300,6 @@
     <t>Was the call played back for you during your last coaching session? (If applicable). |     If no, what reason was provided?</t>
   </si>
   <si>
-    <t>Will you be able to apply the information from your last coaching session? |    If yes, how?  If no, why  not?</t>
-  </si>
-  <si>
     <t>Please rate the effectiveness of the coaching notes provided in the eCL. |   Please explain below.</t>
   </si>
   <si>
@@ -2312,9 +2309,6 @@
     <t>Not Applicable</t>
   </si>
   <si>
-    <t>Did you find the coaching session valuable/effective? |   If yes, what specifically.  If no, why not?</t>
-  </si>
-  <si>
     <t>Enable sup module submissions for job code WACQ13. Updated Module_submission tab.</t>
   </si>
   <si>
@@ -2354,7 +2348,16 @@
     <t>Assoc Administrator, Business</t>
   </si>
   <si>
-    <t>Upadted to remove newly added LSA job codes from internal version 34 from Employee_Selection tab</t>
+    <t>Will you be able to apply the information from your last coaching session? |    If yes, how? If no, what suggestions or recommendations could have made it more useful for you?</t>
+  </si>
+  <si>
+    <t>Did you find the coaching session valuable/effective? |   If yes, what specifically? If no, what could have made it more effective or valuable?</t>
+  </si>
+  <si>
+    <t>Updated to remove newly added LSA job codes from internal version 34 from Employee_Selection tab</t>
+  </si>
+  <si>
+    <t>Updated Survey Question text for Qn Ids 2 and 3 in tab Survey_DIM_Question</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2719,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3301,7 +3304,7 @@
         <v>841</v>
       </c>
       <c r="E34" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,7 +3321,7 @@
         <v>861</v>
       </c>
       <c r="E35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3335,7 +3338,7 @@
         <v>1013</v>
       </c>
       <c r="E36" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,7 +3355,7 @@
         <v>1016</v>
       </c>
       <c r="E37" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3369,7 +3372,7 @@
         <v>1555</v>
       </c>
       <c r="E38" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,6 +3390,23 @@
       </c>
       <c r="E39" t="s">
         <v>771</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1">
+        <v>42450</v>
+      </c>
+      <c r="C40" t="s">
+        <v>434</v>
+      </c>
+      <c r="D40">
+        <v>2249</v>
+      </c>
+      <c r="E40" t="s">
+        <v>772</v>
       </c>
     </row>
   </sheetData>
@@ -4670,10 +4690,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B56" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4693,10 +4713,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B57" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4716,10 +4736,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="B58" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -12382,7 +12402,7 @@
         <v>232</v>
       </c>
       <c r="D152" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -21051,7 +21071,7 @@
         <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -21086,7 +21106,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -25560,12 +25580,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="119.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="169.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -25655,7 +25677,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>753</v>
+        <v>769</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -25681,7 +25703,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>757</v>
+        <v>770</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -25707,7 +25729,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -25733,7 +25755,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -25793,7 +25815,7 @@
         <v>-1</v>
       </c>
       <c r="B2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -26953,7 +26975,7 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -27852,7 +27874,7 @@
         <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -31293,7 +31315,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 37. Updates for TFS 2283.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34095
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3060" uniqueCount="775">
   <si>
     <t>SourceID</t>
   </si>
@@ -2358,6 +2358,12 @@
   </si>
   <si>
     <t>Updated Survey Question text for Qn Ids 2 and 3 in tab Survey_DIM_Question</t>
+  </si>
+  <si>
+    <t>Overdue Training</t>
+  </si>
+  <si>
+    <t>Updated DIM_Sub_Coaching_Reason and Coaching_Reason_Selection tables to add rows for Overdue Training.</t>
   </si>
 </sst>
 </file>
@@ -2719,7 +2725,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3407,6 +3413,23 @@
       </c>
       <c r="E40" t="s">
         <v>772</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" s="1">
+        <v>42454</v>
+      </c>
+      <c r="C41" t="s">
+        <v>434</v>
+      </c>
+      <c r="D41">
+        <v>2283</v>
+      </c>
+      <c r="E41" t="s">
+        <v>774</v>
       </c>
     </row>
   </sheetData>
@@ -4832,9 +4855,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P294"/>
+  <dimension ref="A1:P295"/>
   <sheetViews>
-    <sheetView topLeftCell="A252" workbookViewId="0"/>
+    <sheetView topLeftCell="A254" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12443,19 +12466,19 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="B153" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="C153">
-        <v>-1</v>
+        <v>233</v>
       </c>
       <c r="D153" t="s">
-        <v>4</v>
+        <v>773</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F153">
         <v>0</v>
@@ -12470,7 +12493,7 @@
         <v>1</v>
       </c>
       <c r="J153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -12493,25 +12516,25 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B154" t="s">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="C154">
-        <v>42</v>
+        <v>-1</v>
       </c>
       <c r="D154" t="s">
-        <v>206</v>
+        <v>4</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H154">
         <v>1</v>
@@ -12520,13 +12543,13 @@
         <v>1</v>
       </c>
       <c r="J154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K154">
         <v>0</v>
       </c>
       <c r="L154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M154">
         <v>0</v>
@@ -12543,16 +12566,16 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B155" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C155">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D155" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -12576,7 +12599,7 @@
         <v>0</v>
       </c>
       <c r="L155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M155">
         <v>0</v>
@@ -12599,10 +12622,10 @@
         <v>85</v>
       </c>
       <c r="C156">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D156" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -12649,10 +12672,10 @@
         <v>85</v>
       </c>
       <c r="C157">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D157" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -12699,10 +12722,10 @@
         <v>85</v>
       </c>
       <c r="C158">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D158" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -12749,10 +12772,10 @@
         <v>85</v>
       </c>
       <c r="C159">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D159" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -12799,10 +12822,10 @@
         <v>85</v>
       </c>
       <c r="C160">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D160" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -12849,10 +12872,10 @@
         <v>85</v>
       </c>
       <c r="C161">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D161" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -12899,10 +12922,10 @@
         <v>85</v>
       </c>
       <c r="C162">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D162" t="s">
-        <v>206</v>
+        <v>113</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -12943,16 +12966,16 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B163" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C163">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D163" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -12961,7 +12984,7 @@
         <v>1</v>
       </c>
       <c r="G163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H163">
         <v>1</v>
@@ -12999,10 +13022,10 @@
         <v>86</v>
       </c>
       <c r="C164">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D164" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -13011,7 +13034,7 @@
         <v>1</v>
       </c>
       <c r="G164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H164">
         <v>1</v>
@@ -13023,10 +13046,10 @@
         <v>1</v>
       </c>
       <c r="K164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M164">
         <v>0</v>
@@ -13035,24 +13058,24 @@
         <v>0</v>
       </c>
       <c r="O164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B165" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="C165">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="D165" t="s">
-        <v>98</v>
+        <v>206</v>
       </c>
       <c r="E165">
         <v>1</v>
@@ -13073,7 +13096,7 @@
         <v>1</v>
       </c>
       <c r="K165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L165">
         <v>1</v>
@@ -13085,10 +13108,10 @@
         <v>0</v>
       </c>
       <c r="O165">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P165">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
@@ -13099,10 +13122,10 @@
         <v>181</v>
       </c>
       <c r="C166">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D166" t="s">
-        <v>206</v>
+        <v>98</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -13143,10 +13166,10 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B167" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
       <c r="C167">
         <v>42</v>
@@ -13176,7 +13199,7 @@
         <v>0</v>
       </c>
       <c r="L167">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M167">
         <v>0</v>
@@ -13193,16 +13216,16 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B168" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C168">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="D168" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -13217,7 +13240,7 @@
         <v>1</v>
       </c>
       <c r="I168">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J168">
         <v>1</v>
@@ -13226,13 +13249,13 @@
         <v>0</v>
       </c>
       <c r="L168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M168">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N168">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O168">
         <v>0</v>
@@ -13249,10 +13272,10 @@
         <v>88</v>
       </c>
       <c r="C169">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="D169" t="s">
-        <v>344</v>
+        <v>100</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -13299,10 +13322,10 @@
         <v>88</v>
       </c>
       <c r="C170">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="D170" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -13326,7 +13349,7 @@
         <v>0</v>
       </c>
       <c r="L170">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M170">
         <v>1</v>
@@ -13349,10 +13372,10 @@
         <v>88</v>
       </c>
       <c r="C171">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D171" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -13376,7 +13399,7 @@
         <v>0</v>
       </c>
       <c r="L171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M171">
         <v>1</v>
@@ -13399,10 +13422,10 @@
         <v>88</v>
       </c>
       <c r="C172">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D172" t="s">
-        <v>103</v>
+        <v>346</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -13449,10 +13472,10 @@
         <v>88</v>
       </c>
       <c r="C173">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D173" t="s">
-        <v>347</v>
+        <v>103</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -13499,10 +13522,10 @@
         <v>88</v>
       </c>
       <c r="C174">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D174" t="s">
-        <v>105</v>
+        <v>347</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13549,10 +13572,10 @@
         <v>88</v>
       </c>
       <c r="C175">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D175" t="s">
-        <v>236</v>
+        <v>105</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13599,10 +13622,10 @@
         <v>88</v>
       </c>
       <c r="C176">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D176" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -13649,10 +13672,10 @@
         <v>88</v>
       </c>
       <c r="C177">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D177" t="s">
-        <v>101</v>
+        <v>237</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -13699,10 +13722,10 @@
         <v>88</v>
       </c>
       <c r="C178">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D178" t="s">
-        <v>206</v>
+        <v>101</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -13738,21 +13761,21 @@
         <v>0</v>
       </c>
       <c r="P178">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B179" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C179">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D179" t="s">
-        <v>106</v>
+        <v>206</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -13767,7 +13790,7 @@
         <v>1</v>
       </c>
       <c r="I179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J179">
         <v>1</v>
@@ -13776,19 +13799,19 @@
         <v>0</v>
       </c>
       <c r="L179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N179">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O179">
         <v>0</v>
       </c>
       <c r="P179">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
@@ -13799,10 +13822,10 @@
         <v>89</v>
       </c>
       <c r="C180">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D180" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -13843,10 +13866,10 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B181" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C181">
         <v>42</v>
@@ -13893,16 +13916,16 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B182" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C182">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D182" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -13949,10 +13972,10 @@
         <v>91</v>
       </c>
       <c r="C183">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D183" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -13999,10 +14022,10 @@
         <v>91</v>
       </c>
       <c r="C184">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D184" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -14049,10 +14072,10 @@
         <v>91</v>
       </c>
       <c r="C185">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D185" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -14099,10 +14122,10 @@
         <v>91</v>
       </c>
       <c r="C186">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D186" t="s">
-        <v>348</v>
+        <v>120</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -14149,10 +14172,10 @@
         <v>91</v>
       </c>
       <c r="C187">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D187" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -14199,10 +14222,10 @@
         <v>91</v>
       </c>
       <c r="C188">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D188" t="s">
-        <v>115</v>
+        <v>349</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -14249,10 +14272,10 @@
         <v>91</v>
       </c>
       <c r="C189">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D189" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -14299,10 +14322,10 @@
         <v>91</v>
       </c>
       <c r="C190">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D190" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -14320,7 +14343,7 @@
         <v>1</v>
       </c>
       <c r="J190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K190">
         <v>0</v>
@@ -14349,10 +14372,10 @@
         <v>91</v>
       </c>
       <c r="C191">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D191" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -14370,7 +14393,7 @@
         <v>1</v>
       </c>
       <c r="J191">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K191">
         <v>0</v>
@@ -14399,10 +14422,10 @@
         <v>91</v>
       </c>
       <c r="C192">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D192" t="s">
-        <v>350</v>
+        <v>116</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -14449,10 +14472,10 @@
         <v>91</v>
       </c>
       <c r="C193">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D193" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -14499,10 +14522,10 @@
         <v>91</v>
       </c>
       <c r="C194">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D194" t="s">
-        <v>206</v>
+        <v>351</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -14543,16 +14566,16 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B195" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C195">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D195" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -14599,10 +14622,10 @@
         <v>92</v>
       </c>
       <c r="C196">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D196" t="s">
-        <v>352</v>
+        <v>140</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -14649,10 +14672,10 @@
         <v>92</v>
       </c>
       <c r="C197">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="D197" t="s">
-        <v>19</v>
+        <v>352</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -14699,10 +14722,10 @@
         <v>92</v>
       </c>
       <c r="C198">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D198" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -14749,10 +14772,10 @@
         <v>92</v>
       </c>
       <c r="C199">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D199" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -14799,10 +14822,10 @@
         <v>92</v>
       </c>
       <c r="C200">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D200" t="s">
-        <v>206</v>
+        <v>138</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -14835,7 +14858,7 @@
         <v>0</v>
       </c>
       <c r="O200">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P200">
         <v>0</v>
@@ -14843,10 +14866,10 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B201" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C201">
         <v>42</v>
@@ -14864,7 +14887,7 @@
         <v>1</v>
       </c>
       <c r="H201">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I201">
         <v>1</v>
@@ -14873,7 +14896,7 @@
         <v>1</v>
       </c>
       <c r="K201">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L201">
         <v>0</v>
@@ -14888,7 +14911,7 @@
         <v>1</v>
       </c>
       <c r="P201">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
@@ -14899,10 +14922,10 @@
         <v>93</v>
       </c>
       <c r="C202">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D202" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -14920,7 +14943,7 @@
         <v>1</v>
       </c>
       <c r="J202">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K202">
         <v>1</v>
@@ -14938,7 +14961,7 @@
         <v>1</v>
       </c>
       <c r="P202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
@@ -14949,10 +14972,10 @@
         <v>93</v>
       </c>
       <c r="C203">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D203" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -14985,7 +15008,7 @@
         <v>0</v>
       </c>
       <c r="O203">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P203">
         <v>0</v>
@@ -14993,16 +15016,16 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B204" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C204">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D204" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E204">
         <v>1</v>
@@ -15014,19 +15037,19 @@
         <v>1</v>
       </c>
       <c r="H204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I204">
         <v>1</v>
       </c>
       <c r="J204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K204">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L204">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M204">
         <v>0</v>
@@ -15043,10 +15066,10 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B205" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C205">
         <v>42</v>
@@ -15073,10 +15096,10 @@
         <v>1</v>
       </c>
       <c r="K205">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L205">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M205">
         <v>0</v>
@@ -15085,24 +15108,24 @@
         <v>0</v>
       </c>
       <c r="O205">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P205">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B206" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="C206">
         <v>42</v>
       </c>
       <c r="D206" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="E206">
         <v>1</v>
@@ -15120,10 +15143,10 @@
         <v>1</v>
       </c>
       <c r="J206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L206">
         <v>0</v>
@@ -15135,24 +15158,24 @@
         <v>0</v>
       </c>
       <c r="O206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P206">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B207" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C207">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D207" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="E207">
         <v>1</v>
@@ -15173,7 +15196,7 @@
         <v>0</v>
       </c>
       <c r="K207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L207">
         <v>0</v>
@@ -15199,10 +15222,10 @@
         <v>182</v>
       </c>
       <c r="C208">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D208" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -15249,10 +15272,10 @@
         <v>182</v>
       </c>
       <c r="C209">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D209" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -15299,10 +15322,10 @@
         <v>182</v>
       </c>
       <c r="C210">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D210" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E210">
         <v>1</v>
@@ -15349,10 +15372,10 @@
         <v>182</v>
       </c>
       <c r="C211">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D211" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E211">
         <v>1</v>
@@ -15399,10 +15422,10 @@
         <v>182</v>
       </c>
       <c r="C212">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D212" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -15449,10 +15472,10 @@
         <v>182</v>
       </c>
       <c r="C213">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D213" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E213">
         <v>1</v>
@@ -15499,10 +15522,10 @@
         <v>182</v>
       </c>
       <c r="C214">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D214" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -15549,10 +15572,10 @@
         <v>182</v>
       </c>
       <c r="C215">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D215" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E215">
         <v>1</v>
@@ -15599,10 +15622,10 @@
         <v>182</v>
       </c>
       <c r="C216">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="D216" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -15643,16 +15666,16 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B217" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C217">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="D217" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E217">
         <v>1</v>
@@ -15699,10 +15722,10 @@
         <v>183</v>
       </c>
       <c r="C218">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D218" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -15749,10 +15772,10 @@
         <v>183</v>
       </c>
       <c r="C219">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D219" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E219">
         <v>1</v>
@@ -15793,16 +15816,16 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B220" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C220">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D220" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -15835,7 +15858,7 @@
         <v>0</v>
       </c>
       <c r="O220">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P220">
         <v>0</v>
@@ -15849,10 +15872,10 @@
         <v>184</v>
       </c>
       <c r="C221">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D221" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -15885,7 +15908,7 @@
         <v>0</v>
       </c>
       <c r="O221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P221">
         <v>0</v>
@@ -15899,10 +15922,10 @@
         <v>184</v>
       </c>
       <c r="C222">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D222" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -15923,7 +15946,7 @@
         <v>0</v>
       </c>
       <c r="K222">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L222">
         <v>0</v>
@@ -15949,10 +15972,10 @@
         <v>184</v>
       </c>
       <c r="C223">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D223" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="E223">
         <v>1</v>
@@ -15973,7 +15996,7 @@
         <v>0</v>
       </c>
       <c r="K223">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L223">
         <v>0</v>
@@ -15999,10 +16022,10 @@
         <v>184</v>
       </c>
       <c r="C224">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="D224" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -16035,7 +16058,7 @@
         <v>0</v>
       </c>
       <c r="O224">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P224">
         <v>0</v>
@@ -16043,10 +16066,10 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B225" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C225">
         <v>42</v>
@@ -16067,7 +16090,7 @@
         <v>1</v>
       </c>
       <c r="I225">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J225">
         <v>0</v>
@@ -16085,7 +16108,7 @@
         <v>0</v>
       </c>
       <c r="O225">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P225">
         <v>0</v>
@@ -16093,16 +16116,16 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B226" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C226">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D226" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -16117,7 +16140,7 @@
         <v>1</v>
       </c>
       <c r="I226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J226">
         <v>0</v>
@@ -16135,7 +16158,7 @@
         <v>0</v>
       </c>
       <c r="O226">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P226">
         <v>0</v>
@@ -16149,10 +16172,10 @@
         <v>186</v>
       </c>
       <c r="C227">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D227" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -16193,16 +16216,16 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B228" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C228">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="D228" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -16235,7 +16258,7 @@
         <v>0</v>
       </c>
       <c r="O228">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P228">
         <v>0</v>
@@ -16249,10 +16272,10 @@
         <v>187</v>
       </c>
       <c r="C229">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D229" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -16299,10 +16322,10 @@
         <v>187</v>
       </c>
       <c r="C230">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D230" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -16349,10 +16372,10 @@
         <v>187</v>
       </c>
       <c r="C231">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D231" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -16399,10 +16422,10 @@
         <v>187</v>
       </c>
       <c r="C232">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D232" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -16449,10 +16472,10 @@
         <v>187</v>
       </c>
       <c r="C233">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D233" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -16485,7 +16508,7 @@
         <v>0</v>
       </c>
       <c r="O233">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P233">
         <v>0</v>
@@ -16493,16 +16516,16 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B234" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C234">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D234" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -16523,10 +16546,10 @@
         <v>0</v>
       </c>
       <c r="K234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M234">
         <v>0</v>
@@ -16535,7 +16558,7 @@
         <v>0</v>
       </c>
       <c r="O234">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P234">
         <v>0</v>
@@ -16549,10 +16572,10 @@
         <v>188</v>
       </c>
       <c r="C235">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D235" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E235">
         <v>1</v>
@@ -16599,10 +16622,10 @@
         <v>188</v>
       </c>
       <c r="C236">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D236" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -16643,10 +16666,10 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B237" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="C237">
         <v>42</v>
@@ -16688,21 +16711,21 @@
         <v>0</v>
       </c>
       <c r="P237">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B238" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C238">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D238" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -16738,7 +16761,7 @@
         <v>0</v>
       </c>
       <c r="P238">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.25">
@@ -16749,10 +16772,10 @@
         <v>189</v>
       </c>
       <c r="C239">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D239" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -16799,10 +16822,10 @@
         <v>189</v>
       </c>
       <c r="C240">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D240" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -16849,10 +16872,10 @@
         <v>189</v>
       </c>
       <c r="C241">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D241" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -16899,10 +16922,10 @@
         <v>189</v>
       </c>
       <c r="C242">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D242" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -16949,10 +16972,10 @@
         <v>189</v>
       </c>
       <c r="C243">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D243" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -16999,10 +17022,10 @@
         <v>189</v>
       </c>
       <c r="C244">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D244" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -17049,10 +17072,10 @@
         <v>189</v>
       </c>
       <c r="C245">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D245" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -17093,10 +17116,10 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B246" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C246">
         <v>42</v>
@@ -17114,7 +17137,7 @@
         <v>1</v>
       </c>
       <c r="H246">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I246">
         <v>1</v>
@@ -17143,16 +17166,16 @@
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B247" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C247">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D247" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -17164,7 +17187,7 @@
         <v>1</v>
       </c>
       <c r="H247">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I247">
         <v>1</v>
@@ -17199,10 +17222,10 @@
         <v>191</v>
       </c>
       <c r="C248">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D248" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -17249,10 +17272,10 @@
         <v>191</v>
       </c>
       <c r="C249">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D249" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -17299,10 +17322,10 @@
         <v>191</v>
       </c>
       <c r="C250">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D250" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -17349,10 +17372,10 @@
         <v>191</v>
       </c>
       <c r="C251">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D251" t="s">
-        <v>206</v>
+        <v>229</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -17393,16 +17416,16 @@
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B252" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C252">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D252" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -17449,10 +17472,10 @@
         <v>192</v>
       </c>
       <c r="C253">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D253" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -17499,10 +17522,10 @@
         <v>192</v>
       </c>
       <c r="C254">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D254" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -17549,10 +17572,10 @@
         <v>192</v>
       </c>
       <c r="C255">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="D255" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -17593,16 +17616,16 @@
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B256" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C256">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D256" t="s">
-        <v>353</v>
+        <v>206</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -17649,10 +17672,10 @@
         <v>193</v>
       </c>
       <c r="C257">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D257" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -17699,10 +17722,10 @@
         <v>193</v>
       </c>
       <c r="C258">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D258" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -17749,10 +17772,10 @@
         <v>193</v>
       </c>
       <c r="C259">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D259" t="s">
-        <v>114</v>
+        <v>355</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -17799,10 +17822,10 @@
         <v>193</v>
       </c>
       <c r="C260">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D260" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E260">
         <v>1</v>
@@ -17849,10 +17872,10 @@
         <v>193</v>
       </c>
       <c r="C261">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D261" t="s">
-        <v>356</v>
+        <v>116</v>
       </c>
       <c r="E261">
         <v>1</v>
@@ -17899,10 +17922,10 @@
         <v>193</v>
       </c>
       <c r="C262">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D262" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E262">
         <v>1</v>
@@ -17949,10 +17972,10 @@
         <v>193</v>
       </c>
       <c r="C263">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D263" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -17999,10 +18022,10 @@
         <v>193</v>
       </c>
       <c r="C264">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D264" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E264">
         <v>1</v>
@@ -18049,10 +18072,10 @@
         <v>193</v>
       </c>
       <c r="C265">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D265" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -18099,10 +18122,10 @@
         <v>193</v>
       </c>
       <c r="C266">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D266" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -18149,10 +18172,10 @@
         <v>193</v>
       </c>
       <c r="C267">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D267" t="s">
-        <v>206</v>
+        <v>361</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -18193,16 +18216,16 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B268" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C268">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="D268" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -18249,10 +18272,10 @@
         <v>181</v>
       </c>
       <c r="C269">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D269" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -18299,10 +18322,10 @@
         <v>181</v>
       </c>
       <c r="C270">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D270" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E270">
         <v>1</v>
@@ -18343,16 +18366,16 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B271" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C271">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D271" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -18373,10 +18396,10 @@
         <v>0</v>
       </c>
       <c r="K271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L271">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M271">
         <v>0</v>
@@ -18385,7 +18408,7 @@
         <v>0</v>
       </c>
       <c r="O271">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P271">
         <v>0</v>
@@ -18393,16 +18416,16 @@
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B272" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C272">
-        <v>184</v>
+        <v>76</v>
       </c>
       <c r="D272" t="s">
-        <v>645</v>
+        <v>220</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -18423,7 +18446,7 @@
         <v>0</v>
       </c>
       <c r="K272">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L272">
         <v>0</v>
@@ -18435,10 +18458,10 @@
         <v>0</v>
       </c>
       <c r="O272">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P272">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.25">
@@ -18449,10 +18472,10 @@
         <v>172</v>
       </c>
       <c r="C273">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D273" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -18499,10 +18522,10 @@
         <v>172</v>
       </c>
       <c r="C274">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D274" t="s">
-        <v>689</v>
+        <v>658</v>
       </c>
       <c r="E274">
         <v>1</v>
@@ -18543,16 +18566,16 @@
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B275" t="s">
-        <v>574</v>
+        <v>172</v>
       </c>
       <c r="C275">
-        <v>188</v>
+        <v>228</v>
       </c>
       <c r="D275" t="s">
-        <v>649</v>
+        <v>689</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -18599,10 +18622,10 @@
         <v>574</v>
       </c>
       <c r="C276">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D276" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -18649,10 +18672,10 @@
         <v>574</v>
       </c>
       <c r="C277">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D277" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -18699,10 +18722,10 @@
         <v>574</v>
       </c>
       <c r="C278">
-        <v>42</v>
+        <v>190</v>
       </c>
       <c r="D278" t="s">
-        <v>206</v>
+        <v>651</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -18743,16 +18766,16 @@
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B279" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C279">
-        <v>182</v>
+        <v>42</v>
       </c>
       <c r="D279" t="s">
-        <v>643</v>
+        <v>206</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -18799,10 +18822,10 @@
         <v>575</v>
       </c>
       <c r="C280">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D280" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="E280">
         <v>1</v>
@@ -18849,10 +18872,10 @@
         <v>575</v>
       </c>
       <c r="C281">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D281" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="E281">
         <v>1</v>
@@ -18899,10 +18922,10 @@
         <v>575</v>
       </c>
       <c r="C282">
-        <v>42</v>
+        <v>213</v>
       </c>
       <c r="D282" t="s">
-        <v>206</v>
+        <v>674</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -18943,16 +18966,16 @@
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283">
+        <v>41</v>
+      </c>
+      <c r="B283" t="s">
+        <v>575</v>
+      </c>
+      <c r="C283">
         <v>42</v>
       </c>
-      <c r="B283" t="s">
-        <v>576</v>
-      </c>
-      <c r="C283">
-        <v>156</v>
-      </c>
       <c r="D283" t="s">
-        <v>617</v>
+        <v>206</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -18999,10 +19022,10 @@
         <v>576</v>
       </c>
       <c r="C284">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D284" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="E284">
         <v>1</v>
@@ -19049,10 +19072,10 @@
         <v>576</v>
       </c>
       <c r="C285">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="D285" t="s">
-        <v>641</v>
+        <v>621</v>
       </c>
       <c r="E285">
         <v>1</v>
@@ -19099,10 +19122,10 @@
         <v>576</v>
       </c>
       <c r="C286">
-        <v>211</v>
+        <v>180</v>
       </c>
       <c r="D286" t="s">
-        <v>672</v>
+        <v>641</v>
       </c>
       <c r="E286">
         <v>1</v>
@@ -19149,10 +19172,10 @@
         <v>576</v>
       </c>
       <c r="C287">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D287" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="E287">
         <v>1</v>
@@ -19199,10 +19222,10 @@
         <v>576</v>
       </c>
       <c r="C288">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="D288" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -19249,10 +19272,10 @@
         <v>576</v>
       </c>
       <c r="C289">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="D289" t="s">
-        <v>206</v>
+        <v>690</v>
       </c>
       <c r="E289">
         <v>1</v>
@@ -19293,16 +19316,16 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B290" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C290">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="D290" t="s">
-        <v>611</v>
+        <v>206</v>
       </c>
       <c r="E290">
         <v>1</v>
@@ -19349,10 +19372,10 @@
         <v>577</v>
       </c>
       <c r="C291">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="D291" t="s">
-        <v>206</v>
+        <v>611</v>
       </c>
       <c r="E291">
         <v>1</v>
@@ -19393,16 +19416,16 @@
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B292" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C292">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="D292" t="s">
-        <v>590</v>
+        <v>206</v>
       </c>
       <c r="E292">
         <v>1</v>
@@ -19449,10 +19472,10 @@
         <v>578</v>
       </c>
       <c r="C293">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D293" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="E293">
         <v>1</v>
@@ -19499,45 +19522,95 @@
         <v>578</v>
       </c>
       <c r="C294">
+        <v>152</v>
+      </c>
+      <c r="D294" t="s">
+        <v>613</v>
+      </c>
+      <c r="E294">
+        <v>1</v>
+      </c>
+      <c r="F294">
+        <v>1</v>
+      </c>
+      <c r="G294">
+        <v>1</v>
+      </c>
+      <c r="H294">
+        <v>1</v>
+      </c>
+      <c r="I294">
+        <v>1</v>
+      </c>
+      <c r="J294">
+        <v>0</v>
+      </c>
+      <c r="K294">
+        <v>0</v>
+      </c>
+      <c r="L294">
+        <v>0</v>
+      </c>
+      <c r="M294">
+        <v>0</v>
+      </c>
+      <c r="N294">
+        <v>0</v>
+      </c>
+      <c r="O294">
+        <v>0</v>
+      </c>
+      <c r="P294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>44</v>
+      </c>
+      <c r="B295" t="s">
+        <v>578</v>
+      </c>
+      <c r="C295">
         <v>154</v>
       </c>
-      <c r="D294" t="s">
+      <c r="D295" t="s">
         <v>615</v>
       </c>
-      <c r="E294">
-        <v>1</v>
-      </c>
-      <c r="F294">
-        <v>1</v>
-      </c>
-      <c r="G294">
-        <v>1</v>
-      </c>
-      <c r="H294">
-        <v>1</v>
-      </c>
-      <c r="I294">
-        <v>1</v>
-      </c>
-      <c r="J294">
-        <v>0</v>
-      </c>
-      <c r="K294">
-        <v>0</v>
-      </c>
-      <c r="L294">
-        <v>0</v>
-      </c>
-      <c r="M294">
-        <v>0</v>
-      </c>
-      <c r="N294">
-        <v>0</v>
-      </c>
-      <c r="O294">
-        <v>0</v>
-      </c>
-      <c r="P294">
+      <c r="E295">
+        <v>1</v>
+      </c>
+      <c r="F295">
+        <v>1</v>
+      </c>
+      <c r="G295">
+        <v>1</v>
+      </c>
+      <c r="H295">
+        <v>1</v>
+      </c>
+      <c r="I295">
+        <v>1</v>
+      </c>
+      <c r="J295">
+        <v>0</v>
+      </c>
+      <c r="K295">
+        <v>0</v>
+      </c>
+      <c r="L295">
+        <v>0</v>
+      </c>
+      <c r="M295">
+        <v>0</v>
+      </c>
+      <c r="N295">
+        <v>0</v>
+      </c>
+      <c r="O295">
+        <v>0</v>
+      </c>
+      <c r="P295">
         <v>1</v>
       </c>
     </row>
@@ -29434,10 +29507,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B234"/>
+  <dimension ref="A1:B235"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B234"/>
+      <selection sqref="A1:B235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31316,6 +31389,14 @@
       </c>
       <c r="B234" t="s">
         <v>761</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>233</v>
+      </c>
+      <c r="B235" t="s">
+        <v>773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Internal version 38. Updates for TFS 2332.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34300
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="22995" windowHeight="12840"/>
   </bookViews>
@@ -27,6 +32,7 @@
     <sheet name="Survey_DIM_Question" sheetId="18" r:id="rId18"/>
     <sheet name="Survey_DIM_Response" sheetId="19" r:id="rId19"/>
     <sheet name="Survey_DIM_QAnswer" sheetId="20" r:id="rId20"/>
+    <sheet name="HR_Access" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Coaching_Reason_Selection!$A$1:$P$292</definedName>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3060" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="801">
   <si>
     <t>SourceID</t>
   </si>
@@ -2364,6 +2370,84 @@
   </si>
   <si>
     <t>Updated DIM_Sub_Coaching_Reason and Coaching_Reason_Selection tables to add rows for Overdue Training.</t>
+  </si>
+  <si>
+    <t>Added new tab for HR_Access table to support table based HR access control</t>
+  </si>
+  <si>
+    <t>NewSubmissions</t>
+  </si>
+  <si>
+    <t>MyDashboard</t>
+  </si>
+  <si>
+    <t>MySubmissions</t>
+  </si>
+  <si>
+    <t>HistDashboard</t>
+  </si>
+  <si>
+    <t>DisplayWarnings</t>
+  </si>
+  <si>
+    <t>WHER12</t>
+  </si>
+  <si>
+    <t>Analyst, HR Compliance</t>
+  </si>
+  <si>
+    <t>WHER13</t>
+  </si>
+  <si>
+    <t>Sr Analyst, HR Compliance</t>
+  </si>
+  <si>
+    <t>WHER14</t>
+  </si>
+  <si>
+    <t>Princ Analyst, HR Compliance</t>
+  </si>
+  <si>
+    <t>WHHR02</t>
+  </si>
+  <si>
+    <t>Assistant, HR</t>
+  </si>
+  <si>
+    <t>WHHR12</t>
+  </si>
+  <si>
+    <t>Business Partner, HR</t>
+  </si>
+  <si>
+    <t>WHHR13</t>
+  </si>
+  <si>
+    <t>Sr Business Partner, HR</t>
+  </si>
+  <si>
+    <t>WHHR14</t>
+  </si>
+  <si>
+    <t>Principal Business Partner, HR</t>
+  </si>
+  <si>
+    <t>WHHR50</t>
+  </si>
+  <si>
+    <t>Manager, HR</t>
+  </si>
+  <si>
+    <t>WHHR60</t>
+  </si>
+  <si>
+    <t>Sr Manager, HR</t>
+  </si>
+  <si>
+    <t>WHHR70</t>
+  </si>
+  <si>
+    <t>Director, HR</t>
   </si>
 </sst>
 </file>
@@ -2434,6 +2518,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2481,7 +2568,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2516,7 +2603,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2725,7 +2812,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3430,6 +3517,23 @@
       </c>
       <c r="E41" t="s">
         <v>774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1">
+        <v>42475</v>
+      </c>
+      <c r="C42" t="s">
+        <v>434</v>
+      </c>
+      <c r="D42">
+        <v>2332</v>
+      </c>
+      <c r="E42" t="s">
+        <v>775</v>
       </c>
     </row>
   </sheetData>
@@ -28620,6 +28724,281 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D1" t="s">
+        <v>777</v>
+      </c>
+      <c r="E1" t="s">
+        <v>778</v>
+      </c>
+      <c r="F1" t="s">
+        <v>779</v>
+      </c>
+      <c r="G1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>783</v>
+      </c>
+      <c r="B3" t="s">
+        <v>784</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>785</v>
+      </c>
+      <c r="B4" t="s">
+        <v>786</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>787</v>
+      </c>
+      <c r="B5" t="s">
+        <v>788</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>789</v>
+      </c>
+      <c r="B6" t="s">
+        <v>790</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>791</v>
+      </c>
+      <c r="B7" t="s">
+        <v>792</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>793</v>
+      </c>
+      <c r="B8" t="s">
+        <v>794</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>795</v>
+      </c>
+      <c r="B9" t="s">
+        <v>796</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>797</v>
+      </c>
+      <c r="B10" t="s">
+        <v>798</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>799</v>
+      </c>
+      <c r="B11" t="s">
+        <v>800</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>

</xml_diff>

<commit_message>
Internal revision 41. TFS 2268.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34639
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="808">
   <si>
     <t>SourceID</t>
   </si>
@@ -2466,6 +2466,9 @@
   </si>
   <si>
     <t>OMR: Invalid use of Attestation</t>
+  </si>
+  <si>
+    <t>Added new record to Email notifications table to support Quality Other CTC feed</t>
   </si>
 </sst>
 </file>
@@ -2830,9 +2833,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3603,6 +3608,23 @@
       </c>
       <c r="E45" t="s">
         <v>805</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>41</v>
+      </c>
+      <c r="B46" s="1">
+        <v>42549</v>
+      </c>
+      <c r="C46" t="s">
+        <v>434</v>
+      </c>
+      <c r="D46">
+        <v>2268</v>
+      </c>
+      <c r="E46" t="s">
+        <v>807</v>
       </c>
     </row>
   </sheetData>
@@ -20072,9 +20094,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K159"/>
+  <dimension ref="A1:K160"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0"/>
+    <sheetView topLeftCell="A116" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21528,37 +21550,37 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B42" t="s">
-        <v>380</v>
+        <v>92</v>
       </c>
       <c r="C42" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>756</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G42" t="s">
-        <v>381</v>
+        <v>427</v>
       </c>
       <c r="H42" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="I42" t="s">
-        <v>381</v>
+        <v>475</v>
       </c>
       <c r="J42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" t="s">
-        <v>381</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -21575,19 +21597,19 @@
         <v>6</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H43" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I43" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -21607,7 +21629,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -21622,7 +21644,7 @@
         <v>383</v>
       </c>
       <c r="I44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -21642,7 +21664,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -21657,7 +21679,7 @@
         <v>383</v>
       </c>
       <c r="I45" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -21677,7 +21699,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -21692,7 +21714,7 @@
         <v>383</v>
       </c>
       <c r="I46" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -21712,7 +21734,7 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -21747,7 +21769,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -21782,7 +21804,7 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -21797,7 +21819,7 @@
         <v>383</v>
       </c>
       <c r="I49" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -21817,7 +21839,7 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -21832,7 +21854,7 @@
         <v>383</v>
       </c>
       <c r="I50" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -21852,7 +21874,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -21867,7 +21889,7 @@
         <v>383</v>
       </c>
       <c r="I51" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -21887,22 +21909,22 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>441</v>
+        <v>14</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G52" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H52" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I52" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -21913,7 +21935,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
         <v>380</v>
@@ -21948,7 +21970,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B54" t="s">
         <v>380</v>
@@ -21957,22 +21979,22 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>441</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H54" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I54" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -21992,22 +22014,22 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G55" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H55" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I55" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -22027,10 +22049,10 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="s">
         <v>177</v>
@@ -22039,10 +22061,10 @@
         <v>427</v>
       </c>
       <c r="H56" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -22062,7 +22084,7 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -22097,7 +22119,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -22112,7 +22134,7 @@
         <v>385</v>
       </c>
       <c r="I58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -22132,7 +22154,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -22147,7 +22169,7 @@
         <v>385</v>
       </c>
       <c r="I59" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -22167,7 +22189,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -22202,7 +22224,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -22237,7 +22259,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -22252,7 +22274,7 @@
         <v>385</v>
       </c>
       <c r="I62" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -22272,7 +22294,7 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -22287,7 +22309,7 @@
         <v>385</v>
       </c>
       <c r="I63" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -22307,7 +22329,7 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -22322,7 +22344,7 @@
         <v>385</v>
       </c>
       <c r="I64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -22342,7 +22364,7 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -22374,25 +22396,25 @@
         <v>380</v>
       </c>
       <c r="C66" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G66" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H66" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I66" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -22403,31 +22425,31 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
         <v>380</v>
       </c>
       <c r="C67" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
       <c r="G67" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H67" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I67" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -22447,7 +22469,7 @@
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -22462,7 +22484,7 @@
         <v>391</v>
       </c>
       <c r="I68" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -22482,7 +22504,7 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -22497,7 +22519,7 @@
         <v>391</v>
       </c>
       <c r="I69" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -22517,7 +22539,7 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -22552,7 +22574,7 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -22567,7 +22589,7 @@
         <v>391</v>
       </c>
       <c r="I71" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J71">
         <v>0</v>
@@ -22587,22 +22609,22 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G72" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H72" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I72" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -22622,7 +22644,7 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -22637,7 +22659,7 @@
         <v>385</v>
       </c>
       <c r="I73" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -22657,7 +22679,7 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -22672,7 +22694,7 @@
         <v>385</v>
       </c>
       <c r="I74" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -22692,7 +22714,7 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -22727,7 +22749,7 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -22759,25 +22781,25 @@
         <v>380</v>
       </c>
       <c r="C77" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G77" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H77" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I77" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J77">
         <v>0</v>
@@ -22788,7 +22810,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B78" t="s">
         <v>380</v>
@@ -22797,22 +22819,22 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G78" t="s">
         <v>175</v>
       </c>
       <c r="H78" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I78" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -22832,7 +22854,7 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -22867,7 +22889,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -22882,7 +22904,7 @@
         <v>386</v>
       </c>
       <c r="I80" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J80">
         <v>0</v>
@@ -22902,7 +22924,7 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -22917,7 +22939,7 @@
         <v>386</v>
       </c>
       <c r="I81" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -22937,7 +22959,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -22972,7 +22994,7 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -23007,7 +23029,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -23022,7 +23044,7 @@
         <v>386</v>
       </c>
       <c r="I84" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J84">
         <v>0</v>
@@ -23042,7 +23064,7 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -23057,7 +23079,7 @@
         <v>386</v>
       </c>
       <c r="I85" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -23077,7 +23099,7 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -23092,7 +23114,7 @@
         <v>386</v>
       </c>
       <c r="I86" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -23112,7 +23134,7 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -23127,7 +23149,7 @@
         <v>386</v>
       </c>
       <c r="I87" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -23147,22 +23169,22 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G88" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H88" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I88" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J88">
         <v>0</v>
@@ -23182,7 +23204,7 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -23197,7 +23219,7 @@
         <v>383</v>
       </c>
       <c r="I89" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J89">
         <v>0</v>
@@ -23208,31 +23230,31 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B90" t="s">
         <v>380</v>
       </c>
       <c r="C90" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D90" t="s">
         <v>7</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G90" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H90" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I90" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -23252,7 +23274,7 @@
         <v>5</v>
       </c>
       <c r="D91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -23287,7 +23309,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -23302,7 +23324,7 @@
         <v>385</v>
       </c>
       <c r="I92" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J92">
         <v>0</v>
@@ -23322,7 +23344,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -23337,7 +23359,7 @@
         <v>385</v>
       </c>
       <c r="I93" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="J93">
         <v>0</v>
@@ -23357,7 +23379,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -23392,7 +23414,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -23427,7 +23449,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -23442,7 +23464,7 @@
         <v>385</v>
       </c>
       <c r="I96" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J96">
         <v>0</v>
@@ -23462,7 +23484,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -23477,7 +23499,7 @@
         <v>385</v>
       </c>
       <c r="I97" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J97">
         <v>0</v>
@@ -23497,7 +23519,7 @@
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -23512,7 +23534,7 @@
         <v>385</v>
       </c>
       <c r="I98" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J98">
         <v>0</v>
@@ -23532,7 +23554,7 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -23564,25 +23586,25 @@
         <v>380</v>
       </c>
       <c r="C100" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G100" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H100" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I100" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J100">
         <v>0</v>
@@ -23602,7 +23624,7 @@
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -23637,7 +23659,7 @@
         <v>3</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -23652,7 +23674,7 @@
         <v>392</v>
       </c>
       <c r="I102" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J102">
         <v>0</v>
@@ -23663,7 +23685,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B103" t="s">
         <v>380</v>
@@ -23672,22 +23694,22 @@
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G103" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H103" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I103" t="s">
-        <v>406</v>
+        <v>425</v>
       </c>
       <c r="J103">
         <v>0</v>
@@ -23707,7 +23729,7 @@
         <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -23722,7 +23744,7 @@
         <v>383</v>
       </c>
       <c r="I104" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="J104">
         <v>0</v>
@@ -23742,7 +23764,7 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -23757,7 +23779,7 @@
         <v>383</v>
       </c>
       <c r="I105" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J105">
         <v>0</v>
@@ -23777,7 +23799,7 @@
         <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -23812,7 +23834,7 @@
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -23827,7 +23849,7 @@
         <v>383</v>
       </c>
       <c r="I107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J107">
         <v>0</v>
@@ -23847,7 +23869,7 @@
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -23862,7 +23884,7 @@
         <v>383</v>
       </c>
       <c r="I108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J108">
         <v>0</v>
@@ -23882,7 +23904,7 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -23897,7 +23919,7 @@
         <v>383</v>
       </c>
       <c r="I109" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="J109">
         <v>0</v>
@@ -23917,7 +23939,7 @@
         <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -23932,7 +23954,7 @@
         <v>383</v>
       </c>
       <c r="I110" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J110">
         <v>0</v>
@@ -23952,7 +23974,7 @@
         <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -23981,28 +24003,28 @@
         <v>174</v>
       </c>
       <c r="B112" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C112" t="s">
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G112" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H112" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I112" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J112">
         <v>0</v>
@@ -24016,28 +24038,28 @@
         <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>172</v>
+        <v>387</v>
       </c>
       <c r="C113" t="s">
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="F113" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G113" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H113" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I113" t="s">
-        <v>503</v>
+        <v>399</v>
       </c>
       <c r="J113">
         <v>0</v>
@@ -24048,7 +24070,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B114" t="s">
         <v>172</v>
@@ -24063,16 +24085,16 @@
         <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G114" t="s">
         <v>175</v>
       </c>
       <c r="H114" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I114" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J114">
         <v>0</v>
@@ -24083,31 +24105,31 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>481</v>
+        <v>175</v>
       </c>
       <c r="B115" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C115" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D115" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="E115">
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G115" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H115" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I115" t="s">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="J115">
         <v>0</v>
@@ -24127,7 +24149,7 @@
         <v>5</v>
       </c>
       <c r="D116" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E116">
         <v>0</v>
@@ -24162,7 +24184,7 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>491</v>
+        <v>12</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -24197,7 +24219,7 @@
         <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>170</v>
+        <v>491</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -24232,7 +24254,7 @@
         <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>493</v>
+        <v>170</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -24264,25 +24286,25 @@
         <v>380</v>
       </c>
       <c r="C120" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>8</v>
+        <v>493</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="F120" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G120" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H120" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I120" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J120">
         <v>0</v>
@@ -24302,7 +24324,7 @@
         <v>3</v>
       </c>
       <c r="D121" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E121">
         <v>0</v>
@@ -24337,7 +24359,7 @@
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>491</v>
+        <v>12</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -24372,7 +24394,7 @@
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>170</v>
+        <v>491</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -24407,7 +24429,7 @@
         <v>3</v>
       </c>
       <c r="D124" t="s">
-        <v>493</v>
+        <v>170</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -24433,31 +24455,31 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B125" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C125" t="s">
         <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>16</v>
+        <v>493</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="F125" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G125" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H125" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I125" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="J125">
         <v>0</v>
@@ -24483,16 +24505,16 @@
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G126" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H126" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I126" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="J126">
         <v>0</v>
@@ -24518,16 +24540,16 @@
         <v>0</v>
       </c>
       <c r="F127" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G127" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H127" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I127" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J127">
         <v>0</v>
@@ -24541,28 +24563,28 @@
         <v>174</v>
       </c>
       <c r="B128" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C128" t="s">
         <v>3</v>
       </c>
       <c r="D128" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E128">
         <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G128" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H128" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I128" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -24588,16 +24610,16 @@
         <v>0</v>
       </c>
       <c r="F129" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G129" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H129" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I129" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J129">
         <v>0</v>
@@ -24620,19 +24642,19 @@
         <v>15</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F130" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G130" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H130" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I130" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J130">
         <v>0</v>
@@ -24643,31 +24665,31 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B131" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C131" t="s">
         <v>3</v>
       </c>
       <c r="D131" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F131" t="s">
         <v>27</v>
       </c>
       <c r="G131" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H131" t="s">
         <v>383</v>
       </c>
       <c r="I131" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="J131">
         <v>0</v>
@@ -24687,7 +24709,7 @@
         <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -24702,7 +24724,7 @@
         <v>383</v>
       </c>
       <c r="I132" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J132">
         <v>0</v>
@@ -24722,7 +24744,7 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -24737,7 +24759,7 @@
         <v>383</v>
       </c>
       <c r="I133" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J133">
         <v>0</v>
@@ -24757,7 +24779,7 @@
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -24792,22 +24814,22 @@
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E135">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F135" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G135" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H135" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I135" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J135">
         <v>0</v>
@@ -24827,7 +24849,7 @@
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -24842,7 +24864,7 @@
         <v>391</v>
       </c>
       <c r="I136" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="J136">
         <v>0</v>
@@ -24862,7 +24884,7 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -24877,7 +24899,7 @@
         <v>391</v>
       </c>
       <c r="I137" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J137">
         <v>0</v>
@@ -24897,7 +24919,7 @@
         <v>3</v>
       </c>
       <c r="D138" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -24932,7 +24954,7 @@
         <v>3</v>
       </c>
       <c r="D139" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -24958,7 +24980,7 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B140" t="s">
         <v>380</v>
@@ -24967,22 +24989,22 @@
         <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G140" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H140" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I140" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J140">
         <v>0</v>
@@ -25002,7 +25024,7 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E141">
         <v>0</v>
@@ -25037,7 +25059,7 @@
         <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -25072,7 +25094,7 @@
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -25087,7 +25109,7 @@
         <v>392</v>
       </c>
       <c r="I143" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J143">
         <v>0</v>
@@ -25107,7 +25129,7 @@
         <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -25122,7 +25144,7 @@
         <v>392</v>
       </c>
       <c r="I144" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -25142,7 +25164,7 @@
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -25157,7 +25179,7 @@
         <v>392</v>
       </c>
       <c r="I145" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J145">
         <v>0</v>
@@ -25177,7 +25199,7 @@
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E146">
         <v>0</v>
@@ -25203,31 +25225,31 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B147" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C147" t="s">
         <v>3</v>
       </c>
       <c r="D147" t="s">
-        <v>471</v>
+        <v>171</v>
       </c>
       <c r="E147">
         <v>0</v>
       </c>
       <c r="F147" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="G147" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H147" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="I147" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="J147">
         <v>0</v>
@@ -25253,16 +25275,16 @@
         <v>0</v>
       </c>
       <c r="F148" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G148" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H148" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I148" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J148">
         <v>0</v>
@@ -25285,19 +25307,19 @@
         <v>471</v>
       </c>
       <c r="E149">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F149" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G149" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H149" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I149" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J149">
         <v>0</v>
@@ -25317,22 +25339,22 @@
         <v>3</v>
       </c>
       <c r="D150" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F150" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G150" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="H150" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I150" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J150">
         <v>0</v>
@@ -25358,16 +25380,16 @@
         <v>0</v>
       </c>
       <c r="F151" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G151" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H151" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I151" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J151">
         <v>0</v>
@@ -25390,19 +25412,19 @@
         <v>472</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F152" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G152" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H152" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I152" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J152">
         <v>0</v>
@@ -25422,22 +25444,22 @@
         <v>3</v>
       </c>
       <c r="D153" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F153" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G153" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="H153" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I153" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J153">
         <v>0</v>
@@ -25463,16 +25485,16 @@
         <v>0</v>
       </c>
       <c r="F154" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G154" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H154" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I154" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J154">
         <v>0</v>
@@ -25495,19 +25517,19 @@
         <v>473</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F155" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G155" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H155" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I155" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J155">
         <v>0</v>
@@ -25518,31 +25540,31 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B156" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C156" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D156" t="s">
-        <v>441</v>
+        <v>473</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G156" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="H156" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I156" t="s">
-        <v>381</v>
+        <v>476</v>
       </c>
       <c r="J156">
         <v>0</v>
@@ -25553,31 +25575,31 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>561</v>
+        <v>175</v>
       </c>
       <c r="B157" t="s">
         <v>380</v>
       </c>
       <c r="C157" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D157" t="s">
-        <v>8</v>
+        <v>441</v>
       </c>
       <c r="E157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F157" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G157" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H157" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I157" t="s">
-        <v>713</v>
+        <v>381</v>
       </c>
       <c r="J157">
         <v>0</v>
@@ -25597,7 +25619,7 @@
         <v>3</v>
       </c>
       <c r="D158" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -25632,7 +25654,7 @@
         <v>3</v>
       </c>
       <c r="D159" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -25653,6 +25675,41 @@
         <v>0</v>
       </c>
       <c r="K159" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>561</v>
+      </c>
+      <c r="B160" t="s">
+        <v>380</v>
+      </c>
+      <c r="C160" t="s">
+        <v>3</v>
+      </c>
+      <c r="D160" t="s">
+        <v>7</v>
+      </c>
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160" t="s">
+        <v>27</v>
+      </c>
+      <c r="G160" t="s">
+        <v>382</v>
+      </c>
+      <c r="H160" t="s">
+        <v>383</v>
+      </c>
+      <c r="I160" t="s">
+        <v>713</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160" t="s">
         <v>381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates for TFS 3179 and 3186.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34737
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3115" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="810">
   <si>
     <t>SourceID</t>
   </si>
@@ -2468,7 +2468,13 @@
     <t>OMR: Invalid use of Attestation</t>
   </si>
   <si>
-    <t>Added new record to Email notifications table to support Quality Other CTC feed</t>
+    <t>3179/3186</t>
+  </si>
+  <si>
+    <t>Added new record to Email notifications tab to support Quality Other CTC feed</t>
+  </si>
+  <si>
+    <t>Added new record to Email notifications tab to support Quality Other HFC and KUD feeds</t>
   </si>
 </sst>
 </file>
@@ -2833,10 +2839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,7 +3630,24 @@
         <v>2268</v>
       </c>
       <c r="E46" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" s="1">
+        <v>42566</v>
+      </c>
+      <c r="C47" t="s">
+        <v>434</v>
+      </c>
+      <c r="D47" t="s">
         <v>807</v>
+      </c>
+      <c r="E47" t="s">
+        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -20094,9 +20117,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K160"/>
+  <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection sqref="A1:K161"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21588,34 +21613,34 @@
         <v>174</v>
       </c>
       <c r="B43" t="s">
-        <v>380</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G43" t="s">
-        <v>381</v>
+        <v>427</v>
       </c>
       <c r="H43" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="I43" t="s">
-        <v>381</v>
+        <v>475</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>381</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -21632,19 +21657,19 @@
         <v>6</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H44" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I44" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -21664,7 +21689,7 @@
         <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -21679,7 +21704,7 @@
         <v>383</v>
       </c>
       <c r="I45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -21699,7 +21724,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -21714,7 +21739,7 @@
         <v>383</v>
       </c>
       <c r="I46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -21734,7 +21759,7 @@
         <v>5</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -21749,7 +21774,7 @@
         <v>383</v>
       </c>
       <c r="I47" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -21769,7 +21794,7 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -21804,7 +21829,7 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -21839,7 +21864,7 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -21854,7 +21879,7 @@
         <v>383</v>
       </c>
       <c r="I50" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -21874,7 +21899,7 @@
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -21889,7 +21914,7 @@
         <v>383</v>
       </c>
       <c r="I51" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -21909,7 +21934,7 @@
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -21924,7 +21949,7 @@
         <v>383</v>
       </c>
       <c r="I52" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -21944,22 +21969,22 @@
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>441</v>
+        <v>14</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G53" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H53" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I53" t="s">
-        <v>381</v>
+        <v>395</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -21970,7 +21995,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B54" t="s">
         <v>380</v>
@@ -22005,7 +22030,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
         <v>380</v>
@@ -22014,22 +22039,22 @@
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>171</v>
+        <v>441</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G55" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H55" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I55" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -22049,22 +22074,22 @@
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>171</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G56" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H56" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I56" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -22084,10 +22109,10 @@
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57" t="s">
         <v>177</v>
@@ -22096,10 +22121,10 @@
         <v>427</v>
       </c>
       <c r="H57" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I57" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -22119,7 +22144,7 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -22154,7 +22179,7 @@
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -22169,7 +22194,7 @@
         <v>385</v>
       </c>
       <c r="I59" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J59">
         <v>0</v>
@@ -22189,7 +22214,7 @@
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -22204,7 +22229,7 @@
         <v>385</v>
       </c>
       <c r="I60" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J60">
         <v>0</v>
@@ -22224,7 +22249,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -22259,7 +22284,7 @@
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -22294,7 +22319,7 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -22309,7 +22334,7 @@
         <v>385</v>
       </c>
       <c r="I63" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="J63">
         <v>0</v>
@@ -22329,7 +22354,7 @@
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -22344,7 +22369,7 @@
         <v>385</v>
       </c>
       <c r="I64" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -22364,7 +22389,7 @@
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -22379,7 +22404,7 @@
         <v>385</v>
       </c>
       <c r="I65" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -22399,7 +22424,7 @@
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -22431,25 +22456,25 @@
         <v>380</v>
       </c>
       <c r="C67" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G67" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H67" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I67" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J67">
         <v>0</v>
@@ -22460,31 +22485,31 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B68" t="s">
         <v>380</v>
       </c>
       <c r="C68" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
       <c r="G68" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H68" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I68" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -22504,7 +22529,7 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -22519,7 +22544,7 @@
         <v>391</v>
       </c>
       <c r="I69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -22539,7 +22564,7 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -22554,7 +22579,7 @@
         <v>391</v>
       </c>
       <c r="I70" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -22574,7 +22599,7 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -22609,7 +22634,7 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -22624,7 +22649,7 @@
         <v>391</v>
       </c>
       <c r="I72" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="J72">
         <v>0</v>
@@ -22644,22 +22669,22 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G73" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H73" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="I73" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J73">
         <v>0</v>
@@ -22679,7 +22704,7 @@
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -22694,7 +22719,7 @@
         <v>385</v>
       </c>
       <c r="I74" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J74">
         <v>0</v>
@@ -22714,7 +22739,7 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -22729,7 +22754,7 @@
         <v>385</v>
       </c>
       <c r="I75" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J75">
         <v>0</v>
@@ -22749,7 +22774,7 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -22784,7 +22809,7 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -22816,25 +22841,25 @@
         <v>380</v>
       </c>
       <c r="C78" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="G78" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H78" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I78" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J78">
         <v>0</v>
@@ -22845,7 +22870,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B79" t="s">
         <v>380</v>
@@ -22854,22 +22879,22 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G79" t="s">
         <v>175</v>
       </c>
       <c r="H79" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I79" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -22889,7 +22914,7 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -22924,7 +22949,7 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -22939,7 +22964,7 @@
         <v>386</v>
       </c>
       <c r="I81" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J81">
         <v>0</v>
@@ -22959,7 +22984,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -22974,7 +22999,7 @@
         <v>386</v>
       </c>
       <c r="I82" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J82">
         <v>0</v>
@@ -22994,7 +23019,7 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -23029,7 +23054,7 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -23064,7 +23089,7 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -23079,7 +23104,7 @@
         <v>386</v>
       </c>
       <c r="I85" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J85">
         <v>0</v>
@@ -23099,7 +23124,7 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -23114,7 +23139,7 @@
         <v>386</v>
       </c>
       <c r="I86" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="J86">
         <v>0</v>
@@ -23134,7 +23159,7 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -23149,7 +23174,7 @@
         <v>386</v>
       </c>
       <c r="I87" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J87">
         <v>0</v>
@@ -23169,7 +23194,7 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -23184,7 +23209,7 @@
         <v>386</v>
       </c>
       <c r="I88" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="J88">
         <v>0</v>
@@ -23204,22 +23229,22 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>171</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G89" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H89" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I89" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="J89">
         <v>0</v>
@@ -23239,7 +23264,7 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -23254,7 +23279,7 @@
         <v>383</v>
       </c>
       <c r="I90" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J90">
         <v>0</v>
@@ -23265,31 +23290,31 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
         <v>380</v>
       </c>
       <c r="C91" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G91" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H91" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I91" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="J91">
         <v>0</v>
@@ -23309,7 +23334,7 @@
         <v>5</v>
       </c>
       <c r="D92" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -23344,7 +23369,7 @@
         <v>5</v>
       </c>
       <c r="D93" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -23359,7 +23384,7 @@
         <v>385</v>
       </c>
       <c r="I93" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J93">
         <v>0</v>
@@ -23379,7 +23404,7 @@
         <v>5</v>
       </c>
       <c r="D94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -23394,7 +23419,7 @@
         <v>385</v>
       </c>
       <c r="I94" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="J94">
         <v>0</v>
@@ -23414,7 +23439,7 @@
         <v>5</v>
       </c>
       <c r="D95" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -23449,7 +23474,7 @@
         <v>5</v>
       </c>
       <c r="D96" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -23484,7 +23509,7 @@
         <v>5</v>
       </c>
       <c r="D97" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -23499,7 +23524,7 @@
         <v>385</v>
       </c>
       <c r="I97" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="J97">
         <v>0</v>
@@ -23519,7 +23544,7 @@
         <v>5</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -23534,7 +23559,7 @@
         <v>385</v>
       </c>
       <c r="I98" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J98">
         <v>0</v>
@@ -23554,7 +23579,7 @@
         <v>5</v>
       </c>
       <c r="D99" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -23569,7 +23594,7 @@
         <v>385</v>
       </c>
       <c r="I99" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="J99">
         <v>0</v>
@@ -23589,7 +23614,7 @@
         <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -23621,25 +23646,25 @@
         <v>380</v>
       </c>
       <c r="C101" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D101" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
       <c r="F101" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G101" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H101" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="I101" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J101">
         <v>0</v>
@@ -23659,7 +23684,7 @@
         <v>3</v>
       </c>
       <c r="D102" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -23694,7 +23719,7 @@
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -23709,7 +23734,7 @@
         <v>392</v>
       </c>
       <c r="I103" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J103">
         <v>0</v>
@@ -23720,7 +23745,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B104" t="s">
         <v>380</v>
@@ -23729,22 +23754,22 @@
         <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>27</v>
+        <v>179</v>
       </c>
       <c r="G104" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H104" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="I104" t="s">
-        <v>406</v>
+        <v>425</v>
       </c>
       <c r="J104">
         <v>0</v>
@@ -23764,7 +23789,7 @@
         <v>3</v>
       </c>
       <c r="D105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -23779,7 +23804,7 @@
         <v>383</v>
       </c>
       <c r="I105" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="J105">
         <v>0</v>
@@ -23799,7 +23824,7 @@
         <v>3</v>
       </c>
       <c r="D106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -23814,7 +23839,7 @@
         <v>383</v>
       </c>
       <c r="I106" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J106">
         <v>0</v>
@@ -23834,7 +23859,7 @@
         <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -23869,7 +23894,7 @@
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -23884,7 +23909,7 @@
         <v>383</v>
       </c>
       <c r="I108" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J108">
         <v>0</v>
@@ -23904,7 +23929,7 @@
         <v>3</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -23919,7 +23944,7 @@
         <v>383</v>
       </c>
       <c r="I109" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J109">
         <v>0</v>
@@ -23939,7 +23964,7 @@
         <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -23954,7 +23979,7 @@
         <v>383</v>
       </c>
       <c r="I110" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="J110">
         <v>0</v>
@@ -23974,7 +23999,7 @@
         <v>3</v>
       </c>
       <c r="D111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -23989,7 +24014,7 @@
         <v>383</v>
       </c>
       <c r="I111" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="J111">
         <v>0</v>
@@ -24009,7 +24034,7 @@
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -24038,28 +24063,28 @@
         <v>174</v>
       </c>
       <c r="B113" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C113" t="s">
         <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>16</v>
+        <v>171</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G113" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H113" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I113" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="J113">
         <v>0</v>
@@ -24073,28 +24098,28 @@
         <v>174</v>
       </c>
       <c r="B114" t="s">
-        <v>172</v>
+        <v>387</v>
       </c>
       <c r="C114" t="s">
         <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="E114">
         <v>0</v>
       </c>
       <c r="F114" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G114" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H114" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I114" t="s">
-        <v>503</v>
+        <v>399</v>
       </c>
       <c r="J114">
         <v>0</v>
@@ -24105,7 +24130,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B115" t="s">
         <v>172</v>
@@ -24120,16 +24145,16 @@
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G115" t="s">
         <v>175</v>
       </c>
       <c r="H115" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I115" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J115">
         <v>0</v>
@@ -24140,31 +24165,31 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>481</v>
+        <v>175</v>
       </c>
       <c r="B116" t="s">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="C116" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="E116">
         <v>0</v>
       </c>
       <c r="F116" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="G116" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H116" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I116" t="s">
-        <v>400</v>
+        <v>504</v>
       </c>
       <c r="J116">
         <v>0</v>
@@ -24184,7 +24209,7 @@
         <v>5</v>
       </c>
       <c r="D117" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -24219,7 +24244,7 @@
         <v>5</v>
       </c>
       <c r="D118" t="s">
-        <v>491</v>
+        <v>12</v>
       </c>
       <c r="E118">
         <v>0</v>
@@ -24254,7 +24279,7 @@
         <v>5</v>
       </c>
       <c r="D119" t="s">
-        <v>170</v>
+        <v>491</v>
       </c>
       <c r="E119">
         <v>0</v>
@@ -24289,7 +24314,7 @@
         <v>5</v>
       </c>
       <c r="D120" t="s">
-        <v>493</v>
+        <v>170</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -24321,25 +24346,25 @@
         <v>380</v>
       </c>
       <c r="C121" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
+        <v>493</v>
       </c>
       <c r="E121">
         <v>0</v>
       </c>
       <c r="F121" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G121" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H121" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I121" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="J121">
         <v>0</v>
@@ -24359,7 +24384,7 @@
         <v>3</v>
       </c>
       <c r="D122" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -24394,7 +24419,7 @@
         <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>491</v>
+        <v>12</v>
       </c>
       <c r="E123">
         <v>0</v>
@@ -24429,7 +24454,7 @@
         <v>3</v>
       </c>
       <c r="D124" t="s">
-        <v>170</v>
+        <v>491</v>
       </c>
       <c r="E124">
         <v>0</v>
@@ -24464,7 +24489,7 @@
         <v>3</v>
       </c>
       <c r="D125" t="s">
-        <v>493</v>
+        <v>170</v>
       </c>
       <c r="E125">
         <v>0</v>
@@ -24490,31 +24515,31 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="B126" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C126" t="s">
         <v>3</v>
       </c>
       <c r="D126" t="s">
-        <v>16</v>
+        <v>493</v>
       </c>
       <c r="E126">
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>177</v>
+        <v>28</v>
       </c>
       <c r="G126" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H126" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I126" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="J126">
         <v>0</v>
@@ -24540,16 +24565,16 @@
         <v>0</v>
       </c>
       <c r="F127" t="s">
-        <v>28</v>
+        <v>177</v>
       </c>
       <c r="G127" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H127" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I127" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="J127">
         <v>0</v>
@@ -24575,16 +24600,16 @@
         <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G128" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H128" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I128" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J128">
         <v>0</v>
@@ -24598,28 +24623,28 @@
         <v>174</v>
       </c>
       <c r="B129" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="C129" t="s">
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E129">
         <v>0</v>
       </c>
       <c r="F129" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G129" t="s">
-        <v>427</v>
+        <v>382</v>
       </c>
       <c r="H129" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I129" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J129">
         <v>0</v>
@@ -24645,16 +24670,16 @@
         <v>0</v>
       </c>
       <c r="F130" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G130" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H130" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I130" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J130">
         <v>0</v>
@@ -24677,19 +24702,19 @@
         <v>15</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F131" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G131" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H131" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I131" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J131">
         <v>0</v>
@@ -24700,31 +24725,31 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B132" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C132" t="s">
         <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F132" t="s">
         <v>27</v>
       </c>
       <c r="G132" t="s">
-        <v>175</v>
+        <v>390</v>
       </c>
       <c r="H132" t="s">
         <v>383</v>
       </c>
       <c r="I132" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="J132">
         <v>0</v>
@@ -24744,7 +24769,7 @@
         <v>3</v>
       </c>
       <c r="D133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -24759,7 +24784,7 @@
         <v>383</v>
       </c>
       <c r="I133" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J133">
         <v>0</v>
@@ -24779,7 +24804,7 @@
         <v>3</v>
       </c>
       <c r="D134" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E134">
         <v>0</v>
@@ -24794,7 +24819,7 @@
         <v>383</v>
       </c>
       <c r="I134" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="J134">
         <v>0</v>
@@ -24814,7 +24839,7 @@
         <v>3</v>
       </c>
       <c r="D135" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E135">
         <v>0</v>
@@ -24849,22 +24874,22 @@
         <v>3</v>
       </c>
       <c r="D136" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F136" t="s">
-        <v>178</v>
+        <v>27</v>
       </c>
       <c r="G136" t="s">
-        <v>382</v>
+        <v>175</v>
       </c>
       <c r="H136" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I136" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="J136">
         <v>0</v>
@@ -24884,7 +24909,7 @@
         <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -24899,7 +24924,7 @@
         <v>391</v>
       </c>
       <c r="I137" t="s">
-        <v>414</v>
+        <v>422</v>
       </c>
       <c r="J137">
         <v>0</v>
@@ -24919,7 +24944,7 @@
         <v>3</v>
       </c>
       <c r="D138" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -24934,7 +24959,7 @@
         <v>391</v>
       </c>
       <c r="I138" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J138">
         <v>0</v>
@@ -24954,7 +24979,7 @@
         <v>3</v>
       </c>
       <c r="D139" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -24989,7 +25014,7 @@
         <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -25015,7 +25040,7 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="B141" t="s">
         <v>380</v>
@@ -25024,22 +25049,22 @@
         <v>3</v>
       </c>
       <c r="D141" t="s">
-        <v>10</v>
+        <v>176</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F141" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G141" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="H141" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I141" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="J141">
         <v>0</v>
@@ -25059,7 +25084,7 @@
         <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="E142">
         <v>0</v>
@@ -25094,7 +25119,7 @@
         <v>3</v>
       </c>
       <c r="D143" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="E143">
         <v>0</v>
@@ -25129,7 +25154,7 @@
         <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -25144,7 +25169,7 @@
         <v>392</v>
       </c>
       <c r="I144" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -25164,7 +25189,7 @@
         <v>3</v>
       </c>
       <c r="D145" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -25179,7 +25204,7 @@
         <v>392</v>
       </c>
       <c r="I145" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="J145">
         <v>0</v>
@@ -25199,7 +25224,7 @@
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E146">
         <v>0</v>
@@ -25214,7 +25239,7 @@
         <v>392</v>
       </c>
       <c r="I146" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J146">
         <v>0</v>
@@ -25234,7 +25259,7 @@
         <v>3</v>
       </c>
       <c r="D147" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="E147">
         <v>0</v>
@@ -25260,31 +25285,31 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>174</v>
+        <v>92</v>
       </c>
       <c r="B148" t="s">
-        <v>15</v>
+        <v>380</v>
       </c>
       <c r="C148" t="s">
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>471</v>
+        <v>171</v>
       </c>
       <c r="E148">
         <v>0</v>
       </c>
       <c r="F148" t="s">
-        <v>26</v>
+        <v>179</v>
       </c>
       <c r="G148" t="s">
-        <v>427</v>
+        <v>175</v>
       </c>
       <c r="H148" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="I148" t="s">
-        <v>475</v>
+        <v>425</v>
       </c>
       <c r="J148">
         <v>0</v>
@@ -25310,16 +25335,16 @@
         <v>0</v>
       </c>
       <c r="F149" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G149" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H149" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I149" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J149">
         <v>0</v>
@@ -25342,19 +25367,19 @@
         <v>471</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F150" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G150" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H150" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I150" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J150">
         <v>0</v>
@@ -25374,22 +25399,22 @@
         <v>3</v>
       </c>
       <c r="D151" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F151" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G151" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="H151" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I151" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J151">
         <v>0</v>
@@ -25415,16 +25440,16 @@
         <v>0</v>
       </c>
       <c r="F152" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G152" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H152" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I152" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J152">
         <v>0</v>
@@ -25447,19 +25472,19 @@
         <v>472</v>
       </c>
       <c r="E153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F153" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G153" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H153" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I153" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J153">
         <v>0</v>
@@ -25479,22 +25504,22 @@
         <v>3</v>
       </c>
       <c r="D154" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G154" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="H154" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I154" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="J154">
         <v>0</v>
@@ -25520,16 +25545,16 @@
         <v>0</v>
       </c>
       <c r="F155" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G155" t="s">
-        <v>175</v>
+        <v>427</v>
       </c>
       <c r="H155" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I155" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="J155">
         <v>0</v>
@@ -25552,19 +25577,19 @@
         <v>473</v>
       </c>
       <c r="E156">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F156" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G156" t="s">
-        <v>390</v>
+        <v>175</v>
       </c>
       <c r="H156" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I156" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="J156">
         <v>0</v>
@@ -25575,31 +25600,31 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B157" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
       <c r="C157" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D157" t="s">
-        <v>441</v>
+        <v>473</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G157" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="H157" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I157" t="s">
-        <v>381</v>
+        <v>476</v>
       </c>
       <c r="J157">
         <v>0</v>
@@ -25610,31 +25635,31 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>561</v>
+        <v>175</v>
       </c>
       <c r="B158" t="s">
         <v>380</v>
       </c>
       <c r="C158" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D158" t="s">
-        <v>8</v>
+        <v>441</v>
       </c>
       <c r="E158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F158" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G158" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H158" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I158" t="s">
-        <v>713</v>
+        <v>381</v>
       </c>
       <c r="J158">
         <v>0</v>
@@ -25654,7 +25679,7 @@
         <v>3</v>
       </c>
       <c r="D159" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -25689,7 +25714,7 @@
         <v>3</v>
       </c>
       <c r="D160" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -25710,6 +25735,41 @@
         <v>0</v>
       </c>
       <c r="K160" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>561</v>
+      </c>
+      <c r="B161" t="s">
+        <v>380</v>
+      </c>
+      <c r="C161" t="s">
+        <v>3</v>
+      </c>
+      <c r="D161" t="s">
+        <v>7</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161" t="s">
+        <v>27</v>
+      </c>
+      <c r="G161" t="s">
+        <v>382</v>
+      </c>
+      <c r="H161" t="s">
+        <v>383</v>
+      </c>
+      <c r="I161" t="s">
+        <v>713</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="K161" t="s">
         <v>381</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated for TFS 4137.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C35552
</commit_message>
<xml_diff>
--- a/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
+++ b/Design/CCO_eCoaching_Dimension_Table_Data.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3134" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="815">
   <si>
     <t>SourceID</t>
   </si>
@@ -2484,6 +2484,12 @@
   </si>
   <si>
     <t>Principal Analyst, Systems</t>
+  </si>
+  <si>
+    <t>updated DIM_Coaching_Reason and Coaching_Reason_Selection tabs to add Call Efficiency as a Reason for CSRs and Sups and remove AHT</t>
+  </si>
+  <si>
+    <t>Call Efficiency</t>
   </si>
 </sst>
 </file>
@@ -2848,7 +2854,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3689,6 +3695,23 @@
       </c>
       <c r="E49" t="s">
         <v>810</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" s="1">
+        <v>42646</v>
+      </c>
+      <c r="C50" t="s">
+        <v>432</v>
+      </c>
+      <c r="D50">
+        <v>4137</v>
+      </c>
+      <c r="E50" t="s">
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -5114,9 +5137,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P299"/>
+  <dimension ref="A1:P306"/>
   <sheetViews>
-    <sheetView topLeftCell="A255" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6702,13 +6725,13 @@
         <v>1</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
         <v>0</v>
@@ -6752,13 +6775,13 @@
         <v>1</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -6802,13 +6825,13 @@
         <v>1</v>
       </c>
       <c r="J34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>0</v>
@@ -6852,13 +6875,13 @@
         <v>1</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
       <c r="L35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -6902,13 +6925,13 @@
         <v>1</v>
       </c>
       <c r="J36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
       <c r="L36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>0</v>
@@ -12652,13 +12675,13 @@
         <v>1</v>
       </c>
       <c r="J151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K151">
         <v>0</v>
       </c>
       <c r="L151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M151">
         <v>0</v>
@@ -12975,25 +12998,25 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158">
-        <v>-1</v>
+        <v>55</v>
       </c>
       <c r="B158" t="s">
-        <v>4</v>
+        <v>814</v>
       </c>
       <c r="C158">
-        <v>-1</v>
+        <v>122</v>
       </c>
       <c r="D158" t="s">
-        <v>4</v>
+        <v>553</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H158">
         <v>1</v>
@@ -13002,13 +13025,13 @@
         <v>1</v>
       </c>
       <c r="J158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K158">
         <v>0</v>
       </c>
       <c r="L158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M158">
         <v>0</v>
@@ -13025,16 +13048,16 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="B159" t="s">
-        <v>84</v>
+        <v>814</v>
       </c>
       <c r="C159">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="D159" t="s">
-        <v>206</v>
+        <v>554</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -13075,16 +13098,16 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B160" t="s">
-        <v>85</v>
+        <v>814</v>
       </c>
       <c r="C160">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="D160" t="s">
-        <v>107</v>
+        <v>555</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -13108,7 +13131,7 @@
         <v>0</v>
       </c>
       <c r="L160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M160">
         <v>0</v>
@@ -13125,16 +13148,16 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B161" t="s">
-        <v>85</v>
+        <v>814</v>
       </c>
       <c r="C161">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="D161" t="s">
-        <v>108</v>
+        <v>556</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -13158,7 +13181,7 @@
         <v>0</v>
       </c>
       <c r="L161">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M161">
         <v>0</v>
@@ -13175,16 +13198,16 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B162" t="s">
-        <v>85</v>
+        <v>814</v>
       </c>
       <c r="C162">
-        <v>15</v>
+        <v>126</v>
       </c>
       <c r="D162" t="s">
-        <v>109</v>
+        <v>557</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -13208,7 +13231,7 @@
         <v>0</v>
       </c>
       <c r="L162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M162">
         <v>0</v>
@@ -13225,16 +13248,16 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B163" t="s">
-        <v>85</v>
+        <v>814</v>
       </c>
       <c r="C163">
-        <v>16</v>
+        <v>230</v>
       </c>
       <c r="D163" t="s">
-        <v>110</v>
+        <v>713</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -13258,7 +13281,7 @@
         <v>0</v>
       </c>
       <c r="L163">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M163">
         <v>0</v>
@@ -13275,16 +13298,16 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B164" t="s">
-        <v>85</v>
+        <v>814</v>
       </c>
       <c r="C164">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D164" t="s">
-        <v>111</v>
+        <v>206</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -13308,7 +13331,7 @@
         <v>0</v>
       </c>
       <c r="L164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M164">
         <v>0</v>
@@ -13325,25 +13348,25 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="B165" t="s">
-        <v>85</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>18</v>
+        <v>-1</v>
       </c>
       <c r="D165" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="E165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H165">
         <v>1</v>
@@ -13352,7 +13375,7 @@
         <v>1</v>
       </c>
       <c r="J165">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K165">
         <v>0</v>
@@ -13375,16 +13398,16 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C166">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D166" t="s">
-        <v>113</v>
+        <v>206</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -13402,7 +13425,7 @@
         <v>1</v>
       </c>
       <c r="J166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K166">
         <v>0</v>
@@ -13431,10 +13454,10 @@
         <v>85</v>
       </c>
       <c r="C167">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D167" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -13475,16 +13498,16 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B168" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C168">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="D168" t="s">
-        <v>172</v>
+        <v>108</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -13493,7 +13516,7 @@
         <v>1</v>
       </c>
       <c r="G168">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H168">
         <v>1</v>
@@ -13525,16 +13548,16 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B169" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C169">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D169" t="s">
-        <v>206</v>
+        <v>109</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -13555,10 +13578,10 @@
         <v>1</v>
       </c>
       <c r="K169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M169">
         <v>0</v>
@@ -13567,24 +13590,24 @@
         <v>0</v>
       </c>
       <c r="O169">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B170" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
       <c r="C170">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D170" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -13608,7 +13631,7 @@
         <v>0</v>
       </c>
       <c r="L170">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M170">
         <v>0</v>
@@ -13625,16 +13648,16 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B171" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
       <c r="C171">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D171" t="s">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -13658,7 +13681,7 @@
         <v>0</v>
       </c>
       <c r="L171">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M171">
         <v>0</v>
@@ -13675,16 +13698,16 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B172" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C172">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D172" t="s">
-        <v>206</v>
+        <v>112</v>
       </c>
       <c r="E172">
         <v>1</v>
@@ -13725,16 +13748,16 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B173" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C173">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D173" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="E173">
         <v>1</v>
@@ -13749,7 +13772,7 @@
         <v>1</v>
       </c>
       <c r="I173">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J173">
         <v>1</v>
@@ -13758,13 +13781,13 @@
         <v>0</v>
       </c>
       <c r="L173">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M173">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N173">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O173">
         <v>0</v>
@@ -13775,16 +13798,16 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B174" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C174">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D174" t="s">
-        <v>342</v>
+        <v>206</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13799,7 +13822,7 @@
         <v>1</v>
       </c>
       <c r="I174">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J174">
         <v>1</v>
@@ -13808,13 +13831,13 @@
         <v>0</v>
       </c>
       <c r="L174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M174">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N174">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O174">
         <v>0</v>
@@ -13825,16 +13848,16 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B175" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C175">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D175" t="s">
-        <v>343</v>
+        <v>172</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13843,13 +13866,13 @@
         <v>1</v>
       </c>
       <c r="G175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H175">
         <v>1</v>
       </c>
       <c r="I175">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J175">
         <v>1</v>
@@ -13861,10 +13884,10 @@
         <v>0</v>
       </c>
       <c r="M175">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N175">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O175">
         <v>0</v>
@@ -13875,16 +13898,16 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B176" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C176">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D176" t="s">
-        <v>344</v>
+        <v>206</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -13899,42 +13922,42 @@
         <v>1</v>
       </c>
       <c r="I176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J176">
         <v>1</v>
       </c>
       <c r="K176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L176">
         <v>1</v>
       </c>
       <c r="M176">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N176">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O176">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="C177">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D177" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -13949,7 +13972,7 @@
         <v>1</v>
       </c>
       <c r="I177">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J177">
         <v>1</v>
@@ -13961,10 +13984,10 @@
         <v>1</v>
       </c>
       <c r="M177">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N177">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O177">
         <v>0</v>
@@ -13975,16 +13998,16 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B178" t="s">
-        <v>88</v>
+        <v>181</v>
       </c>
       <c r="C178">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="D178" t="s">
-        <v>345</v>
+        <v>206</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -13999,7 +14022,7 @@
         <v>1</v>
       </c>
       <c r="I178">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J178">
         <v>1</v>
@@ -14011,10 +14034,10 @@
         <v>1</v>
       </c>
       <c r="M178">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N178">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O178">
         <v>0</v>
@@ -14025,16 +14048,16 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B179" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C179">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D179" t="s">
-        <v>105</v>
+        <v>206</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -14049,7 +14072,7 @@
         <v>1</v>
       </c>
       <c r="I179">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J179">
         <v>1</v>
@@ -14058,13 +14081,13 @@
         <v>0</v>
       </c>
       <c r="L179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M179">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N179">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O179">
         <v>0</v>
@@ -14081,10 +14104,10 @@
         <v>88</v>
       </c>
       <c r="C180">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D180" t="s">
-        <v>236</v>
+        <v>100</v>
       </c>
       <c r="E180">
         <v>1</v>
@@ -14131,10 +14154,10 @@
         <v>88</v>
       </c>
       <c r="C181">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="D181" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="E181">
         <v>1</v>
@@ -14181,10 +14204,10 @@
         <v>88</v>
       </c>
       <c r="C182">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D182" t="s">
-        <v>101</v>
+        <v>343</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -14208,7 +14231,7 @@
         <v>0</v>
       </c>
       <c r="L182">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M182">
         <v>1</v>
@@ -14231,10 +14254,10 @@
         <v>88</v>
       </c>
       <c r="C183">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D183" t="s">
-        <v>206</v>
+        <v>344</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -14270,21 +14293,21 @@
         <v>0</v>
       </c>
       <c r="P183">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B184" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C184">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D184" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -14299,7 +14322,7 @@
         <v>1</v>
       </c>
       <c r="I184">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J184">
         <v>1</v>
@@ -14308,13 +14331,13 @@
         <v>0</v>
       </c>
       <c r="L184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M184">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N184">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O184">
         <v>0</v>
@@ -14325,16 +14348,16 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B185" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C185">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="D185" t="s">
-        <v>206</v>
+        <v>345</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -14349,7 +14372,7 @@
         <v>1</v>
       </c>
       <c r="I185">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J185">
         <v>1</v>
@@ -14358,13 +14381,13 @@
         <v>0</v>
       </c>
       <c r="L185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N185">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O185">
         <v>0</v>
@@ -14375,16 +14398,16 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B186" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C186">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D186" t="s">
-        <v>206</v>
+        <v>105</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -14399,7 +14422,7 @@
         <v>1</v>
       </c>
       <c r="I186">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J186">
         <v>1</v>
@@ -14408,13 +14431,13 @@
         <v>0</v>
       </c>
       <c r="L186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M186">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N186">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O186">
         <v>0</v>
@@ -14425,16 +14448,16 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187">
+        <v>6</v>
+      </c>
+      <c r="B187" t="s">
+        <v>88</v>
+      </c>
+      <c r="C187">
         <v>9</v>
       </c>
-      <c r="B187" t="s">
-        <v>91</v>
-      </c>
-      <c r="C187">
-        <v>40</v>
-      </c>
       <c r="D187" t="s">
-        <v>134</v>
+        <v>236</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -14449,7 +14472,7 @@
         <v>1</v>
       </c>
       <c r="I187">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J187">
         <v>1</v>
@@ -14458,13 +14481,13 @@
         <v>0</v>
       </c>
       <c r="L187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M187">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N187">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O187">
         <v>0</v>
@@ -14475,16 +14498,16 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B188" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C188">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D188" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
       <c r="E188">
         <v>1</v>
@@ -14499,7 +14522,7 @@
         <v>1</v>
       </c>
       <c r="I188">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J188">
         <v>1</v>
@@ -14508,13 +14531,13 @@
         <v>0</v>
       </c>
       <c r="L188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M188">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N188">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O188">
         <v>0</v>
@@ -14525,16 +14548,16 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B189" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C189">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D189" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -14549,7 +14572,7 @@
         <v>1</v>
       </c>
       <c r="I189">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J189">
         <v>1</v>
@@ -14558,13 +14581,13 @@
         <v>0</v>
       </c>
       <c r="L189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M189">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N189">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O189">
         <v>0</v>
@@ -14575,16 +14598,16 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B190" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C190">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D190" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -14599,7 +14622,7 @@
         <v>1</v>
       </c>
       <c r="I190">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J190">
         <v>1</v>
@@ -14608,33 +14631,33 @@
         <v>0</v>
       </c>
       <c r="L190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N190">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O190">
         <v>0</v>
       </c>
       <c r="P190">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B191" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C191">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D191" t="s">
-        <v>346</v>
+        <v>106</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -14675,16 +14698,16 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B192" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C192">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D192" t="s">
-        <v>347</v>
+        <v>206</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -14725,16 +14748,16 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B193" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C193">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D193" t="s">
-        <v>115</v>
+        <v>206</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -14781,10 +14804,10 @@
         <v>91</v>
       </c>
       <c r="C194">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D194" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -14831,10 +14854,10 @@
         <v>91</v>
       </c>
       <c r="C195">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D195" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="E195">
         <v>1</v>
@@ -14852,7 +14875,7 @@
         <v>1</v>
       </c>
       <c r="J195">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K195">
         <v>0</v>
@@ -14881,10 +14904,10 @@
         <v>91</v>
       </c>
       <c r="C196">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D196" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -14931,10 +14954,10 @@
         <v>91</v>
       </c>
       <c r="C197">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D197" t="s">
-        <v>348</v>
+        <v>120</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -14981,10 +15004,10 @@
         <v>91</v>
       </c>
       <c r="C198">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D198" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -15031,10 +15054,10 @@
         <v>91</v>
       </c>
       <c r="C199">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D199" t="s">
-        <v>206</v>
+        <v>347</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -15075,16 +15098,16 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B200" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C200">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D200" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="E200">
         <v>1</v>
@@ -15125,16 +15148,16 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B201" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C201">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D201" t="s">
-        <v>350</v>
+        <v>122</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -15175,16 +15198,16 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B202" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C202">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D202" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -15202,7 +15225,7 @@
         <v>1</v>
       </c>
       <c r="J202">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K202">
         <v>0</v>
@@ -15225,16 +15248,16 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B203" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C203">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D203" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -15275,16 +15298,16 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B204" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C204">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D204" t="s">
-        <v>138</v>
+        <v>348</v>
       </c>
       <c r="E204">
         <v>1</v>
@@ -15325,16 +15348,16 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B205" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C205">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D205" t="s">
-        <v>206</v>
+        <v>349</v>
       </c>
       <c r="E205">
         <v>1</v>
@@ -15367,7 +15390,7 @@
         <v>0</v>
       </c>
       <c r="O205">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P205">
         <v>0</v>
@@ -15375,10 +15398,10 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B206" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C206">
         <v>42</v>
@@ -15396,7 +15419,7 @@
         <v>1</v>
       </c>
       <c r="H206">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I206">
         <v>1</v>
@@ -15405,7 +15428,7 @@
         <v>1</v>
       </c>
       <c r="K206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L206">
         <v>0</v>
@@ -15417,24 +15440,24 @@
         <v>0</v>
       </c>
       <c r="O206">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P206">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B207" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C207">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D207" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="E207">
         <v>1</v>
@@ -15446,16 +15469,16 @@
         <v>1</v>
       </c>
       <c r="H207">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I207">
         <v>1</v>
       </c>
       <c r="J207">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L207">
         <v>0</v>
@@ -15467,7 +15490,7 @@
         <v>0</v>
       </c>
       <c r="O207">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P207">
         <v>0</v>
@@ -15475,16 +15498,16 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B208" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C208">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D208" t="s">
-        <v>194</v>
+        <v>350</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -15496,16 +15519,16 @@
         <v>1</v>
       </c>
       <c r="H208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I208">
         <v>1</v>
       </c>
       <c r="J208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K208">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L208">
         <v>0</v>
@@ -15525,16 +15548,16 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209">
+        <v>10</v>
+      </c>
+      <c r="B209" t="s">
+        <v>92</v>
+      </c>
+      <c r="C209">
         <v>12</v>
       </c>
-      <c r="B209" t="s">
-        <v>94</v>
-      </c>
-      <c r="C209">
-        <v>42</v>
-      </c>
       <c r="D209" t="s">
-        <v>206</v>
+        <v>19</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -15558,7 +15581,7 @@
         <v>0</v>
       </c>
       <c r="L209">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M209">
         <v>0</v>
@@ -15575,16 +15598,16 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A210">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B210" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C210">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D210" t="s">
-        <v>206</v>
+        <v>139</v>
       </c>
       <c r="E210">
         <v>1</v>
@@ -15605,7 +15628,7 @@
         <v>1</v>
       </c>
       <c r="K210">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L210">
         <v>0</v>
@@ -15617,24 +15640,24 @@
         <v>0</v>
       </c>
       <c r="O210">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P210">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B211" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="C211">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D211" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="E211">
         <v>1</v>
@@ -15652,7 +15675,7 @@
         <v>1</v>
       </c>
       <c r="J211">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K211">
         <v>0</v>
@@ -15675,16 +15698,16 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B212" t="s">
-        <v>182</v>
+        <v>92</v>
       </c>
       <c r="C212">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D212" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -15702,10 +15725,10 @@
         <v>1</v>
       </c>
       <c r="J212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K212">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L212">
         <v>0</v>
@@ -15717,7 +15740,7 @@
         <v>0</v>
       </c>
       <c r="O212">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P212">
         <v>0</v>
@@ -15725,16 +15748,16 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B213" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="C213">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D213" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E213">
         <v>1</v>
@@ -15746,13 +15769,13 @@
         <v>1</v>
       </c>
       <c r="H213">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I213">
         <v>1</v>
       </c>
       <c r="J213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K213">
         <v>1</v>
@@ -15767,24 +15790,24 @@
         <v>0</v>
       </c>
       <c r="O213">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P213">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B214" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="C214">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D214" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -15796,7 +15819,7 @@
         <v>1</v>
       </c>
       <c r="H214">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I214">
         <v>1</v>
@@ -15817,7 +15840,7 @@
         <v>0</v>
       </c>
       <c r="O214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P214">
         <v>0</v>
@@ -15825,16 +15848,16 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B215" t="s">
-        <v>182</v>
+        <v>93</v>
       </c>
       <c r="C215">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D215" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E215">
         <v>1</v>
@@ -15846,7 +15869,7 @@
         <v>1</v>
       </c>
       <c r="H215">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I215">
         <v>1</v>
@@ -15875,16 +15898,16 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B216" t="s">
-        <v>182</v>
+        <v>94</v>
       </c>
       <c r="C216">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D216" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -15902,13 +15925,13 @@
         <v>1</v>
       </c>
       <c r="J216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K216">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L216">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M216">
         <v>0</v>
@@ -15925,16 +15948,16 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B217" t="s">
-        <v>182</v>
+        <v>95</v>
       </c>
       <c r="C217">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D217" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E217">
         <v>1</v>
@@ -15952,7 +15975,7 @@
         <v>1</v>
       </c>
       <c r="J217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K217">
         <v>1</v>
@@ -15967,24 +15990,24 @@
         <v>0</v>
       </c>
       <c r="O217">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P217">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B218" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="C218">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="D218" t="s">
-        <v>201</v>
+        <v>17</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -16005,7 +16028,7 @@
         <v>0</v>
       </c>
       <c r="K218">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L218">
         <v>0</v>
@@ -16031,10 +16054,10 @@
         <v>182</v>
       </c>
       <c r="C219">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D219" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E219">
         <v>1</v>
@@ -16081,10 +16104,10 @@
         <v>182</v>
       </c>
       <c r="C220">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D220" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E220">
         <v>1</v>
@@ -16131,10 +16154,10 @@
         <v>182</v>
       </c>
       <c r="C221">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D221" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E221">
         <v>1</v>
@@ -16175,16 +16198,16 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B222" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C222">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D222" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E222">
         <v>1</v>
@@ -16225,16 +16248,16 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B223" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C223">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D223" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E223">
         <v>1</v>
@@ -16275,16 +16298,16 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B224" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C224">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D224" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E224">
         <v>1</v>
@@ -16325,16 +16348,16 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B225" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C225">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D225" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="E225">
         <v>1</v>
@@ -16367,7 +16390,7 @@
         <v>0</v>
       </c>
       <c r="O225">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P225">
         <v>0</v>
@@ -16375,16 +16398,16 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B226" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C226">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D226" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E226">
         <v>1</v>
@@ -16425,16 +16448,16 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B227" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C227">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D227" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E227">
         <v>1</v>
@@ -16455,7 +16478,7 @@
         <v>0</v>
       </c>
       <c r="K227">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L227">
         <v>0</v>
@@ -16475,16 +16498,16 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B228" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C228">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D228" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E228">
         <v>1</v>
@@ -16525,16 +16548,16 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B229" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C229">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D229" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E229">
         <v>1</v>
@@ -16567,7 +16590,7 @@
         <v>0</v>
       </c>
       <c r="O229">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P229">
         <v>0</v>
@@ -16575,16 +16598,16 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B230" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C230">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D230" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E230">
         <v>1</v>
@@ -16599,7 +16622,7 @@
         <v>1</v>
       </c>
       <c r="I230">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J230">
         <v>0</v>
@@ -16625,16 +16648,16 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B231" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C231">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D231" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -16667,7 +16690,7 @@
         <v>0</v>
       </c>
       <c r="O231">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P231">
         <v>0</v>
@@ -16675,16 +16698,16 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B232" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C232">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D232" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -16725,16 +16748,16 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B233" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C233">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D233" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E233">
         <v>1</v>
@@ -16775,16 +16798,16 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B234" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C234">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D234" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="E234">
         <v>1</v>
@@ -16805,7 +16828,7 @@
         <v>0</v>
       </c>
       <c r="K234">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L234">
         <v>0</v>
@@ -16825,16 +16848,16 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B235" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C235">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D235" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E235">
         <v>1</v>
@@ -16875,16 +16898,16 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B236" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C236">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="D236" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E236">
         <v>1</v>
@@ -16917,7 +16940,7 @@
         <v>0</v>
       </c>
       <c r="O236">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P236">
         <v>0</v>
@@ -16925,16 +16948,16 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B237" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C237">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D237" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E237">
         <v>1</v>
@@ -16949,7 +16972,7 @@
         <v>1</v>
       </c>
       <c r="I237">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J237">
         <v>0</v>
@@ -16975,16 +16998,16 @@
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B238" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C238">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D238" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E238">
         <v>1</v>
@@ -17025,16 +17048,16 @@
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B239" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C239">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D239" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E239">
         <v>1</v>
@@ -17055,10 +17078,10 @@
         <v>0</v>
       </c>
       <c r="K239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L239">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M239">
         <v>0</v>
@@ -17067,7 +17090,7 @@
         <v>0</v>
       </c>
       <c r="O239">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P239">
         <v>0</v>
@@ -17075,16 +17098,16 @@
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B240" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C240">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D240" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="E240">
         <v>1</v>
@@ -17105,10 +17128,10 @@
         <v>0</v>
       </c>
       <c r="K240">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L240">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M240">
         <v>0</v>
@@ -17125,16 +17148,16 @@
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B241" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C241">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D241" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="E241">
         <v>1</v>
@@ -17155,10 +17178,10 @@
         <v>0</v>
       </c>
       <c r="K241">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L241">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M241">
         <v>0</v>
@@ -17175,16 +17198,16 @@
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B242" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="C242">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D242" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E242">
         <v>1</v>
@@ -17205,10 +17228,10 @@
         <v>0</v>
       </c>
       <c r="K242">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L242">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M242">
         <v>0</v>
@@ -17220,21 +17243,21 @@
         <v>0</v>
       </c>
       <c r="P242">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B243" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C243">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D243" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E243">
         <v>1</v>
@@ -17255,10 +17278,10 @@
         <v>0</v>
       </c>
       <c r="K243">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L243">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M243">
         <v>0</v>
@@ -17275,16 +17298,16 @@
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B244" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C244">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D244" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E244">
         <v>1</v>
@@ -17305,10 +17328,10 @@
         <v>0</v>
       </c>
       <c r="K244">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L244">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M244">
         <v>0</v>
@@ -17325,16 +17348,16 @@
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B245" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C245">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="D245" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="E245">
         <v>1</v>
@@ -17355,10 +17378,10 @@
         <v>0</v>
       </c>
       <c r="K245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L245">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M245">
         <v>0</v>
@@ -17367,7 +17390,7 @@
         <v>0</v>
       </c>
       <c r="O245">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P245">
         <v>0</v>
@@ -17375,16 +17398,16 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B246" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C246">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D246" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E246">
         <v>1</v>
@@ -17425,16 +17448,16 @@
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B247" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C247">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D247" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E247">
         <v>1</v>
@@ -17475,16 +17498,16 @@
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B248" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C248">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D248" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="E248">
         <v>1</v>
@@ -17525,16 +17548,16 @@
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B249" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C249">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="D249" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="E249">
         <v>1</v>
@@ -17570,7 +17593,7 @@
         <v>0</v>
       </c>
       <c r="P249">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.3">
@@ -17581,10 +17604,10 @@
         <v>189</v>
       </c>
       <c r="C250">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="D250" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E250">
         <v>1</v>
@@ -17625,16 +17648,16 @@
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B251" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C251">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D251" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -17646,7 +17669,7 @@
         <v>1</v>
       </c>
       <c r="H251">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I251">
         <v>1</v>
@@ -17675,16 +17698,16 @@
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B252" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C252">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D252" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="E252">
         <v>1</v>
@@ -17725,16 +17748,16 @@
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B253" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C253">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D253" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E253">
         <v>1</v>
@@ -17775,16 +17798,16 @@
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B254" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C254">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D254" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E254">
         <v>1</v>
@@ -17825,16 +17848,16 @@
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B255" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C255">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D255" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E255">
         <v>1</v>
@@ -17875,16 +17898,16 @@
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B256" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C256">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D256" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="E256">
         <v>1</v>
@@ -17925,16 +17948,16 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B257" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C257">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D257" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="E257">
         <v>1</v>
@@ -17975,16 +17998,16 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B258" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C258">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D258" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="E258">
         <v>1</v>
@@ -17996,7 +18019,7 @@
         <v>1</v>
       </c>
       <c r="H258">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I258">
         <v>1</v>
@@ -18025,16 +18048,16 @@
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B259" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C259">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D259" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E259">
         <v>1</v>
@@ -18075,16 +18098,16 @@
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B260" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C260">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D260" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="E260">
         <v>1</v>
@@ -18125,16 +18148,16 @@
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B261" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C261">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="D261" t="s">
-        <v>351</v>
+        <v>228</v>
       </c>
       <c r="E261">
         <v>1</v>
@@ -18175,16 +18198,16 @@
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B262" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C262">
-        <v>24</v>
+        <v>85</v>
       </c>
       <c r="D262" t="s">
-        <v>352</v>
+        <v>229</v>
       </c>
       <c r="E262">
         <v>1</v>
@@ -18225,16 +18248,16 @@
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B263" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C263">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D263" t="s">
-        <v>353</v>
+        <v>206</v>
       </c>
       <c r="E263">
         <v>1</v>
@@ -18275,16 +18298,16 @@
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B264" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C264">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="D264" t="s">
-        <v>114</v>
+        <v>230</v>
       </c>
       <c r="E264">
         <v>1</v>
@@ -18325,16 +18348,16 @@
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B265" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C265">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="D265" t="s">
-        <v>116</v>
+        <v>231</v>
       </c>
       <c r="E265">
         <v>1</v>
@@ -18375,16 +18398,16 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B266" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C266">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D266" t="s">
-        <v>354</v>
+        <v>232</v>
       </c>
       <c r="E266">
         <v>1</v>
@@ -18425,16 +18448,16 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B267" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C267">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D267" t="s">
-        <v>355</v>
+        <v>206</v>
       </c>
       <c r="E267">
         <v>1</v>
@@ -18481,10 +18504,10 @@
         <v>193</v>
       </c>
       <c r="C268">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D268" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E268">
         <v>1</v>
@@ -18531,10 +18554,10 @@
         <v>193</v>
       </c>
       <c r="C269">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D269" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E269">
         <v>1</v>
@@ -18581,10 +18604,10 @@
         <v>193</v>
       </c>
       <c r="C270">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D270" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E270">
         <v>1</v>
@@ -18631,10 +18654,10 @@
         <v>193</v>
       </c>
       <c r="C271">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D271" t="s">
-        <v>359</v>
+        <v>114</v>
       </c>
       <c r="E271">
         <v>1</v>
@@ -18681,10 +18704,10 @@
         <v>193</v>
       </c>
       <c r="C272">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D272" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="E272">
         <v>1</v>
@@ -18725,16 +18748,16 @@
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B273" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C273">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="D273" t="s">
-        <v>209</v>
+        <v>354</v>
       </c>
       <c r="E273">
         <v>1</v>
@@ -18775,16 +18798,16 @@
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B274" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C274">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="D274" t="s">
-        <v>234</v>
+        <v>355</v>
       </c>
       <c r="E274">
         <v>1</v>
@@ -18825,16 +18848,16 @@
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B275" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="C275">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="D275" t="s">
-        <v>235</v>
+        <v>356</v>
       </c>
       <c r="E275">
         <v>1</v>
@@ -18875,16 +18898,16 @@
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B276" t="s">
-        <v>95</v>
+        <v>193</v>
       </c>
       <c r="C276">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="D276" t="s">
-        <v>220</v>
+        <v>357</v>
       </c>
       <c r="E276">
         <v>1</v>
@@ -18905,10 +18928,10 @@
         <v>0</v>
       </c>
       <c r="K276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L276">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M276">
         <v>0</v>
@@ -18917,7 +18940,7 @@
         <v>0</v>
       </c>
       <c r="O276">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P276">
         <v>0</v>
@@ -18925,16 +18948,16 @@
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B277" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="C277">
-        <v>184</v>
+        <v>36</v>
       </c>
       <c r="D277" t="s">
-        <v>643</v>
+        <v>358</v>
       </c>
       <c r="E277">
         <v>1</v>
@@ -18958,7 +18981,7 @@
         <v>0</v>
       </c>
       <c r="L277">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M277">
         <v>0</v>
@@ -18970,21 +18993,21 @@
         <v>0</v>
       </c>
       <c r="P277">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B278" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="C278">
-        <v>197</v>
+        <v>29</v>
       </c>
       <c r="D278" t="s">
-        <v>653</v>
+        <v>359</v>
       </c>
       <c r="E278">
         <v>1</v>
@@ -19008,7 +19031,7 @@
         <v>0</v>
       </c>
       <c r="L278">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M278">
         <v>0</v>
@@ -19020,21 +19043,21 @@
         <v>0</v>
       </c>
       <c r="P278">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B279" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="C279">
-        <v>228</v>
+        <v>42</v>
       </c>
       <c r="D279" t="s">
-        <v>684</v>
+        <v>206</v>
       </c>
       <c r="E279">
         <v>1</v>
@@ -19058,7 +19081,7 @@
         <v>0</v>
       </c>
       <c r="L279">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M279">
         <v>0</v>
@@ -19070,21 +19093,21 @@
         <v>0</v>
       </c>
       <c r="P279">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B280" t="s">
-        <v>572</v>
+        <v>181</v>
       </c>
       <c r="C280">
-        <v>188</v>
+        <v>65</v>
       </c>
       <c r="D280" t="s">
-        <v>797</v>
+        <v>209</v>
       </c>
       <c r="E280">
         <v>1</v>
@@ -19108,7 +19131,7 @@
         <v>0</v>
       </c>
       <c r="L280">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M280">
         <v>0</v>
@@ -19120,21 +19143,21 @@
         <v>0</v>
       </c>
       <c r="P280">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B281" t="s">
-        <v>572</v>
+        <v>181</v>
       </c>
       <c r="C281">
-        <v>189</v>
+        <v>90</v>
       </c>
       <c r="D281" t="s">
-        <v>798</v>
+        <v>234</v>
       </c>
       <c r="E281">
         <v>1</v>
@@ -19158,7 +19181,7 @@
         <v>0</v>
       </c>
       <c r="L281">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M281">
         <v>0</v>
@@ -19170,21 +19193,21 @@
         <v>0</v>
       </c>
       <c r="P281">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B282" t="s">
-        <v>572</v>
+        <v>181</v>
       </c>
       <c r="C282">
-        <v>190</v>
+        <v>91</v>
       </c>
       <c r="D282" t="s">
-        <v>799</v>
+        <v>235</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -19208,7 +19231,7 @@
         <v>0</v>
       </c>
       <c r="L282">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M282">
         <v>0</v>
@@ -19220,21 +19243,21 @@
         <v>0</v>
       </c>
       <c r="P282">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B283" t="s">
-        <v>572</v>
+        <v>95</v>
       </c>
       <c r="C283">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="D283" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="E283">
         <v>1</v>
@@ -19255,7 +19278,7 @@
         <v>0</v>
       </c>
       <c r="K283">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L283">
         <v>0</v>
@@ -19267,24 +19290,24 @@
         <v>0</v>
       </c>
       <c r="O283">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P283">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B284" t="s">
-        <v>573</v>
+        <v>172</v>
       </c>
       <c r="C284">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D284" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="E284">
         <v>1</v>
@@ -19325,16 +19348,16 @@
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B285" t="s">
-        <v>573</v>
+        <v>172</v>
       </c>
       <c r="C285">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D285" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="E285">
         <v>1</v>
@@ -19375,16 +19398,16 @@
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B286" t="s">
-        <v>573</v>
+        <v>172</v>
       </c>
       <c r="C286">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D286" t="s">
-        <v>669</v>
+        <v>684</v>
       </c>
       <c r="E286">
         <v>1</v>
@@ -19425,16 +19448,16 @@
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B287" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C287">
-        <v>42</v>
+        <v>188</v>
       </c>
       <c r="D287" t="s">
-        <v>206</v>
+        <v>797</v>
       </c>
       <c r="E287">
         <v>1</v>
@@ -19475,16 +19498,16 @@
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B288" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C288">
-        <v>156</v>
+        <v>189</v>
       </c>
       <c r="D288" t="s">
-        <v>615</v>
+        <v>798</v>
       </c>
       <c r="E288">
         <v>1</v>
@@ -19525,16 +19548,16 @@
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B289" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C289">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="D289" t="s">
-        <v>619</v>
+        <v>799</v>
       </c>
       <c r="E289">
         <v>1</v>
@@ -19575,16 +19598,16 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A290">
+        <v>40</v>
+      </c>
+      <c r="B290" t="s">
+        <v>572</v>
+      </c>
+      <c r="C290">
         <v>42</v>
       </c>
-      <c r="B290" t="s">
-        <v>574</v>
-      </c>
-      <c r="C290">
-        <v>180</v>
-      </c>
       <c r="D290" t="s">
-        <v>639</v>
+        <v>206</v>
       </c>
       <c r="E290">
         <v>1</v>
@@ -19625,16 +19648,16 @@
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B291" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C291">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="D291" t="s">
-        <v>667</v>
+        <v>641</v>
       </c>
       <c r="E291">
         <v>1</v>
@@ -19675,16 +19698,16 @@
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B292" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C292">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D292" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
       <c r="E292">
         <v>1</v>
@@ -19725,16 +19748,16 @@
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B293" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C293">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D293" t="s">
-        <v>685</v>
+        <v>669</v>
       </c>
       <c r="E293">
         <v>1</v>
@@ -19775,10 +19798,10 @@
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B294" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C294">
         <v>42</v>
@@ -19825,16 +19848,16 @@
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B295" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C295">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D295" t="s">
-        <v>609</v>
+        <v>615</v>
       </c>
       <c r="E295">
         <v>1</v>
@@ -19875,16 +19898,16 @@
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B296" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C296">
-        <v>42</v>
+        <v>160</v>
       </c>
       <c r="D296" t="s">
-        <v>206</v>
+        <v>619</v>
       </c>
       <c r="E296">
         <v>1</v>
@@ -19925,16 +19948,16 @@
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B297" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C297">
-        <v>129</v>
+        <v>180</v>
       </c>
       <c r="D297" t="s">
-        <v>588</v>
+        <v>639</v>
       </c>
       <c r="E297">
         <v>1</v>
@@ -19975,16 +19998,16 @@
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B298" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C298">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="D298" t="s">
-        <v>611</v>
+        <v>667</v>
       </c>
       <c r="E298">
         <v>1</v>
@@ -20025,51 +20048,401 @@
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A299">
+        <v>42</v>
+      </c>
+      <c r="B299" t="s">
+        <v>574</v>
+      </c>
+      <c r="C299">
+        <v>216</v>
+      </c>
+      <c r="D299" t="s">
+        <v>672</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+      <c r="F299">
+        <v>1</v>
+      </c>
+      <c r="G299">
+        <v>1</v>
+      </c>
+      <c r="H299">
+        <v>1</v>
+      </c>
+      <c r="I299">
+        <v>1</v>
+      </c>
+      <c r="J299">
+        <v>0</v>
+      </c>
+      <c r="K299">
+        <v>0</v>
+      </c>
+      <c r="L299">
+        <v>0</v>
+      </c>
+      <c r="M299">
+        <v>0</v>
+      </c>
+      <c r="N299">
+        <v>0</v>
+      </c>
+      <c r="O299">
+        <v>0</v>
+      </c>
+      <c r="P299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>42</v>
+      </c>
+      <c r="B300" t="s">
+        <v>574</v>
+      </c>
+      <c r="C300">
+        <v>229</v>
+      </c>
+      <c r="D300" t="s">
+        <v>685</v>
+      </c>
+      <c r="E300">
+        <v>1</v>
+      </c>
+      <c r="F300">
+        <v>1</v>
+      </c>
+      <c r="G300">
+        <v>1</v>
+      </c>
+      <c r="H300">
+        <v>1</v>
+      </c>
+      <c r="I300">
+        <v>1</v>
+      </c>
+      <c r="J300">
+        <v>0</v>
+      </c>
+      <c r="K300">
+        <v>0</v>
+      </c>
+      <c r="L300">
+        <v>0</v>
+      </c>
+      <c r="M300">
+        <v>0</v>
+      </c>
+      <c r="N300">
+        <v>0</v>
+      </c>
+      <c r="O300">
+        <v>0</v>
+      </c>
+      <c r="P300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>42</v>
+      </c>
+      <c r="B301" t="s">
+        <v>574</v>
+      </c>
+      <c r="C301">
+        <v>42</v>
+      </c>
+      <c r="D301" t="s">
+        <v>206</v>
+      </c>
+      <c r="E301">
+        <v>1</v>
+      </c>
+      <c r="F301">
+        <v>1</v>
+      </c>
+      <c r="G301">
+        <v>1</v>
+      </c>
+      <c r="H301">
+        <v>1</v>
+      </c>
+      <c r="I301">
+        <v>1</v>
+      </c>
+      <c r="J301">
+        <v>0</v>
+      </c>
+      <c r="K301">
+        <v>0</v>
+      </c>
+      <c r="L301">
+        <v>0</v>
+      </c>
+      <c r="M301">
+        <v>0</v>
+      </c>
+      <c r="N301">
+        <v>0</v>
+      </c>
+      <c r="O301">
+        <v>0</v>
+      </c>
+      <c r="P301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>43</v>
+      </c>
+      <c r="B302" t="s">
+        <v>575</v>
+      </c>
+      <c r="C302">
+        <v>150</v>
+      </c>
+      <c r="D302" t="s">
+        <v>609</v>
+      </c>
+      <c r="E302">
+        <v>1</v>
+      </c>
+      <c r="F302">
+        <v>1</v>
+      </c>
+      <c r="G302">
+        <v>1</v>
+      </c>
+      <c r="H302">
+        <v>1</v>
+      </c>
+      <c r="I302">
+        <v>1</v>
+      </c>
+      <c r="J302">
+        <v>0</v>
+      </c>
+      <c r="K302">
+        <v>0</v>
+      </c>
+      <c r="L302">
+        <v>0</v>
+      </c>
+      <c r="M302">
+        <v>0</v>
+      </c>
+      <c r="N302">
+        <v>0</v>
+      </c>
+      <c r="O302">
+        <v>0</v>
+      </c>
+      <c r="P302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>43</v>
+      </c>
+      <c r="B303" t="s">
+        <v>575</v>
+      </c>
+      <c r="C303">
+        <v>42</v>
+      </c>
+      <c r="D303" t="s">
+        <v>206</v>
+      </c>
+      <c r="E303">
+        <v>1</v>
+      </c>
+      <c r="F303">
+        <v>1</v>
+      </c>
+      <c r="G303">
+        <v>1</v>
+      </c>
+      <c r="H303">
+        <v>1</v>
+      </c>
+      <c r="I303">
+        <v>1</v>
+      </c>
+      <c r="J303">
+        <v>0</v>
+      </c>
+      <c r="K303">
+        <v>0</v>
+      </c>
+      <c r="L303">
+        <v>0</v>
+      </c>
+      <c r="M303">
+        <v>0</v>
+      </c>
+      <c r="N303">
+        <v>0</v>
+      </c>
+      <c r="O303">
+        <v>0</v>
+      </c>
+      <c r="P303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A304">
         <v>44</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B304" t="s">
         <v>576</v>
       </c>
-      <c r="C299">
+      <c r="C304">
+        <v>129</v>
+      </c>
+      <c r="D304" t="s">
+        <v>588</v>
+      </c>
+      <c r="E304">
+        <v>1</v>
+      </c>
+      <c r="F304">
+        <v>1</v>
+      </c>
+      <c r="G304">
+        <v>1</v>
+      </c>
+      <c r="H304">
+        <v>1</v>
+      </c>
+      <c r="I304">
+        <v>1</v>
+      </c>
+      <c r="J304">
+        <v>0</v>
+      </c>
+      <c r="K304">
+        <v>0</v>
+      </c>
+      <c r="L304">
+        <v>0</v>
+      </c>
+      <c r="M304">
+        <v>0</v>
+      </c>
+      <c r="N304">
+        <v>0</v>
+      </c>
+      <c r="O304">
+        <v>0</v>
+      </c>
+      <c r="P304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>44</v>
+      </c>
+      <c r="B305" t="s">
+        <v>576</v>
+      </c>
+      <c r="C305">
+        <v>152</v>
+      </c>
+      <c r="D305" t="s">
+        <v>611</v>
+      </c>
+      <c r="E305">
+        <v>1</v>
+      </c>
+      <c r="F305">
+        <v>1</v>
+      </c>
+      <c r="G305">
+        <v>1</v>
+      </c>
+      <c r="H305">
+        <v>1</v>
+      </c>
+      <c r="I305">
+        <v>1</v>
+      </c>
+      <c r="J305">
+        <v>0</v>
+      </c>
+      <c r="K305">
+        <v>0</v>
+      </c>
+      <c r="L305">
+        <v>0</v>
+      </c>
+      <c r="M305">
+        <v>0</v>
+      </c>
+      <c r="N305">
+        <v>0</v>
+      </c>
+      <c r="O305">
+        <v>0</v>
+      </c>
+      <c r="P305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>44</v>
+      </c>
+      <c r="B306" t="s">
+        <v>576</v>
+      </c>
+      <c r="C306">
         <v>154</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D306" t="s">
         <v>613</v>
       </c>
-      <c r="E299">
-        <v>1</v>
-      </c>
-      <c r="F299">
-        <v>1</v>
-      </c>
-      <c r="G299">
-        <v>1</v>
-      </c>
-      <c r="H299">
-        <v>1</v>
-      </c>
-      <c r="I299">
-        <v>1</v>
-      </c>
-      <c r="J299">
-        <v>0</v>
-      </c>
-      <c r="K299">
-        <v>0</v>
-      </c>
-      <c r="L299">
-        <v>0</v>
-      </c>
-      <c r="M299">
-        <v>0</v>
-      </c>
-      <c r="N299">
-        <v>0</v>
-      </c>
-      <c r="O299">
-        <v>0</v>
-      </c>
-      <c r="P299">
+      <c r="E306">
+        <v>1</v>
+      </c>
+      <c r="F306">
+        <v>1</v>
+      </c>
+      <c r="G306">
+        <v>1</v>
+      </c>
+      <c r="H306">
+        <v>1</v>
+      </c>
+      <c r="I306">
+        <v>1</v>
+      </c>
+      <c r="J306">
+        <v>0</v>
+      </c>
+      <c r="K306">
+        <v>0</v>
+      </c>
+      <c r="L306">
+        <v>0</v>
+      </c>
+      <c r="M306">
+        <v>0</v>
+      </c>
+      <c r="N306">
+        <v>0</v>
+      </c>
+      <c r="O306">
+        <v>0</v>
+      </c>
+      <c r="P306">
         <v>1</v>
       </c>
     </row>
@@ -29848,9 +30221,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -30304,6 +30679,14 @@
       </c>
       <c r="B56" t="s">
         <v>585</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>